<commit_message>
business logic and json output and graphs
</commit_message>
<xml_diff>
--- a/tumlknexpectimax/excel_data/input_data_business.xlsx
+++ b/tumlknexpectimax/excel_data/input_data_business.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="525" windowWidth="13680" windowHeight="11370" tabRatio="847"/>
+    <workbookView xWindow="480" yWindow="645" windowWidth="13680" windowHeight="11250" tabRatio="847" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CAPEX" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="FTTB_Hybridpon_100" sheetId="19" r:id="rId17"/>
     <sheet name="MIG_MATRIX" sheetId="11" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -44,7 +44,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Patri, Sai Kireet:</t>
         </r>
@@ -53,7 +53,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Since each business would need its own ONT, and 7% of the buildings are business buildings, there would be 342 buildings
@@ -69,7 +69,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Patri, Sai Kireet:</t>
         </r>
@@ -78,7 +78,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Here we have 93% of the buildings which are residential and we need 1 ONT per 2 buildings, hence the number of ONTs required are 0.93*4877/2
@@ -94,7 +94,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Patri, Sai Kireet:</t>
         </r>
@@ -103,7 +103,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 table 5-6
@@ -120,7 +120,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Patri, Sai Kireet:</t>
         </r>
@@ -129,7 +129,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Table 5-13, each building needs about 300 mbps, so only 1 OLT is enough</t>
@@ -144,7 +144,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Patri, Sai Kireet:</t>
         </r>
@@ -153,7 +153,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Table 5-19 only 1 OLT needed to cater to the buildings
@@ -169,7 +169,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Patri, Sai Kireet:</t>
         </r>
@@ -178,35 +178,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Need double the racks of Technology 3 to realise a GPON FTTH
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="R7" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Patri, Sai Kireet:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-The fiber length increases
 </t>
         </r>
       </text>
@@ -219,7 +194,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Patri, Sai Kireet:</t>
         </r>
@@ -228,7 +203,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 For per household speed of 100 mbps, every building needs 1 ONT of 625 Mbps
@@ -583,14 +558,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -813,7 +788,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>Capital Expenditure of various technologies</a:t>
+              <a:t>Capital Expenditure of various technologies in business scenario</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -897,28 +872,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>62152.255239580772</c:v>
+                  <c:v>146337.87420813384</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>69006.714747374324</c:v>
+                  <c:v>146337.87420813384</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>79930.990263899323</c:v>
+                  <c:v>78872.086550701642</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>79930.990263899323</c:v>
+                  <c:v>78872.086550701642</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>69006.714747374324</c:v>
+                  <c:v>146337.87420813384</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62152.255239580772</c:v>
+                  <c:v>146337.87420813384</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69006.714747374324</c:v>
+                  <c:v>146337.87420813384</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79930.990263899323</c:v>
+                  <c:v>78872.086550701642</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>114876.35990534152</c:v>
@@ -1008,28 +983,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>1.7284661718921301</c:v>
+                  <c:v>18.840228189119191</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3716993665534263</c:v>
+                  <c:v>12.814589886676153</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.345777258575282</c:v>
+                  <c:v>14.612123172178348</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.64097725857528</c:v>
+                  <c:v>14.612123172178348</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.256899366553426</c:v>
+                  <c:v>12.814589886676153</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7284661718921301</c:v>
+                  <c:v>18.840228189119191</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.3716993665534263</c:v>
+                  <c:v>12.814589886676153</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.64097725857528</c:v>
+                  <c:v>14.612123172178348</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>12.594228370284263</c:v>
@@ -1038,13 +1013,13 @@
                   <c:v>12.211670303203721</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>23.096870303203723</c:v>
+                  <c:v>10.331648594515361</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>12.594228370284263</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.211670303203721</c:v>
+                  <c:v>9.5120485945153614</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1282,11 +1257,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="52156928"/>
-        <c:axId val="167935296"/>
+        <c:axId val="180975616"/>
+        <c:axId val="109072896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="52156928"/>
+        <c:axId val="180975616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1314,7 +1289,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="167935296"/>
+        <c:crossAx val="109072896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1322,7 +1297,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="167935296"/>
+        <c:axId val="109072896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1352,7 +1327,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52156928"/>
+        <c:crossAx val="180975616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1399,7 +1374,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Approx. OPEX per year per subscriber</a:t>
+              <a:t>Approx. OPEX per year</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1486,31 +1461,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>4000</c:v>
+                  <c:v>2500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1279.259837057527</c:v>
+                  <c:v>2121.2871443632298</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1997.126864467409</c:v>
+                  <c:v>2770.5428879802053</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2428.4913604115791</c:v>
+                  <c:v>2417.7849867387386</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12484.748312411579</c:v>
+                  <c:v>12474.158986738737</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8532.4157164674089</c:v>
+                  <c:v>9305.722887980206</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2513.815837057527</c:v>
+                  <c:v>3355.8431443632298</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2377.5328644674091</c:v>
+                  <c:v>3150.9488879802052</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2438.1283124115794</c:v>
+                  <c:v>2427.5389867387385</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1708.7975413371182</c:v>
@@ -1519,13 +1494,13 @@
                   <c:v>2920.9008073992691</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12626.239659399269</c:v>
+                  <c:v>12626.112007182181</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>2621.7435413371186</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3067.2108073992695</c:v>
+                  <c:v>3067.1838111821821</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1540,11 +1515,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="52157440"/>
-        <c:axId val="168038336"/>
+        <c:axId val="180985344"/>
+        <c:axId val="181187072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="52157440"/>
+        <c:axId val="180985344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1553,7 +1528,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168038336"/>
+        <c:crossAx val="181187072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1561,7 +1536,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="168038336"/>
+        <c:axId val="181187072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1591,7 +1566,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52157440"/>
+        <c:crossAx val="180985344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1622,6 +1597,436 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Revenue per customer per year</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.35058114754098363"/>
+          <c:y val="1.9393951833607006E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Revenue!$I$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Residential </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Revenue!$H$5:$H$18</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>ADSL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FTTC_GPON_25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FTTB_XGPON_50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>FTTB_UDWDM_50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FTTH_UDWDM_100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>FTTH_XGPON_100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>FTTC_GPON_100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>FTTB_XGPON_100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>FTTB_UDWDM_100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>FTTC_Hybridpon_25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>FTTB_Hybridpon_50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>FTTH_Hybridpon_100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>FTTC_Hybridpon_100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>FTTB_Hybridpon_100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Revenue!$I$5:$I$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Revenue!$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Business</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Revenue!$H$5:$H$18</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>ADSL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FTTC_GPON_25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FTTB_XGPON_50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>FTTB_UDWDM_50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FTTH_UDWDM_100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>FTTH_XGPON_100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>FTTC_GPON_100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>FTTB_XGPON_100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>FTTB_UDWDM_100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>FTTC_Hybridpon_25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>FTTB_Hybridpon_50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>FTTH_Hybridpon_100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>FTTC_Hybridpon_100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>FTTB_Hybridpon_100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Revenue!$J$5:$J$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>36</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="76395520"/>
+        <c:axId val="180820160"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="76395520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="180820160"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="180820160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1200"/>
+                  <a:t>Cost Units</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="76395520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.87384462659380691"/>
+          <c:y val="0.39990941434044891"/>
+          <c:w val="0.11921548269581056"/>
+          <c:h val="0.13931390257252324"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -2118,11 +2523,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="173515776"/>
-        <c:axId val="168040064"/>
+        <c:axId val="183711744"/>
+        <c:axId val="181188800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="173515776"/>
+        <c:axId val="183711744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2132,7 +2537,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168040064"/>
+        <c:crossAx val="181188800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2140,7 +2545,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="168040064"/>
+        <c:axId val="181188800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2151,14 +2556,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="173515776"/>
+        <c:crossAx val="183711744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2183,10 +2587,10 @@
       <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>744008</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>155575</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>84667</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>21167</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2212,16 +2616,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>197701</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>88050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2244,6 +2648,41 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>685798</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>521548</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>40425</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2567,8 +3006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2746,37 +3185,37 @@
         <v>151</v>
       </c>
       <c r="M3" s="7">
-        <v>12553.667997790501</v>
+        <v>31505.122417993502</v>
       </c>
       <c r="N3" s="7">
-        <v>24253.936567201501</v>
+        <v>54442.326843564399</v>
       </c>
       <c r="O3" s="7">
-        <v>28668.134420259899</v>
+        <v>68598.261692039698</v>
       </c>
       <c r="P3" s="7">
-        <v>18947.874843170201</v>
+        <v>171056.49354431301</v>
       </c>
       <c r="Q3" s="7">
-        <v>33521.641099943598</v>
+        <v>85582.633114971599</v>
       </c>
       <c r="R3" s="7">
-        <v>33953.792651492702</v>
+        <v>685372.28279667499</v>
       </c>
       <c r="S3" s="11">
         <f>M3*S46+N3*T46+O3*W46</f>
-        <v>62152.255239580772</v>
+        <v>146337.87420813384</v>
       </c>
       <c r="T3" s="11">
-        <f>(P3+Q3+R3)*$Q$27</f>
-        <v>1.7284661718921301</v>
+        <f t="shared" ref="T3:T15" si="0">(P3+Q3+R3)*$Q$27</f>
+        <v>18.840228189119191</v>
       </c>
       <c r="U3" s="11">
-        <f>(B3+C3)*H3</f>
+        <f t="shared" ref="U3:U15" si="1">(B3+C3)*H3</f>
         <v>1670.4</v>
       </c>
       <c r="V3" s="11">
-        <f>(B3+C3)*I3+(B3+C3)*J3</f>
+        <f t="shared" ref="V3:V15" si="2">(B3+C3)*I3+(B3+C3)*J3</f>
         <v>4906.8</v>
       </c>
       <c r="W3" s="11">
@@ -2784,8 +3223,8 @@
         <v>6577.2000000000007</v>
       </c>
       <c r="X3" s="12">
-        <f>S3+T3+U3+V3</f>
-        <v>68731.183705752672</v>
+        <f t="shared" ref="X3:X14" si="3">S3+T3+U3+V3</f>
+        <v>152933.91443632296</v>
       </c>
     </row>
     <row r="4" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -2828,46 +3267,46 @@
         <v>151</v>
       </c>
       <c r="M4" s="7">
-        <v>12553.667997790501</v>
+        <v>31505.122417993502</v>
       </c>
       <c r="N4" s="7">
-        <v>24253.936567201501</v>
+        <v>54442.326843564399</v>
       </c>
       <c r="O4" s="7">
-        <v>38057.804978881199</v>
+        <v>68598.261692039698</v>
       </c>
       <c r="P4" s="7">
-        <v>18947.874843170201</v>
+        <v>171056.49354431301</v>
       </c>
       <c r="Q4" s="7">
-        <v>33521.641099943598</v>
+        <v>85582.633114971599</v>
       </c>
       <c r="R4" s="7">
-        <v>66115.452384557502</v>
+        <v>384090.36767452297</v>
       </c>
       <c r="S4" s="11">
-        <f>M4*$S$46+N4*$T$46+O4*$W$46</f>
-        <v>69006.714747374324</v>
+        <f t="shared" ref="S4:S15" si="4">M4*$S$46+N4*$T$46+O4*$W$46</f>
+        <v>146337.87420813384</v>
       </c>
       <c r="T4" s="11">
-        <f>(P4+Q4+R4)*$Q$27</f>
-        <v>2.3716993665534263</v>
+        <f t="shared" si="0"/>
+        <v>12.814589886676153</v>
       </c>
       <c r="U4" s="11">
-        <f>(B4+C4)*H4</f>
+        <f t="shared" si="1"/>
         <v>1463.1</v>
       </c>
       <c r="V4" s="11">
-        <f>(B4+C4)*I4+(B4+C4)*J4</f>
+        <f t="shared" si="2"/>
         <v>11607.26</v>
       </c>
       <c r="W4" s="11">
-        <f t="shared" ref="W4:W15" si="0">SUM(U4,V4)</f>
+        <f t="shared" ref="W4:W15" si="5">SUM(U4,V4)</f>
         <v>13070.36</v>
       </c>
       <c r="X4" s="12">
-        <f>S4+T4+U4+V4</f>
-        <v>82079.446446740883</v>
+        <f t="shared" si="3"/>
+        <v>159421.04879802052</v>
       </c>
     </row>
     <row r="5" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -2906,7 +3345,7 @@
         <v>4877</v>
       </c>
       <c r="M5" s="7">
-        <v>24307.908063783601</v>
+        <v>23362.458319857102</v>
       </c>
       <c r="N5" s="7">
         <v>0</v>
@@ -2915,38 +3354,37 @@
         <v>72200.182510221493</v>
       </c>
       <c r="P5" s="7">
-        <v>73762.710265517904</v>
+        <v>72320.005945671393</v>
       </c>
       <c r="Q5" s="7">
         <v>0</v>
       </c>
       <c r="R5" s="7">
-        <f>658286.152663246+20*(B6+C6)</f>
-        <v>1243526.152663246</v>
+        <v>658286.15266324603</v>
       </c>
       <c r="S5" s="11">
-        <f>M5*$S$46+N5*$T$46+O5*$W$46</f>
-        <v>79930.990263899323</v>
+        <f t="shared" si="4"/>
+        <v>78872.086550701642</v>
       </c>
       <c r="T5" s="11">
-        <f>(P5+Q5+R5)*$Q$27</f>
-        <v>26.345777258575282</v>
+        <f t="shared" si="0"/>
+        <v>14.612123172178348</v>
       </c>
       <c r="U5" s="11">
-        <f>(B5+C5)*H5</f>
+        <f t="shared" si="1"/>
         <v>5754.86</v>
       </c>
       <c r="V5" s="11">
-        <f>(B5+C5)*I5+(B5+C5)*J5</f>
+        <f t="shared" si="2"/>
         <v>10534.320000000002</v>
       </c>
       <c r="W5" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>16289.18</v>
       </c>
       <c r="X5" s="12">
-        <f>S5+T5+U5+V5</f>
-        <v>96246.516041157913</v>
+        <f t="shared" si="3"/>
+        <v>95175.878673873827</v>
       </c>
     </row>
     <row r="6" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -2989,7 +3427,7 @@
         <v>4877</v>
       </c>
       <c r="M6" s="7">
-        <v>24307.908063783601</v>
+        <v>23362.458319857102</v>
       </c>
       <c r="N6" s="7">
         <v>0</v>
@@ -2998,7 +3436,7 @@
         <v>72200.182510221493</v>
       </c>
       <c r="P6" s="7">
-        <v>73762.710265517904</v>
+        <v>72320.005945671393</v>
       </c>
       <c r="Q6" s="7">
         <v>0</v>
@@ -3007,28 +3445,28 @@
         <v>658286.15266324603</v>
       </c>
       <c r="S6" s="11">
-        <f>M6*$S$46+N6*$T$46+O6*$W$46</f>
-        <v>79930.990263899323</v>
+        <f t="shared" si="4"/>
+        <v>78872.086550701642</v>
       </c>
       <c r="T6" s="11">
-        <f>(P6+Q6+R6)*$Q$27</f>
-        <v>14.64097725857528</v>
+        <f t="shared" si="0"/>
+        <v>14.612123172178348</v>
       </c>
       <c r="U6" s="11">
-        <f>(B6+C6)*H6</f>
+        <f t="shared" si="1"/>
         <v>19410.46</v>
       </c>
       <c r="V6" s="11">
-        <f>(B6+C6)*I6+(B6+C6)*J6</f>
+        <f t="shared" si="2"/>
         <v>97442.459999999992</v>
       </c>
       <c r="W6" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>116852.91999999998</v>
       </c>
       <c r="X6" s="12">
-        <f>S6+T6+U6+V6</f>
-        <v>196798.5512411579</v>
+        <f t="shared" si="3"/>
+        <v>195739.6186738738</v>
       </c>
     </row>
     <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3071,47 +3509,46 @@
         <v>151</v>
       </c>
       <c r="M7" s="7">
-        <v>12553.667997790501</v>
+        <v>31505.122417993502</v>
       </c>
       <c r="N7" s="7">
-        <v>24253.936567201501</v>
+        <v>54442.326843564399</v>
       </c>
       <c r="O7" s="7">
-        <v>38057.804978881199</v>
+        <v>68598.261692039698</v>
       </c>
       <c r="P7" s="7">
-        <v>18947.874843170201</v>
+        <v>171056.49354431301</v>
       </c>
       <c r="Q7" s="7">
-        <v>33521.641099943598</v>
+        <v>85582.633114971599</v>
       </c>
       <c r="R7" s="7">
-        <f>66115.4523845575+C7*20</f>
-        <v>610375.45238455746</v>
+        <v>384090.36767452297</v>
       </c>
       <c r="S7" s="11">
-        <f>M7*$S$46+N7*$T$46+O7*$W$46</f>
-        <v>69006.714747374324</v>
+        <f t="shared" si="4"/>
+        <v>146337.87420813384</v>
       </c>
       <c r="T7" s="11">
-        <f>(P7+Q7+R7)*$Q$27</f>
-        <v>13.256899366553426</v>
+        <f t="shared" si="0"/>
+        <v>12.814589886676153</v>
       </c>
       <c r="U7" s="11">
-        <f>(B7+C7)*H7</f>
+        <f t="shared" si="1"/>
         <v>8778.6</v>
       </c>
       <c r="V7" s="11">
-        <f>(B7+C7)*I7+(B7+C7)*J7</f>
+        <f t="shared" si="2"/>
         <v>69643.56</v>
       </c>
       <c r="W7" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>78422.16</v>
       </c>
       <c r="X7" s="12">
-        <f>S7+T7+U7+V7</f>
-        <v>147442.13164674089</v>
+        <f t="shared" si="3"/>
+        <v>224772.84879802051</v>
       </c>
     </row>
     <row r="8" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3152,46 +3589,46 @@
         <v>151</v>
       </c>
       <c r="M8" s="7">
-        <v>12553.667997790501</v>
+        <v>31505.122417993502</v>
       </c>
       <c r="N8" s="7">
-        <v>24253.936567201501</v>
+        <v>54442.326843564399</v>
       </c>
       <c r="O8" s="7">
-        <v>28668.134420259899</v>
+        <v>68598.261692039698</v>
       </c>
       <c r="P8" s="7">
-        <v>18947.874843170201</v>
+        <v>171056.49354431301</v>
       </c>
       <c r="Q8" s="7">
-        <v>33521.641099943598</v>
+        <v>85582.633114971599</v>
       </c>
       <c r="R8" s="7">
-        <v>33953.792651492702</v>
+        <v>685372.28279667499</v>
       </c>
       <c r="S8" s="11">
-        <f>M8*$S$46+N8*$T$46+O8*$W$46</f>
-        <v>62152.255239580772</v>
+        <f t="shared" si="4"/>
+        <v>146337.87420813384</v>
       </c>
       <c r="T8" s="11">
-        <f>(P8+Q8+R8)*$Q$27</f>
-        <v>1.7284661718921301</v>
+        <f t="shared" si="0"/>
+        <v>18.840228189119191</v>
       </c>
       <c r="U8" s="11">
-        <f>(B8+C8)*H8</f>
+        <f t="shared" si="1"/>
         <v>6340.1</v>
       </c>
       <c r="V8" s="11">
-        <f>(B8+C8)*I8+(B8+C8)*J8</f>
+        <f t="shared" si="2"/>
         <v>12582.66</v>
       </c>
       <c r="W8" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>18922.760000000002</v>
       </c>
       <c r="X8" s="12">
-        <f>S8+T8+U8+V8</f>
-        <v>81076.743705752669</v>
+        <f t="shared" si="3"/>
+        <v>165279.47443632298</v>
       </c>
     </row>
     <row r="9" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3232,46 +3669,46 @@
         <v>151</v>
       </c>
       <c r="M9" s="7">
-        <v>12553.667997790501</v>
+        <v>31505.122417993502</v>
       </c>
       <c r="N9" s="7">
-        <v>24253.936567201501</v>
+        <v>54442.326843564399</v>
       </c>
       <c r="O9" s="7">
-        <v>38057.804978881199</v>
+        <v>68598.261692039698</v>
       </c>
       <c r="P9" s="7">
-        <v>18947.874843170201</v>
+        <v>171056.49354431301</v>
       </c>
       <c r="Q9" s="7">
-        <v>33521.641099943598</v>
+        <v>85582.633114971599</v>
       </c>
       <c r="R9" s="7">
-        <v>66115.452384557502</v>
+        <v>384090.36767452297</v>
       </c>
       <c r="S9" s="11">
-        <f>M9*$S$46+N9*$T$46+O9*$W$46</f>
-        <v>69006.714747374324</v>
+        <f t="shared" si="4"/>
+        <v>146337.87420813384</v>
       </c>
       <c r="T9" s="11">
-        <f>(P9+Q9+R9)*$Q$27</f>
-        <v>2.3716993665534263</v>
+        <f t="shared" si="0"/>
+        <v>12.814589886676153</v>
       </c>
       <c r="U9" s="11">
-        <f>(B9+C9)*H9</f>
+        <f t="shared" si="1"/>
         <v>3511.44</v>
       </c>
       <c r="V9" s="11">
-        <f>(B9+C9)*I9+(B9+C9)*J9</f>
+        <f t="shared" si="2"/>
         <v>13362.98</v>
       </c>
       <c r="W9" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>16874.419999999998</v>
       </c>
       <c r="X9" s="12">
-        <f>S9+T9+U9+V9</f>
-        <v>85883.506446740881</v>
+        <f t="shared" si="3"/>
+        <v>163225.10879802052</v>
       </c>
     </row>
     <row r="10" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3311,17 +3748,16 @@
         <v>4877</v>
       </c>
       <c r="M10" s="7">
-        <v>24307.908063783601</v>
+        <v>23362.458319857102</v>
       </c>
       <c r="N10" s="7">
         <v>0</v>
       </c>
       <c r="O10" s="7">
-        <f>72200.1825102215</f>
         <v>72200.182510221493</v>
       </c>
       <c r="P10" s="7">
-        <v>73762.710265517904</v>
+        <v>72320.005945671393</v>
       </c>
       <c r="Q10" s="7">
         <v>0</v>
@@ -3330,28 +3766,28 @@
         <v>658286.15266324603</v>
       </c>
       <c r="S10" s="11">
-        <f>M10*$S$46+N10*$T$46+O10*$W$46</f>
-        <v>79930.990263899323</v>
+        <f t="shared" si="4"/>
+        <v>78872.086550701642</v>
       </c>
       <c r="T10" s="11">
-        <f>(P10+Q10+R10)*$Q$27</f>
-        <v>14.64097725857528</v>
+        <f t="shared" si="0"/>
+        <v>14.612123172178348</v>
       </c>
       <c r="U10" s="11">
-        <f>(B10+C10)*H10</f>
+        <f t="shared" si="1"/>
         <v>5852.4</v>
       </c>
       <c r="V10" s="11">
-        <f>(B10+C10)*I10+(B10+C10)*J10</f>
+        <f t="shared" si="2"/>
         <v>10534.320000000002</v>
       </c>
       <c r="W10" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>16386.72</v>
       </c>
       <c r="X10" s="12">
-        <f>S10+T10+U10+V10</f>
-        <v>96332.351241157899</v>
+        <f t="shared" si="3"/>
+        <v>95273.418673873821</v>
       </c>
     </row>
     <row r="11" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3411,27 +3847,27 @@
         <v>387592.626526276</v>
       </c>
       <c r="S11" s="11">
-        <f>M11*$S$46+N11*$T$46+O11*$W$46</f>
+        <f t="shared" si="4"/>
         <v>114876.35990534152</v>
       </c>
       <c r="T11" s="11">
-        <f>(P11+Q11+R11)*$Q$27</f>
+        <f t="shared" si="0"/>
         <v>12.594228370284263</v>
       </c>
       <c r="U11" s="11">
-        <f>(B11+C11)*H11</f>
+        <f t="shared" si="1"/>
         <v>1001.1600000000001</v>
       </c>
       <c r="V11" s="11">
-        <f>(B11+C11)*I11+(B11+C11)*J11</f>
+        <f t="shared" si="2"/>
         <v>4597.92</v>
       </c>
       <c r="W11" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>5599.08</v>
       </c>
       <c r="X11" s="12">
-        <f>S11+T11+U11+V11</f>
+        <f t="shared" si="3"/>
         <v>120488.03413371182</v>
       </c>
     </row>
@@ -3491,27 +3927,27 @@
         <v>368464.72317224898</v>
       </c>
       <c r="S12" s="11">
-        <f>M12*$S$46+N12*$T$46+O12*$W$46</f>
+        <f t="shared" si="4"/>
         <v>115530.46906962365</v>
       </c>
       <c r="T12" s="11">
-        <f>(P12+Q12+R12)*$Q$27</f>
+        <f t="shared" si="0"/>
         <v>12.211670303203721</v>
       </c>
       <c r="U12" s="11">
-        <f>(B12+C12)*H12</f>
+        <f t="shared" si="1"/>
         <v>1365.5600000000002</v>
       </c>
       <c r="V12" s="11">
-        <f>(B12+C12)*I12+(B12+C12)*J12</f>
+        <f t="shared" si="2"/>
         <v>16289.18</v>
       </c>
       <c r="W12" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>17654.740000000002</v>
       </c>
       <c r="X12" s="12">
-        <f>S12+T12+U12+V12</f>
+        <f t="shared" si="3"/>
         <v>133197.42073992686</v>
       </c>
     </row>
@@ -3559,7 +3995,6 @@
         <v>50467.597460168901</v>
       </c>
       <c r="O13" s="7">
-        <f>70030.50575712</f>
         <v>70030.505757120001</v>
       </c>
       <c r="P13" s="7">
@@ -3569,32 +4004,32 @@
         <v>233483.63773783101</v>
       </c>
       <c r="R13" s="7">
-        <f>$R$12+20*$C$13</f>
-        <v>912724.72317224904</v>
+        <f>$Q$12+20*$B$13</f>
+        <v>274463.63773783098</v>
       </c>
       <c r="S13" s="11">
-        <f>M13*$S$46+N13*$T$46+O13*$W$46</f>
+        <f t="shared" si="4"/>
         <v>115530.46906962365</v>
       </c>
       <c r="T13" s="11">
-        <f>(P13+Q13+R13)*$Q$27</f>
-        <v>23.096870303203723</v>
+        <f t="shared" si="0"/>
+        <v>10.331648594515361</v>
       </c>
       <c r="U13" s="11">
-        <f>(B13+C13)*H13</f>
+        <f t="shared" si="1"/>
         <v>15801.480000000001</v>
       </c>
       <c r="V13" s="11">
-        <f>(B13+C13)*I13+(B13+C13)*J13</f>
+        <f t="shared" si="2"/>
         <v>98905.56</v>
       </c>
       <c r="W13" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>114707.04</v>
       </c>
       <c r="X13" s="12">
-        <f>S13+T13+U13+V13</f>
-        <v>230260.60593992684</v>
+        <f t="shared" si="3"/>
+        <v>230247.84071821815</v>
       </c>
     </row>
     <row r="14" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3653,27 +4088,27 @@
         <v>387592.626526276</v>
       </c>
       <c r="S14" s="11">
-        <f>M14*$S$46+N14*$T$46+O14*$W$46</f>
+        <f t="shared" si="4"/>
         <v>114876.35990534152</v>
       </c>
       <c r="T14" s="11">
-        <f>(P14+Q14+R14)*$Q$27</f>
+        <f t="shared" si="0"/>
         <v>12.594228370284263</v>
       </c>
       <c r="U14" s="11">
-        <f>(B14+C14)*H14</f>
+        <f t="shared" si="1"/>
         <v>2633.5800000000004</v>
       </c>
       <c r="V14" s="11">
-        <f>(B14+C14)*I14+(B14+C14)*J14</f>
+        <f t="shared" si="2"/>
         <v>12094.960000000001</v>
       </c>
       <c r="W14" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>14728.54</v>
       </c>
       <c r="X14" s="12">
-        <f>S14+T14+U14+V14</f>
+        <f t="shared" si="3"/>
         <v>129617.49413371182</v>
       </c>
     </row>
@@ -3730,32 +4165,32 @@
         <v>233483.63773783101</v>
       </c>
       <c r="R15" s="7">
-        <f>$R$12</f>
-        <v>368464.72317224898</v>
+        <f>$Q$12</f>
+        <v>233483.63773783101</v>
       </c>
       <c r="S15" s="11">
-        <f>M15*$S$46+N15*$T$46+O15*$W$46</f>
+        <f t="shared" si="4"/>
         <v>115530.46906962365</v>
       </c>
       <c r="T15" s="11">
-        <f>(P15+Q15+R15)*$Q$27</f>
-        <v>12.211670303203721</v>
+        <f t="shared" si="0"/>
+        <v>9.5120485945153614</v>
       </c>
       <c r="U15" s="11">
-        <f>(B15+C15)*H15</f>
+        <f t="shared" si="1"/>
         <v>2633.5800000000004</v>
       </c>
       <c r="V15" s="11">
-        <f>(B15+C15)*I15+(B15+C15)*J15</f>
+        <f t="shared" si="2"/>
         <v>16484.260000000002</v>
       </c>
       <c r="W15" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>19117.840000000004</v>
       </c>
       <c r="X15" s="12">
-        <f t="shared" ref="X8:X15" si="1">SUM(S15:V15)</f>
-        <v>134660.52073992687</v>
+        <f t="shared" ref="X15" si="6">SUM(S15:V15)</f>
+        <v>134657.82111821815</v>
       </c>
     </row>
     <row r="27" spans="17:17" x14ac:dyDescent="0.25">
@@ -5288,7 +5723,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:U22"/>
+      <selection activeCell="S46" sqref="S46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15484,35 +15919,35 @@
       </c>
       <c r="C2">
         <f>CAPEX!$X3</f>
-        <v>68731.183705752672</v>
+        <v>152933.91443632296</v>
       </c>
       <c r="D2">
         <f>CAPEX!$X4</f>
-        <v>82079.446446740883</v>
+        <v>159421.04879802052</v>
       </c>
       <c r="E2">
         <f>CAPEX!$X5</f>
-        <v>96246.516041157913</v>
+        <v>95175.878673873827</v>
       </c>
       <c r="F2">
         <f>CAPEX!$X6</f>
-        <v>196798.5512411579</v>
+        <v>195739.6186738738</v>
       </c>
       <c r="G2">
         <f>CAPEX!$X7</f>
-        <v>147442.13164674089</v>
+        <v>224772.84879802051</v>
       </c>
       <c r="H2">
         <f>CAPEX!$X8</f>
-        <v>81076.743705752669</v>
+        <v>165279.47443632298</v>
       </c>
       <c r="I2">
         <f>CAPEX!$X9</f>
-        <v>85883.506446740881</v>
+        <v>163225.10879802052</v>
       </c>
       <c r="J2">
         <f>CAPEX!$X10</f>
-        <v>96332.351241157899</v>
+        <v>95273.418673873821</v>
       </c>
       <c r="K2">
         <f>CAPEX!$X11</f>
@@ -15524,7 +15959,7 @@
       </c>
       <c r="M2">
         <f>CAPEX!$X13</f>
-        <v>230260.60593992684</v>
+        <v>230247.84071821815</v>
       </c>
       <c r="N2">
         <f>CAPEX!$X14</f>
@@ -15532,7 +15967,7 @@
       </c>
       <c r="O2">
         <f>CAPEX!$X15</f>
-        <v>134660.52073992687</v>
+        <v>134657.82111821815</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -15547,7 +15982,7 @@
       </c>
       <c r="D3">
         <f>D2-C2</f>
-        <v>13348.262740988212</v>
+        <v>6487.1343616975646</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -15557,15 +15992,15 @@
       </c>
       <c r="G3">
         <f>G2-C2</f>
-        <v>78710.947940988219</v>
+        <v>71838.934361697553</v>
       </c>
       <c r="H3">
         <f>H2-C2</f>
-        <v>12345.559999999998</v>
+        <v>12345.560000000027</v>
       </c>
       <c r="I3">
         <f>I2-D2+D3</f>
-        <v>17152.322740988209</v>
+        <v>10291.194361697562</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -15607,7 +16042,7 @@
       </c>
       <c r="G4">
         <f>G2-D2</f>
-        <v>65362.685200000007</v>
+        <v>65351.799999999988</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -15653,7 +16088,7 @@
       </c>
       <c r="F5">
         <f>F2-E2</f>
-        <v>100552.03519999998</v>
+        <v>100563.73999999998</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -15666,7 +16101,7 @@
       </c>
       <c r="J5">
         <f>J2-E2</f>
-        <v>85.835199999986799</v>
+        <v>97.539999999993597</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -15799,14 +16234,14 @@
       </c>
       <c r="G8">
         <f>G2-H2</f>
-        <v>66365.387940988221</v>
+        <v>59493.374361697526</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
         <f>I2-H2</f>
-        <v>4806.7627409882116</v>
+        <v>-2054.3656383024645</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -15848,7 +16283,7 @@
       </c>
       <c r="G9">
         <f>G2-I2</f>
-        <v>61558.625200000009</v>
+        <v>61547.739999999991</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -15893,7 +16328,7 @@
       </c>
       <c r="F10">
         <f>F2-J2</f>
-        <v>100466.2</v>
+        <v>100466.19999999998</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -15963,7 +16398,7 @@
       </c>
       <c r="M11">
         <f>M2-K2</f>
-        <v>109772.57180621503</v>
+        <v>109759.80658450634</v>
       </c>
       <c r="N11">
         <f>N2-K2</f>
@@ -15971,7 +16406,7 @@
       </c>
       <c r="O11">
         <f>O2-L2+L11</f>
-        <v>14172.486606215054</v>
+        <v>14169.78698450634</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -16013,14 +16448,14 @@
       </c>
       <c r="M12">
         <f>M2-L2</f>
-        <v>97063.185199999978</v>
+        <v>97050.419978291291</v>
       </c>
       <c r="N12">
         <v>0</v>
       </c>
       <c r="O12">
         <f>O2-L2</f>
-        <v>1463.1000000000058</v>
+        <v>1460.4003782912914</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -16109,14 +16544,14 @@
       </c>
       <c r="M14">
         <f>M2-N2</f>
-        <v>100643.11180621502</v>
+        <v>100630.34658450633</v>
       </c>
       <c r="N14">
         <v>0</v>
       </c>
       <c r="O14">
         <f>O2-N2</f>
-        <v>5043.0266062150477</v>
+        <v>5040.3269845063332</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -16158,7 +16593,7 @@
       </c>
       <c r="M15">
         <f>M2-O2</f>
-        <v>95600.085199999972</v>
+        <v>95590.0196</v>
       </c>
       <c r="N15">
         <v>0</v>
@@ -16192,8 +16627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16216,7 +16651,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="12">
-        <v>4000</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -16225,7 +16660,7 @@
       </c>
       <c r="B3" s="12">
         <f>0.1*(CAPEX!U3+CAPEX!V3)+0.01*(CAPEX!S3+CAPEX!T3)</f>
-        <v>1279.259837057527</v>
+        <v>2121.2871443632298</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -16234,7 +16669,7 @@
       </c>
       <c r="B4" s="12">
         <f>0.1*(CAPEX!U4+CAPEX!V4)+0.01*(CAPEX!S4+CAPEX!T4)</f>
-        <v>1997.126864467409</v>
+        <v>2770.5428879802053</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -16243,7 +16678,7 @@
       </c>
       <c r="B5" s="12">
         <f>0.1*(CAPEX!U5+CAPEX!V5)+0.01*(CAPEX!S5+CAPEX!T5)</f>
-        <v>2428.4913604115791</v>
+        <v>2417.7849867387386</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -16252,7 +16687,7 @@
       </c>
       <c r="B6" s="12">
         <f>0.1*(CAPEX!U6+CAPEX!V6)+0.01*(CAPEX!S6+CAPEX!T6)</f>
-        <v>12484.748312411579</v>
+        <v>12474.158986738737</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -16261,7 +16696,7 @@
       </c>
       <c r="B7" s="12">
         <f>0.1*(CAPEX!U7+CAPEX!V7)+0.01*(CAPEX!S7+CAPEX!T7)</f>
-        <v>8532.4157164674089</v>
+        <v>9305.722887980206</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -16270,7 +16705,7 @@
       </c>
       <c r="B8" s="12">
         <f>0.1*(CAPEX!U8+CAPEX!V8)+0.01*(CAPEX!S8+CAPEX!T8)</f>
-        <v>2513.815837057527</v>
+        <v>3355.8431443632298</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -16279,7 +16714,7 @@
       </c>
       <c r="B9" s="12">
         <f>0.1*(CAPEX!U9+CAPEX!V9)+0.01*(CAPEX!S9+CAPEX!T9)</f>
-        <v>2377.5328644674091</v>
+        <v>3150.9488879802052</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -16288,7 +16723,7 @@
       </c>
       <c r="B10" s="12">
         <f>0.1*(CAPEX!U10+CAPEX!V10)+0.01*(CAPEX!S10+CAPEX!T10)</f>
-        <v>2438.1283124115794</v>
+        <v>2427.5389867387385</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -16315,7 +16750,7 @@
       </c>
       <c r="B13" s="12">
         <f>0.1*(CAPEX!U13+CAPEX!V13)+0.01*(CAPEX!S13+CAPEX!T13)</f>
-        <v>12626.239659399269</v>
+        <v>12626.112007182181</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -16333,7 +16768,7 @@
       </c>
       <c r="B15" s="12">
         <f>0.1*(CAPEX!U15+CAPEX!V15)+0.01*(CAPEX!S15+CAPEX!T15)</f>
-        <v>3067.2108073992695</v>
+        <v>3067.1838111821821</v>
       </c>
     </row>
   </sheetData>
@@ -16346,8 +16781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH74"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:H18"/>
+    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
+      <selection activeCell="AA54" sqref="AA54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16493,31 +16928,31 @@
       </c>
       <c r="U2" s="7">
         <f>OPEX!$B$15</f>
-        <v>3067.2108073992695</v>
+        <v>3067.1838111821821</v>
       </c>
       <c r="V2" s="11">
         <f>O2-U2</f>
-        <v>-1783.2108073992695</v>
+        <v>-1783.1838111821821</v>
       </c>
       <c r="W2" s="11">
         <f>P2-U2</f>
-        <v>-1783.2108073992695</v>
+        <v>-1783.1838111821821</v>
       </c>
       <c r="X2" s="11">
         <f t="shared" ref="X2:X22" si="1">Q2-U2</f>
-        <v>-1783.2108073992695</v>
+        <v>-1783.1838111821821</v>
       </c>
       <c r="Y2" s="11">
         <f>R2-$U2</f>
-        <v>-1927.2108073992695</v>
+        <v>-1927.1838111821821</v>
       </c>
       <c r="Z2" s="11">
         <f>S2-$U2</f>
-        <v>-1927.2108073992695</v>
+        <v>-1927.1838111821821</v>
       </c>
       <c r="AA2" s="11">
         <f>T2-$U2</f>
-        <v>-1927.2108073992695</v>
+        <v>-1927.1838111821821</v>
       </c>
       <c r="AB2" s="11">
         <f>1/POWER(1+$L$25,N2-2018)</f>
@@ -16525,27 +16960,27 @@
       </c>
       <c r="AC2" s="12">
         <f>V2*AB2</f>
-        <v>-1783.2108073992695</v>
+        <v>-1783.1838111821821</v>
       </c>
       <c r="AD2" s="12">
         <f>W2*AB2</f>
-        <v>-1783.2108073992695</v>
+        <v>-1783.1838111821821</v>
       </c>
       <c r="AE2" s="12">
         <f>X2*AB2</f>
-        <v>-1783.2108073992695</v>
+        <v>-1783.1838111821821</v>
       </c>
       <c r="AF2" s="12">
         <f>Y2*$AB2</f>
-        <v>-1927.2108073992695</v>
+        <v>-1927.1838111821821</v>
       </c>
       <c r="AG2" s="12">
         <f>Z2*$AB2</f>
-        <v>-1927.2108073992695</v>
+        <v>-1927.1838111821821</v>
       </c>
       <c r="AH2" s="12">
         <f>AA2*$AB2</f>
-        <v>-1927.2108073992695</v>
+        <v>-1927.1838111821821</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
@@ -16595,31 +17030,31 @@
       </c>
       <c r="U3" s="7">
         <f>OPEX!$B$15</f>
-        <v>3067.2108073992695</v>
+        <v>3067.1838111821821</v>
       </c>
       <c r="V3" s="11">
         <f t="shared" ref="V3:V22" si="8">O3-U3</f>
-        <v>-1351.2108073992695</v>
+        <v>-1351.1838111821821</v>
       </c>
       <c r="W3" s="11">
         <f t="shared" ref="W3:W22" si="9">P3-U3</f>
-        <v>-1267.2108073992695</v>
+        <v>-1267.1838111821821</v>
       </c>
       <c r="X3" s="11">
         <f t="shared" si="1"/>
-        <v>-631.21080739926947</v>
+        <v>-631.18381118218213</v>
       </c>
       <c r="Y3" s="11">
         <f t="shared" ref="Y3:Y22" si="10">R3-$U3</f>
-        <v>-1531.2108073992695</v>
+        <v>-1531.1838111821821</v>
       </c>
       <c r="Z3" s="11">
         <f t="shared" ref="Z3:Z22" si="11">S3-$U3</f>
-        <v>-1459.2108073992695</v>
+        <v>-1459.1838111821821</v>
       </c>
       <c r="AA3" s="11">
         <f t="shared" ref="AA3:AA22" si="12">T3-$U3</f>
-        <v>-907.21080739926947</v>
+        <v>-907.18381118218213</v>
       </c>
       <c r="AB3" s="11">
         <f t="shared" ref="AB3:AB22" si="13">1/POWER(1+$L$25,N3-2018)</f>
@@ -16627,27 +17062,27 @@
       </c>
       <c r="AC3" s="12">
         <f t="shared" ref="AC3:AC22" si="14">V3*AB3</f>
-        <v>-1228.3734612720632</v>
+        <v>-1228.3489192565291</v>
       </c>
       <c r="AD3" s="12">
         <f t="shared" ref="AD3:AD22" si="15">W3*AB3</f>
-        <v>-1152.0098249084267</v>
+        <v>-1151.9852828928929</v>
       </c>
       <c r="AE3" s="12">
         <f t="shared" ref="AE3:AE22" si="16">X3*AB3</f>
-        <v>-573.82800672660858</v>
+        <v>-573.80346471107464</v>
       </c>
       <c r="AF3" s="12">
         <f t="shared" ref="AF3:AF22" si="17">Y3*$AB3</f>
-        <v>-1392.0098249084267</v>
+        <v>-1391.9852828928929</v>
       </c>
       <c r="AG3" s="12">
         <f t="shared" ref="AG3:AG22" si="18">Z3*$AB3</f>
-        <v>-1326.5552794538812</v>
+        <v>-1326.5307374383474</v>
       </c>
       <c r="AH3" s="12">
         <f t="shared" ref="AH3:AH22" si="19">AA3*$AB3</f>
-        <v>-824.73709763569946</v>
+        <v>-824.71255562016552</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
@@ -16706,31 +17141,31 @@
       </c>
       <c r="U4" s="7">
         <f>OPEX!$B$15</f>
-        <v>3067.2108073992695</v>
+        <v>3067.1838111821821</v>
       </c>
       <c r="V4" s="11">
         <f t="shared" si="8"/>
-        <v>-715.21080739926947</v>
+        <v>-715.18381118218213</v>
       </c>
       <c r="W4" s="11">
         <f t="shared" si="9"/>
-        <v>-595.21080739926947</v>
+        <v>-595.18381118218213</v>
       </c>
       <c r="X4" s="11">
         <f t="shared" si="1"/>
-        <v>1576.7891926007305</v>
+        <v>1576.8161888178179</v>
       </c>
       <c r="Y4" s="11">
         <f t="shared" si="10"/>
-        <v>-979.21080739926947</v>
+        <v>-979.18381118218213</v>
       </c>
       <c r="Z4" s="11">
         <f t="shared" si="11"/>
-        <v>-871.21080739926947</v>
+        <v>-871.18381118218213</v>
       </c>
       <c r="AA4" s="11">
         <f t="shared" si="12"/>
-        <v>1084.7891926007305</v>
+        <v>1084.8161888178179</v>
       </c>
       <c r="AB4" s="11">
         <f t="shared" si="13"/>
@@ -16738,27 +17173,27 @@
       </c>
       <c r="AC4" s="12">
         <f t="shared" si="14"/>
-        <v>-591.08331190022261</v>
+        <v>-591.06100097700994</v>
       </c>
       <c r="AD4" s="12">
         <f t="shared" si="15"/>
-        <v>-491.90975818121439</v>
+        <v>-491.88744725800171</v>
       </c>
       <c r="AE4" s="12">
         <f t="shared" si="16"/>
-        <v>1303.1315641328349</v>
+        <v>1303.1538750560476</v>
       </c>
       <c r="AF4" s="12">
         <f t="shared" si="17"/>
-        <v>-809.26513008204074</v>
+        <v>-809.24281915882807</v>
       </c>
       <c r="AG4" s="12">
         <f t="shared" si="18"/>
-        <v>-720.00893173493341</v>
+        <v>-719.98662081172074</v>
       </c>
       <c r="AH4" s="12">
         <f t="shared" si="19"/>
-        <v>896.51999388490117</v>
+        <v>896.54230480811384</v>
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
@@ -16818,31 +17253,31 @@
       </c>
       <c r="U5" s="7">
         <f>OPEX!$B$15</f>
-        <v>3067.2108073992695</v>
+        <v>3067.1838111821821</v>
       </c>
       <c r="V5" s="11">
         <f t="shared" si="8"/>
-        <v>112.78919260073053</v>
+        <v>112.81618881781787</v>
       </c>
       <c r="W5" s="11">
         <f t="shared" si="9"/>
-        <v>448.78919260073053</v>
+        <v>448.81618881781787</v>
       </c>
       <c r="X5" s="11">
         <f t="shared" si="1"/>
-        <v>5968.7891926007305</v>
+        <v>5968.8161888178183</v>
       </c>
       <c r="Y5" s="11">
         <f t="shared" si="10"/>
-        <v>-223.21080739926947</v>
+        <v>-223.18381118218213</v>
       </c>
       <c r="Z5" s="11">
         <f t="shared" si="11"/>
-        <v>88.78919260073053</v>
+        <v>88.816188817817874</v>
       </c>
       <c r="AA5" s="11">
         <f t="shared" si="12"/>
-        <v>5044.7891926007305</v>
+        <v>5044.8161888178183</v>
       </c>
       <c r="AB5" s="11">
         <f t="shared" si="13"/>
@@ -16850,27 +17285,27 @@
       </c>
       <c r="AC5" s="12">
         <f t="shared" si="14"/>
-        <v>84.740189782667542</v>
+        <v>84.760472440133611</v>
       </c>
       <c r="AD5" s="12">
         <f t="shared" si="15"/>
-        <v>337.18196288559761</v>
+        <v>337.20224554306367</v>
       </c>
       <c r="AE5" s="12">
         <f t="shared" si="16"/>
-        <v>4484.4396638623057</v>
+        <v>4484.4599465197716</v>
       </c>
       <c r="AF5" s="12">
         <f t="shared" si="17"/>
-        <v>-167.7015833202625</v>
+        <v>-167.68130066279645</v>
       </c>
       <c r="AG5" s="12">
         <f t="shared" si="18"/>
-        <v>66.708634561029683</v>
+        <v>66.728917218495752</v>
       </c>
       <c r="AH5" s="12">
         <f t="shared" si="19"/>
-        <v>3790.2247878292478</v>
+        <v>3790.2450704867142</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
@@ -16930,31 +17365,31 @@
       </c>
       <c r="U6" s="7">
         <f>OPEX!$B$15</f>
-        <v>3067.2108073992695</v>
+        <v>3067.1838111821821</v>
       </c>
       <c r="V6" s="11">
         <f t="shared" si="8"/>
-        <v>1276.7891926007305</v>
+        <v>1276.8161888178179</v>
       </c>
       <c r="W6" s="11">
         <f t="shared" si="9"/>
-        <v>1888.7891926007305</v>
+        <v>1888.8161888178179</v>
       </c>
       <c r="X6" s="11">
         <f t="shared" si="1"/>
-        <v>14464.789192600731</v>
+        <v>14464.816188817818</v>
       </c>
       <c r="Y6" s="11">
         <f t="shared" si="10"/>
-        <v>808.78919260073053</v>
+        <v>808.81618881781787</v>
       </c>
       <c r="Z6" s="11">
         <f t="shared" si="11"/>
-        <v>1372.7891926007305</v>
+        <v>1372.8161888178179</v>
       </c>
       <c r="AA6" s="11">
         <f t="shared" si="12"/>
-        <v>12700.789192600731</v>
+        <v>12700.816188817818</v>
       </c>
       <c r="AB6" s="11">
         <f t="shared" si="13"/>
@@ -16962,27 +17397,27 @@
       </c>
       <c r="AC6" s="12">
         <f t="shared" si="14"/>
-        <v>872.06419821100349</v>
+        <v>872.08263699051815</v>
       </c>
       <c r="AD6" s="12">
         <f t="shared" si="15"/>
-        <v>1290.0684328944267</v>
+        <v>1290.0868716739412</v>
       </c>
       <c r="AE6" s="12">
         <f t="shared" si="16"/>
-        <v>9879.6456475655541</v>
+        <v>9879.6640863450684</v>
       </c>
       <c r="AF6" s="12">
         <f t="shared" si="17"/>
-        <v>552.4139011001505</v>
+        <v>552.43233987966505</v>
       </c>
       <c r="AG6" s="12">
         <f t="shared" si="18"/>
-        <v>937.63348992605029</v>
+        <v>937.65192870556484</v>
       </c>
       <c r="AH6" s="12">
         <f t="shared" si="19"/>
-        <v>8674.8099123015691</v>
+        <v>8674.8283510810834</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
@@ -17042,31 +17477,31 @@
       </c>
       <c r="U7" s="7">
         <f>OPEX!$B$15</f>
-        <v>3067.2108073992695</v>
+        <v>3067.1838111821821</v>
       </c>
       <c r="V7" s="11">
         <f t="shared" si="8"/>
-        <v>2860.7891926007305</v>
+        <v>2860.8161888178179</v>
       </c>
       <c r="W7" s="11">
         <f t="shared" si="9"/>
-        <v>3928.7891926007305</v>
+        <v>3928.8161888178179</v>
       </c>
       <c r="X7" s="11">
         <f t="shared" si="1"/>
-        <v>30760.789192600729</v>
+        <v>30760.816188817818</v>
       </c>
       <c r="Y7" s="11">
         <f t="shared" si="10"/>
-        <v>2260.7891926007305</v>
+        <v>2260.8161888178179</v>
       </c>
       <c r="Z7" s="11">
         <f t="shared" si="11"/>
-        <v>3208.7891926007305</v>
+        <v>3208.8161888178179</v>
       </c>
       <c r="AA7" s="11">
         <f t="shared" si="12"/>
-        <v>27352.789192600729</v>
+        <v>27352.816188817818</v>
       </c>
       <c r="AB7" s="11">
         <f t="shared" si="13"/>
@@ -17074,27 +17509,27 @@
       </c>
       <c r="AC7" s="12">
         <f t="shared" si="14"/>
-        <v>1776.3250104629772</v>
+        <v>1776.3417729898088</v>
       </c>
       <c r="AD7" s="12">
         <f t="shared" si="15"/>
-        <v>2439.4689834901546</v>
+        <v>2439.485746016986</v>
       </c>
       <c r="AE7" s="12">
         <f t="shared" si="16"/>
-        <v>19100.029923813399</v>
+        <v>19100.046686340233</v>
       </c>
       <c r="AF7" s="12">
         <f t="shared" si="17"/>
-        <v>1403.7722166274843</v>
+        <v>1403.7889791543157</v>
       </c>
       <c r="AG7" s="12">
         <f t="shared" si="18"/>
-        <v>1992.4056308875631</v>
+        <v>1992.4223934143945</v>
       </c>
       <c r="AH7" s="12">
         <f t="shared" si="19"/>
-        <v>16983.930054827797</v>
+        <v>16983.94681735463</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
@@ -17154,31 +17589,31 @@
       </c>
       <c r="U8" s="7">
         <f>OPEX!$B$15</f>
-        <v>3067.2108073992695</v>
+        <v>3067.1838111821821</v>
       </c>
       <c r="V8" s="11">
         <f t="shared" si="8"/>
-        <v>5044.7891926007305</v>
+        <v>5044.8161888178183</v>
       </c>
       <c r="W8" s="11">
         <f t="shared" si="9"/>
-        <v>6844.7891926007305</v>
+        <v>6844.8161888178183</v>
       </c>
       <c r="X8" s="11">
         <f t="shared" si="1"/>
-        <v>60664.789192600729</v>
+        <v>60664.816188817815</v>
       </c>
       <c r="Y8" s="11">
         <f t="shared" si="10"/>
-        <v>4192.7891926007305</v>
+        <v>4192.8161888178183</v>
       </c>
       <c r="Z8" s="11">
         <f t="shared" si="11"/>
-        <v>5848.7891926007305</v>
+        <v>5848.8161888178183</v>
       </c>
       <c r="AA8" s="11">
         <f t="shared" si="12"/>
-        <v>54268.789192600729</v>
+        <v>54268.816188817815</v>
       </c>
       <c r="AB8" s="11">
         <f t="shared" si="13"/>
@@ -17186,27 +17621,27 @@
       </c>
       <c r="AC8" s="12">
         <f t="shared" si="14"/>
-        <v>2847.6519818401562</v>
+        <v>2847.6672205009122</v>
       </c>
       <c r="AD8" s="12">
         <f t="shared" si="15"/>
-        <v>3863.705055936955</v>
+        <v>3863.720294597711</v>
       </c>
       <c r="AE8" s="12">
         <f t="shared" si="16"/>
-        <v>34243.691971431246</v>
+        <v>34243.707210091998</v>
       </c>
       <c r="AF8" s="12">
         <f t="shared" si="17"/>
-        <v>2366.7201934343379</v>
+        <v>2366.735432095094</v>
       </c>
       <c r="AG8" s="12">
         <f t="shared" si="18"/>
-        <v>3301.4890216033928</v>
+        <v>3301.5042602641493</v>
       </c>
       <c r="AH8" s="12">
         <f t="shared" si="19"/>
-        <v>30633.316714807286</v>
+        <v>30633.331953468041</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
@@ -17265,31 +17700,31 @@
       </c>
       <c r="U9" s="7">
         <f>OPEX!$B$15</f>
-        <v>3067.2108073992695</v>
+        <v>3067.1838111821821</v>
       </c>
       <c r="V9" s="11">
         <f t="shared" si="8"/>
-        <v>8020.7891926007305</v>
+        <v>8020.8161888178183</v>
       </c>
       <c r="W9" s="11">
         <f t="shared" si="9"/>
-        <v>10948.789192600731</v>
+        <v>10948.816188817818</v>
       </c>
       <c r="X9" s="11">
         <f t="shared" si="1"/>
-        <v>111472.78919260073</v>
+        <v>111472.81618881781</v>
       </c>
       <c r="Y9" s="11">
         <f t="shared" si="10"/>
-        <v>6892.7891926007305</v>
+        <v>6892.8161888178183</v>
       </c>
       <c r="Z9" s="11">
         <f t="shared" si="11"/>
-        <v>9508.7891926007305</v>
+        <v>9508.8161888178183</v>
       </c>
       <c r="AA9" s="11">
         <f t="shared" si="12"/>
-        <v>100000.78919260073</v>
+        <v>100000.81618881781</v>
       </c>
       <c r="AB9" s="11">
         <f t="shared" si="13"/>
@@ -17297,27 +17732,27 @@
       </c>
       <c r="AC9" s="12">
         <f t="shared" si="14"/>
-        <v>4115.9330888001778</v>
+        <v>4115.9469421281383</v>
       </c>
       <c r="AD9" s="12">
         <f t="shared" si="15"/>
-        <v>5618.4600589796864</v>
+        <v>5618.473912307647</v>
       </c>
       <c r="AE9" s="12">
         <f t="shared" si="16"/>
-        <v>57203.166736003222</v>
+        <v>57203.180589331183</v>
       </c>
       <c r="AF9" s="12">
         <f t="shared" si="17"/>
-        <v>3537.0907314359415</v>
+        <v>3537.1045847639016</v>
       </c>
       <c r="AG9" s="12">
         <f t="shared" si="18"/>
-        <v>4879.512368727469</v>
+        <v>4879.5262220554296</v>
       </c>
       <c r="AH9" s="12">
         <f t="shared" si="19"/>
-        <v>51316.216803660558</v>
+        <v>51316.230656988519</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
@@ -17376,31 +17811,31 @@
       </c>
       <c r="U10" s="7">
         <f>OPEX!$B$15</f>
-        <v>3067.2108073992695</v>
+        <v>3067.1838111821821</v>
       </c>
       <c r="V10" s="11">
         <f t="shared" si="8"/>
-        <v>12076.789192600731</v>
+        <v>12076.816188817818</v>
       </c>
       <c r="W10" s="11">
         <f t="shared" si="9"/>
-        <v>16708.789192600729</v>
+        <v>16708.816188817818</v>
       </c>
       <c r="X10" s="11">
         <f t="shared" si="1"/>
-        <v>185164.78919260073</v>
+        <v>185164.81618881781</v>
       </c>
       <c r="Y10" s="11">
         <f t="shared" si="10"/>
-        <v>10540.789192600731</v>
+        <v>10540.816188817818</v>
       </c>
       <c r="Z10" s="11">
         <f t="shared" si="11"/>
-        <v>14692.789192600731</v>
+        <v>14692.816188817818</v>
       </c>
       <c r="AA10" s="11">
         <f t="shared" si="12"/>
-        <v>166312.78919260073</v>
+        <v>166312.81618881781</v>
       </c>
       <c r="AB10" s="11">
         <f t="shared" si="13"/>
@@ -17408,27 +17843,27 @@
       </c>
       <c r="AC10" s="12">
         <f t="shared" si="14"/>
-        <v>5633.9112875853853</v>
+        <v>5633.9238815198942</v>
       </c>
       <c r="AD10" s="12">
         <f t="shared" si="15"/>
-        <v>7794.7734727168681</v>
+        <v>7794.786066651378</v>
       </c>
       <c r="AE10" s="12">
         <f t="shared" si="16"/>
-        <v>86380.740713327672</v>
+        <v>86380.753307262188</v>
       </c>
       <c r="AF10" s="12">
         <f t="shared" si="17"/>
-        <v>4917.3559515832349</v>
+        <v>4917.3685455177447</v>
       </c>
       <c r="AG10" s="12">
         <f t="shared" si="18"/>
-        <v>6854.2945942140468</v>
+        <v>6854.3071881485566</v>
       </c>
       <c r="AH10" s="12">
         <f t="shared" si="19"/>
-        <v>77586.143581613782</v>
+        <v>77586.156175548298</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
@@ -17487,31 +17922,31 @@
       </c>
       <c r="U11" s="7">
         <f>OPEX!$B$15</f>
-        <v>3067.2108073992695</v>
+        <v>3067.1838111821821</v>
       </c>
       <c r="V11" s="11">
         <f t="shared" si="8"/>
-        <v>17548.789192600729</v>
+        <v>17548.816188817818</v>
       </c>
       <c r="W11" s="11">
         <f t="shared" si="9"/>
-        <v>24676.789192600729</v>
+        <v>24676.816188817818</v>
       </c>
       <c r="X11" s="11">
         <f t="shared" si="1"/>
-        <v>263908.78919260076</v>
+        <v>263908.81618881784</v>
       </c>
       <c r="Y11" s="11">
         <f t="shared" si="10"/>
-        <v>15460.789192600731</v>
+        <v>15460.816188817818</v>
       </c>
       <c r="Z11" s="11">
         <f t="shared" si="11"/>
-        <v>21868.789192600729</v>
+        <v>21868.816188817818</v>
       </c>
       <c r="AA11" s="11">
         <f t="shared" si="12"/>
-        <v>237196.78919260073</v>
+        <v>237196.81618881781</v>
       </c>
       <c r="AB11" s="11">
         <f t="shared" si="13"/>
@@ -17519,27 +17954,27 @@
       </c>
       <c r="AC11" s="12">
         <f t="shared" si="14"/>
-        <v>7442.3997019027674</v>
+        <v>7442.4111509341401</v>
       </c>
       <c r="AD11" s="12">
         <f t="shared" si="15"/>
-        <v>10465.367525661837</v>
+        <v>10465.378974693211</v>
       </c>
       <c r="AE11" s="12">
         <f t="shared" si="16"/>
-        <v>111923.0889641481</v>
+        <v>111923.10041317948</v>
       </c>
       <c r="AF11" s="12">
         <f t="shared" si="17"/>
-        <v>6556.88387474102</v>
+        <v>6556.8953237723917</v>
       </c>
       <c r="AG11" s="12">
         <f t="shared" si="18"/>
-        <v>9274.5014132719007</v>
+        <v>9274.5128623032742</v>
       </c>
       <c r="AH11" s="12">
         <f t="shared" si="19"/>
-        <v>100594.59338218228</v>
+        <v>100594.60483121366</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
@@ -17599,31 +18034,31 @@
       </c>
       <c r="U12" s="7">
         <f>OPEX!$B$15</f>
-        <v>3067.2108073992695</v>
+        <v>3067.1838111821821</v>
       </c>
       <c r="V12" s="11">
         <f t="shared" si="8"/>
-        <v>24892.789192600729</v>
+        <v>24892.816188817818</v>
       </c>
       <c r="W12" s="11">
         <f t="shared" si="9"/>
-        <v>35512.789192600729</v>
+        <v>35512.816188817815</v>
       </c>
       <c r="X12" s="11">
         <f t="shared" si="1"/>
-        <v>311188.78919260076</v>
+        <v>311188.81618881784</v>
       </c>
       <c r="Y12" s="11">
         <f t="shared" si="10"/>
-        <v>22060.789192600729</v>
+        <v>22060.816188817818</v>
       </c>
       <c r="Z12" s="11">
         <f t="shared" si="11"/>
-        <v>31636.789192600729</v>
+        <v>31636.816188817818</v>
       </c>
       <c r="AA12" s="11">
         <f t="shared" si="12"/>
-        <v>279748.78919260076</v>
+        <v>279748.81618881784</v>
       </c>
       <c r="AB12" s="11">
         <f t="shared" si="13"/>
@@ -17631,27 +18066,27 @@
       </c>
       <c r="AC12" s="12">
         <f t="shared" si="14"/>
-        <v>9597.2478283911751</v>
+        <v>9597.258236601514</v>
       </c>
       <c r="AD12" s="12">
         <f t="shared" si="15"/>
-        <v>13691.717562132801</v>
+        <v>13691.727970343138</v>
       </c>
       <c r="AE12" s="12">
         <f t="shared" si="16"/>
-        <v>119976.74941890834</v>
+        <v>119976.75982711867</v>
       </c>
       <c r="AF12" s="12">
         <f t="shared" si="17"/>
-        <v>8505.3892327267422</v>
+        <v>8505.3996409370811</v>
       </c>
       <c r="AG12" s="12">
         <f t="shared" si="18"/>
-        <v>12197.351772303937</v>
+        <v>12197.362180514276</v>
       </c>
       <c r="AH12" s="12">
         <f t="shared" si="19"/>
-        <v>107855.26839924385</v>
+        <v>107855.2788074542</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
@@ -17710,31 +18145,31 @@
       </c>
       <c r="U13" s="7">
         <f>OPEX!$B$15</f>
-        <v>3067.2108073992695</v>
+        <v>3067.1838111821821</v>
       </c>
       <c r="V13" s="11">
         <f t="shared" si="8"/>
-        <v>34540.789192600729</v>
+        <v>34540.816188817815</v>
       </c>
       <c r="W13" s="11">
         <f t="shared" si="9"/>
-        <v>50104.789192600729</v>
+        <v>50104.816188817815</v>
       </c>
       <c r="X13" s="11">
         <f t="shared" si="1"/>
-        <v>321328.78919260076</v>
+        <v>321328.81618881784</v>
       </c>
       <c r="Y13" s="11">
         <f t="shared" si="10"/>
-        <v>30748.789192600729</v>
+        <v>30748.816188817818</v>
       </c>
       <c r="Z13" s="11">
         <f t="shared" si="11"/>
-        <v>44752.789192600729</v>
+        <v>44752.816188817815</v>
       </c>
       <c r="AA13" s="11">
         <f t="shared" si="12"/>
-        <v>288880.78919260076</v>
+        <v>288880.81618881784</v>
       </c>
       <c r="AB13" s="11">
         <f t="shared" si="13"/>
@@ -17742,27 +18177,27 @@
       </c>
       <c r="AC13" s="12">
         <f t="shared" si="14"/>
-        <v>12106.335895279359</v>
+        <v>12106.345357288756</v>
       </c>
       <c r="AD13" s="12">
         <f t="shared" si="15"/>
-        <v>17561.422946807746</v>
+        <v>17561.432408817145</v>
       </c>
       <c r="AE13" s="12">
         <f t="shared" si="16"/>
-        <v>112623.78033974888</v>
+        <v>112623.78980175828</v>
       </c>
       <c r="AF13" s="12">
         <f t="shared" si="17"/>
-        <v>10777.263028445919</v>
+        <v>10777.272490455318</v>
       </c>
       <c r="AG13" s="12">
         <f t="shared" si="18"/>
-        <v>15685.579596783335</v>
+        <v>15685.589058792733</v>
       </c>
       <c r="AH13" s="12">
         <f t="shared" si="19"/>
-        <v>101250.95428937666</v>
+        <v>101250.96375138607</v>
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
@@ -17821,31 +18256,31 @@
       </c>
       <c r="U14" s="7">
         <f>OPEX!$B$15</f>
-        <v>3067.2108073992695</v>
+        <v>3067.1838111821821</v>
       </c>
       <c r="V14" s="11">
         <f t="shared" si="8"/>
-        <v>47164.789192600729</v>
+        <v>47164.816188817815</v>
       </c>
       <c r="W14" s="11">
         <f t="shared" si="9"/>
-        <v>69148.789192600729</v>
+        <v>69148.816188817815</v>
       </c>
       <c r="X14" s="11">
         <f t="shared" si="1"/>
-        <v>321784.78919260076</v>
+        <v>321784.81618881784</v>
       </c>
       <c r="Y14" s="11">
         <f t="shared" si="10"/>
-        <v>42124.789192600729</v>
+        <v>42124.816188817815</v>
       </c>
       <c r="Z14" s="11">
         <f t="shared" si="11"/>
-        <v>61912.789192600729</v>
+        <v>61912.816188817815</v>
       </c>
       <c r="AA14" s="11">
         <f t="shared" si="12"/>
-        <v>289264.78919260076</v>
+        <v>289264.81618881784</v>
       </c>
       <c r="AB14" s="11">
         <f t="shared" si="13"/>
@@ -17853,27 +18288,27 @@
       </c>
       <c r="AC14" s="12">
         <f t="shared" si="14"/>
-        <v>15028.155347574959</v>
+        <v>15028.163949401684</v>
       </c>
       <c r="AD14" s="12">
         <f t="shared" si="15"/>
-        <v>22032.935244119435</v>
+        <v>22032.943845946163</v>
       </c>
       <c r="AE14" s="12">
         <f t="shared" si="16"/>
-        <v>102530.55050719308</v>
+        <v>102530.55910901981</v>
       </c>
       <c r="AF14" s="12">
         <f t="shared" si="17"/>
-        <v>13422.256026314761</v>
+        <v>13422.264628141485</v>
       </c>
       <c r="AG14" s="12">
         <f t="shared" si="18"/>
-        <v>19727.322647167297</v>
+        <v>19727.331248994022</v>
       </c>
       <c r="AH14" s="12">
         <f t="shared" si="19"/>
-        <v>92168.676315252291</v>
+        <v>92168.684917079023</v>
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
@@ -17932,31 +18367,31 @@
       </c>
       <c r="U15" s="7">
         <f>OPEX!$B$15</f>
-        <v>3067.2108073992695</v>
+        <v>3067.1838111821821</v>
       </c>
       <c r="V15" s="11">
         <f t="shared" si="8"/>
-        <v>63244.789192600729</v>
+        <v>63244.816188817815</v>
       </c>
       <c r="W15" s="11">
         <f t="shared" si="9"/>
-        <v>93268.789192600729</v>
+        <v>93268.816188817815</v>
       </c>
       <c r="X15" s="11">
         <f t="shared" si="1"/>
-        <v>321868.78919260076</v>
+        <v>321868.81618881784</v>
       </c>
       <c r="Y15" s="11">
         <f t="shared" si="10"/>
-        <v>56608.789192600729</v>
+        <v>56608.816188817815</v>
       </c>
       <c r="Z15" s="11">
         <f t="shared" si="11"/>
-        <v>83608.789192600729</v>
+        <v>83608.816188817815</v>
       </c>
       <c r="AA15" s="11">
         <f t="shared" si="12"/>
-        <v>289348.78919260076</v>
+        <v>289348.81618881784</v>
       </c>
       <c r="AB15" s="11">
         <f t="shared" si="13"/>
@@ -17964,27 +18399,27 @@
       </c>
       <c r="AC15" s="12">
         <f t="shared" si="14"/>
-        <v>18319.762633052265</v>
+        <v>18319.770452894743</v>
       </c>
       <c r="AD15" s="12">
         <f t="shared" si="15"/>
-        <v>27016.645970266582</v>
+        <v>27016.653790109056</v>
       </c>
       <c r="AE15" s="12">
         <f t="shared" si="16"/>
-        <v>93233.923178073412</v>
+        <v>93233.930997915901</v>
       </c>
       <c r="AF15" s="12">
         <f t="shared" si="17"/>
-        <v>16397.549809119606</v>
+        <v>16397.557628962084</v>
       </c>
       <c r="AG15" s="12">
         <f t="shared" si="18"/>
-        <v>24218.488062010176</v>
+        <v>24218.495881852654</v>
       </c>
       <c r="AH15" s="12">
         <f t="shared" si="19"/>
-        <v>83814.037549036337</v>
+        <v>83814.045368878811</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
@@ -18043,31 +18478,31 @@
       </c>
       <c r="U16" s="7">
         <f>OPEX!$B$15</f>
-        <v>3067.2108073992695</v>
+        <v>3067.1838111821821</v>
       </c>
       <c r="V16" s="11">
         <f t="shared" si="8"/>
-        <v>83236.789192600729</v>
+        <v>83236.816188817815</v>
       </c>
       <c r="W16" s="11">
         <f t="shared" si="9"/>
-        <v>122296.78919260073</v>
+        <v>122296.81618881781</v>
       </c>
       <c r="X16" s="11">
         <f t="shared" si="1"/>
-        <v>321904.78919260076</v>
+        <v>321904.81618881784</v>
       </c>
       <c r="Y16" s="11">
         <f t="shared" si="10"/>
-        <v>74572.789192600729</v>
+        <v>74572.816188817815</v>
       </c>
       <c r="Z16" s="11">
         <f t="shared" si="11"/>
-        <v>109720.78919260073</v>
+        <v>109720.81618881781</v>
       </c>
       <c r="AA16" s="11">
         <f t="shared" si="12"/>
-        <v>289372.78919260076</v>
+        <v>289372.81618881784</v>
       </c>
       <c r="AB16" s="11">
         <f t="shared" si="13"/>
@@ -18075,27 +18510,27 @@
       </c>
       <c r="AC16" s="12">
         <f t="shared" si="14"/>
-        <v>21918.84810249829</v>
+        <v>21918.855211446</v>
       </c>
       <c r="AD16" s="12">
         <f t="shared" si="15"/>
-        <v>32204.566895693766</v>
+        <v>32204.574004641472</v>
       </c>
       <c r="AE16" s="12">
         <f t="shared" si="16"/>
-        <v>84767.591905221736</v>
+        <v>84767.599014169449</v>
       </c>
       <c r="AF16" s="12">
         <f t="shared" si="17"/>
-        <v>19637.346115190416</v>
+        <v>19637.353224138122</v>
       </c>
       <c r="AG16" s="12">
         <f t="shared" si="18"/>
-        <v>28892.913041540509</v>
+        <v>28892.920150488215</v>
       </c>
       <c r="AH16" s="12">
         <f t="shared" si="19"/>
-        <v>76200.89954013635</v>
+        <v>76200.906649084063</v>
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
@@ -18154,31 +18589,31 @@
       </c>
       <c r="U17" s="7">
         <f>OPEX!$B$15</f>
-        <v>3067.2108073992695</v>
+        <v>3067.1838111821821</v>
       </c>
       <c r="V17" s="11">
         <f t="shared" si="8"/>
-        <v>107272.78919260073</v>
+        <v>107272.81618881781</v>
       </c>
       <c r="W17" s="11">
         <f t="shared" si="9"/>
-        <v>155320.78919260073</v>
+        <v>155320.81618881781</v>
       </c>
       <c r="X17" s="11">
         <f t="shared" si="1"/>
-        <v>321928.78919260076</v>
+        <v>321928.81618881784</v>
       </c>
       <c r="Y17" s="11">
         <f t="shared" si="10"/>
-        <v>96208.789192600729</v>
+        <v>96208.816188817815</v>
       </c>
       <c r="Z17" s="11">
         <f t="shared" si="11"/>
-        <v>139480.78919260073</v>
+        <v>139480.81618881781</v>
       </c>
       <c r="AA17" s="11">
         <f t="shared" si="12"/>
-        <v>289396.78919260076</v>
+        <v>289396.81618881784</v>
       </c>
       <c r="AB17" s="11">
         <f t="shared" si="13"/>
@@ -18186,27 +18621,27 @@
       </c>
       <c r="AC17" s="12">
         <f t="shared" si="14"/>
-        <v>25680.252846362931</v>
+        <v>25680.259309042664</v>
       </c>
       <c r="AD17" s="12">
         <f t="shared" si="15"/>
-        <v>37182.562034452494</v>
+        <v>37182.568497132226</v>
       </c>
       <c r="AE17" s="12">
         <f t="shared" si="16"/>
-        <v>77067.192595750079</v>
+        <v>77067.199058429804</v>
       </c>
       <c r="AF17" s="12">
         <f t="shared" si="17"/>
-        <v>23031.619212142508</v>
+        <v>23031.62567482224</v>
       </c>
       <c r="AG17" s="12">
         <f t="shared" si="18"/>
-        <v>33390.591972444949</v>
+        <v>33390.598435124681</v>
       </c>
       <c r="AH17" s="12">
         <f t="shared" si="19"/>
-        <v>69279.29044567245</v>
+        <v>69279.296908352189</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
@@ -18265,31 +18700,31 @@
       </c>
       <c r="U18" s="7">
         <f>OPEX!$B$15</f>
-        <v>3067.2108073992695</v>
+        <v>3067.1838111821821</v>
       </c>
       <c r="V18" s="11">
         <f t="shared" si="8"/>
-        <v>134920.78919260073</v>
+        <v>134920.81618881781</v>
       </c>
       <c r="W18" s="11">
         <f t="shared" si="9"/>
-        <v>190180.78919260073</v>
+        <v>190180.81618881781</v>
       </c>
       <c r="X18" s="11">
         <f t="shared" si="1"/>
-        <v>321940.78919260076</v>
+        <v>321940.81618881784</v>
       </c>
       <c r="Y18" s="11">
         <f t="shared" si="10"/>
-        <v>121096.78919260073</v>
+        <v>121096.81618881781</v>
       </c>
       <c r="Z18" s="11">
         <f t="shared" si="11"/>
-        <v>170848.78919260073</v>
+        <v>170848.81618881781</v>
       </c>
       <c r="AA18" s="11">
         <f t="shared" si="12"/>
-        <v>289408.78919260076</v>
+        <v>289408.81618881784</v>
       </c>
       <c r="AB18" s="11">
         <f t="shared" si="13"/>
@@ -18297,27 +18732,27 @@
       </c>
       <c r="AC18" s="12">
         <f t="shared" si="14"/>
-        <v>29362.694752110507</v>
+        <v>29362.700627273902</v>
       </c>
       <c r="AD18" s="12">
         <f t="shared" si="15"/>
-        <v>41388.880795874116</v>
+        <v>41388.886671037508</v>
       </c>
       <c r="AE18" s="12">
         <f t="shared" si="16"/>
-        <v>70063.695727584098</v>
+        <v>70063.701602747489</v>
       </c>
       <c r="AF18" s="12">
         <f t="shared" si="17"/>
-        <v>26354.189578947495</v>
+        <v>26354.19545411089</v>
       </c>
       <c r="AG18" s="12">
         <f t="shared" si="18"/>
-        <v>37181.674342778962</v>
+        <v>37181.680217942361</v>
       </c>
       <c r="AH18" s="12">
         <f t="shared" si="19"/>
-        <v>62983.784682058984</v>
+        <v>62983.790557222375</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
@@ -18367,31 +18802,31 @@
       </c>
       <c r="U19" s="7">
         <f>OPEX!$B$15</f>
-        <v>3067.2108073992695</v>
+        <v>3067.1838111821821</v>
       </c>
       <c r="V19" s="11">
         <f t="shared" si="8"/>
-        <v>165004.78919260073</v>
+        <v>165004.81618881781</v>
       </c>
       <c r="W19" s="11">
         <f t="shared" si="9"/>
-        <v>223780.78919260073</v>
+        <v>223780.81618881781</v>
       </c>
       <c r="X19" s="11">
         <f t="shared" si="1"/>
-        <v>321952.78919260076</v>
+        <v>321952.81618881784</v>
       </c>
       <c r="Y19" s="11">
         <f t="shared" si="10"/>
-        <v>148192.78919260073</v>
+        <v>148192.81618881781</v>
       </c>
       <c r="Z19" s="11">
         <f t="shared" si="11"/>
-        <v>201052.78919260073</v>
+        <v>201052.81618881781</v>
       </c>
       <c r="AA19" s="11">
         <f t="shared" si="12"/>
-        <v>289420.78919260076</v>
+        <v>289420.81618881784</v>
       </c>
       <c r="AB19" s="11">
         <f t="shared" si="13"/>
@@ -18399,27 +18834,27 @@
       </c>
       <c r="AC19" s="12">
         <f t="shared" si="14"/>
-        <v>32645.31788474667</v>
+        <v>32645.323225804299</v>
       </c>
       <c r="AD19" s="12">
         <f t="shared" si="15"/>
-        <v>44273.836144021006</v>
+        <v>44273.841485078636</v>
       </c>
       <c r="AE19" s="12">
         <f t="shared" si="16"/>
-        <v>63696.642979285069</v>
+        <v>63696.648320342698</v>
       </c>
       <c r="AF19" s="12">
         <f t="shared" si="17"/>
-        <v>29319.153311197599</v>
+        <v>29319.158652255232</v>
       </c>
       <c r="AG19" s="12">
         <f t="shared" si="18"/>
-        <v>39777.22250925874</v>
+        <v>39777.227850316369</v>
       </c>
       <c r="AH19" s="12">
         <f t="shared" si="19"/>
-        <v>57260.360210625877</v>
+        <v>57260.365551683506</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
@@ -18469,31 +18904,31 @@
       </c>
       <c r="U20" s="7">
         <f>OPEX!$B$15</f>
-        <v>3067.2108073992695</v>
+        <v>3067.1838111821821</v>
       </c>
       <c r="V20" s="11">
         <f t="shared" si="8"/>
-        <v>195760.78919260073</v>
+        <v>195760.81618881781</v>
       </c>
       <c r="W20" s="11">
         <f t="shared" si="9"/>
-        <v>253156.78919260073</v>
+        <v>253156.81618881781</v>
       </c>
       <c r="X20" s="11">
         <f t="shared" si="1"/>
-        <v>321952.78919260076</v>
+        <v>321952.81618881784</v>
       </c>
       <c r="Y20" s="11">
         <f t="shared" si="10"/>
-        <v>175864.78919260073</v>
+        <v>175864.81618881781</v>
       </c>
       <c r="Z20" s="11">
         <f t="shared" si="11"/>
-        <v>227500.78919260073</v>
+        <v>227500.81618881781</v>
       </c>
       <c r="AA20" s="11">
         <f t="shared" si="12"/>
-        <v>289420.78919260076</v>
+        <v>289420.81618881784</v>
       </c>
       <c r="AB20" s="11">
         <f t="shared" si="13"/>
@@ -18501,27 +18936,27 @@
       </c>
       <c r="AC20" s="12">
         <f t="shared" si="14"/>
-        <v>35209.298655853832</v>
+        <v>35209.303511360769</v>
       </c>
       <c r="AD20" s="12">
         <f t="shared" si="15"/>
-        <v>45532.473761483059</v>
+        <v>45532.478616989996</v>
       </c>
       <c r="AE20" s="12">
         <f t="shared" si="16"/>
-        <v>57906.039072077328</v>
+        <v>57906.043927584265</v>
       </c>
       <c r="AF20" s="12">
         <f t="shared" si="17"/>
-        <v>31630.828171820121</v>
+        <v>31630.833027327059</v>
       </c>
       <c r="AG20" s="12">
         <f t="shared" si="18"/>
-        <v>40918.016647572273</v>
+        <v>40918.02150307921</v>
       </c>
       <c r="AH20" s="12">
         <f t="shared" si="19"/>
-        <v>52054.872918750792</v>
+        <v>52054.877774257729</v>
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
@@ -18571,31 +19006,31 @@
       </c>
       <c r="U21" s="7">
         <f>OPEX!$B$15</f>
-        <v>3067.2108073992695</v>
+        <v>3067.1838111821821</v>
       </c>
       <c r="V21" s="11">
         <f t="shared" si="8"/>
-        <v>225016.78919260073</v>
+        <v>225016.81618881781</v>
       </c>
       <c r="W21" s="11">
         <f t="shared" si="9"/>
-        <v>276412.78919260076</v>
+        <v>276412.81618881784</v>
       </c>
       <c r="X21" s="11">
         <f t="shared" si="1"/>
-        <v>321952.78919260076</v>
+        <v>321952.81618881784</v>
       </c>
       <c r="Y21" s="11">
         <f t="shared" si="10"/>
-        <v>202192.78919260073</v>
+        <v>202192.81618881781</v>
       </c>
       <c r="Z21" s="11">
         <f t="shared" si="11"/>
-        <v>248464.78919260073</v>
+        <v>248464.81618881781</v>
       </c>
       <c r="AA21" s="11">
         <f t="shared" si="12"/>
-        <v>289420.78919260076</v>
+        <v>289420.81618881784</v>
       </c>
       <c r="AB21" s="11">
         <f t="shared" si="13"/>
@@ -18603,27 +19038,27 @@
       </c>
       <c r="AC21" s="12">
         <f t="shared" si="14"/>
-        <v>36792.043103125252</v>
+        <v>36792.047517222469</v>
       </c>
       <c r="AD21" s="12">
         <f t="shared" si="15"/>
-        <v>45195.699799647024</v>
+        <v>45195.70421374424</v>
       </c>
       <c r="AE21" s="12">
         <f t="shared" si="16"/>
-        <v>52641.853701888467</v>
+        <v>52641.858115985684</v>
       </c>
       <c r="AF21" s="12">
         <f t="shared" si="17"/>
-        <v>33060.136720499897</v>
+        <v>33060.141134597114</v>
       </c>
       <c r="AG21" s="12">
         <f t="shared" si="18"/>
-        <v>40625.978472026378</v>
+        <v>40625.982886123595</v>
       </c>
       <c r="AH21" s="12">
         <f t="shared" si="19"/>
-        <v>47322.611744318885</v>
+        <v>47322.616158416102</v>
       </c>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
@@ -18673,31 +19108,31 @@
       </c>
       <c r="U22" s="7">
         <f>OPEX!$B$15</f>
-        <v>3067.2108073992695</v>
+        <v>3067.1838111821821</v>
       </c>
       <c r="V22" s="11">
         <f t="shared" si="8"/>
-        <v>250804.78919260073</v>
+        <v>250804.81618881781</v>
       </c>
       <c r="W22" s="11">
         <f t="shared" si="9"/>
-        <v>293212.78919260076</v>
+        <v>293212.81618881784</v>
       </c>
       <c r="X22" s="11">
         <f t="shared" si="1"/>
-        <v>321952.78919260076</v>
+        <v>321952.81618881784</v>
       </c>
       <c r="Y22" s="11">
         <f t="shared" si="10"/>
-        <v>225412.78919260073</v>
+        <v>225412.81618881781</v>
       </c>
       <c r="Z22" s="11">
         <f t="shared" si="11"/>
-        <v>263560.78919260076</v>
+        <v>263560.81618881784</v>
       </c>
       <c r="AA22" s="11">
         <f t="shared" si="12"/>
-        <v>289420.78919260076</v>
+        <v>289420.81618881784</v>
       </c>
       <c r="AB22" s="11">
         <f t="shared" si="13"/>
@@ -18705,27 +19140,27 @@
       </c>
       <c r="AC22" s="12">
         <f t="shared" si="14"/>
-        <v>37280.533791418668</v>
+        <v>37280.537804234315</v>
       </c>
       <c r="AD22" s="12">
         <f t="shared" si="15"/>
-        <v>43584.212768666548</v>
+        <v>43584.216781482202</v>
       </c>
       <c r="AE22" s="12">
         <f t="shared" si="16"/>
-        <v>47856.230638080429</v>
+        <v>47856.234650896084</v>
       </c>
       <c r="AF22" s="12">
         <f t="shared" si="17"/>
-        <v>33506.174788629614</v>
+        <v>33506.178801445269</v>
       </c>
       <c r="AG22" s="12">
         <f t="shared" si="18"/>
-        <v>39176.631910494645</v>
+        <v>39176.635923310299</v>
       </c>
       <c r="AH22" s="12">
         <f t="shared" si="19"/>
-        <v>43020.556131198995</v>
+        <v>43020.560144014649</v>
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.25">
@@ -20045,6 +20480,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -22947,7 +23383,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25837,7 +26273,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:U22"/>
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed PV calculation. Errors galore
</commit_message>
<xml_diff>
--- a/tumlknexpectimax/excel_data/input_data_business.xlsx
+++ b/tumlknexpectimax/excel_data/input_data_business.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="645" windowWidth="13680" windowHeight="11250" tabRatio="847" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="645" windowWidth="13680" windowHeight="11250" tabRatio="847" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CAPEX" sheetId="1" r:id="rId1"/>
@@ -335,9 +335,6 @@
     <t>IRR</t>
   </si>
   <si>
-    <t>Approx OPEX per year per subscriber</t>
-  </si>
-  <si>
     <t>PS+ONT+DSLAM</t>
   </si>
   <si>
@@ -537,6 +534,9 @@
   </si>
   <si>
     <t>FTTB_Hybridpon_120</t>
+  </si>
+  <si>
+    <t>Approx OPEX per year</t>
   </si>
 </sst>
 </file>
@@ -766,7 +766,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -793,7 +793,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1257,11 +1256,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="180975616"/>
-        <c:axId val="109072896"/>
+        <c:axId val="41646720"/>
+        <c:axId val="41661184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="180975616"/>
+        <c:axId val="41646720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1283,13 +1282,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109072896"/>
+        <c:crossAx val="41661184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1297,7 +1295,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="109072896"/>
+        <c:axId val="41661184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1320,21 +1318,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="180975616"/>
+        <c:crossAx val="41646720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1352,7 +1348,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1398,7 +1394,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Approx OPEX per year per subscriber</c:v>
+                  <c:v>Approx OPEX per year</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1515,11 +1511,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="180985344"/>
-        <c:axId val="181187072"/>
+        <c:axId val="41813504"/>
+        <c:axId val="41815040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="180985344"/>
+        <c:axId val="41813504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1528,7 +1524,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181187072"/>
+        <c:crossAx val="41815040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1536,7 +1532,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181187072"/>
+        <c:axId val="41815040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1566,7 +1562,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="180985344"/>
+        <c:crossAx val="41813504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1586,7 +1582,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1885,11 +1881,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="76395520"/>
-        <c:axId val="180820160"/>
+        <c:axId val="41843328"/>
+        <c:axId val="41857408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="76395520"/>
+        <c:axId val="41843328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1905,10 +1901,10 @@
             <a:pPr>
               <a:defRPr sz="1200"/>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="180820160"/>
+        <c:crossAx val="41857408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1916,7 +1912,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="180820160"/>
+        <c:axId val="41857408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1953,10 +1949,10 @@
             <a:pPr>
               <a:defRPr sz="1200"/>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76395520"/>
+        <c:crossAx val="41843328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1972,7 +1968,7 @@
             <a:pPr>
               <a:defRPr sz="1400"/>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
       </c:legendEntry>
@@ -1985,7 +1981,7 @@
             <a:pPr>
               <a:defRPr sz="1400"/>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
       </c:legendEntry>
@@ -2016,7 +2012,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2523,11 +2519,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="183711744"/>
-        <c:axId val="181188800"/>
+        <c:axId val="41879040"/>
+        <c:axId val="41880576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="183711744"/>
+        <c:axId val="41879040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2537,7 +2533,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181188800"/>
+        <c:crossAx val="41880576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2545,7 +2541,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181188800"/>
+        <c:axId val="41880576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2556,7 +2552,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183711744"/>
+        <c:crossAx val="41879040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2651,16 +2647,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>685798</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>514348</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>521548</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>40425</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>73873</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>30900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3035,10 +3031,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>63</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -3059,7 +3055,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K1" s="9" t="s">
         <v>5</v>
@@ -3098,7 +3094,7 @@
         <v>19</v>
       </c>
       <c r="W1" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="X1" s="9" t="s">
         <v>20</v>
@@ -3146,7 +3142,7 @@
     </row>
     <row r="3" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" s="7">
         <v>342</v>
@@ -3165,7 +3161,7 @@
         <v>8</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H3" s="7">
         <f>0.64</f>
@@ -3229,7 +3225,7 @@
     </row>
     <row r="4" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="7">
         <v>342</v>
@@ -3311,7 +3307,7 @@
     </row>
     <row r="5" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" s="7">
         <v>342</v>
@@ -3389,7 +3385,7 @@
     </row>
     <row r="6" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" s="7">
         <v>2049</v>
@@ -3471,7 +3467,7 @@
     </row>
     <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" s="7">
         <v>2049</v>
@@ -3553,7 +3549,7 @@
     </row>
     <row r="8" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" s="7">
         <v>342</v>
@@ -3571,7 +3567,7 @@
         <v>8</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H8" s="7">
         <v>1.3</v>
@@ -3633,7 +3629,7 @@
     </row>
     <row r="9" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9" s="7">
         <v>342</v>
@@ -3713,7 +3709,7 @@
     </row>
     <row r="10" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B10" s="7">
         <v>342</v>
@@ -3792,7 +3788,7 @@
     </row>
     <row r="11" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="7">
         <v>342</v>
@@ -3811,7 +3807,7 @@
         <v>21</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H11" s="7">
         <v>0.54</v>
@@ -3873,7 +3869,7 @@
     </row>
     <row r="12" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12" s="7">
         <v>342</v>
@@ -3953,7 +3949,7 @@
     </row>
     <row r="13" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" s="7">
         <v>2049</v>
@@ -4034,7 +4030,7 @@
     </row>
     <row r="14" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14" s="7">
         <v>342</v>
@@ -4052,7 +4048,7 @@
         <v>21</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H14" s="7">
         <v>0.54</v>
@@ -4114,7 +4110,7 @@
     </row>
     <row r="15" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15" s="7">
         <v>342</v>
@@ -4201,7 +4197,7 @@
     </row>
     <row r="42" spans="18:25" x14ac:dyDescent="0.25">
       <c r="R42" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="S42" s="5"/>
       <c r="T42" s="5"/>
@@ -4210,17 +4206,17 @@
       <c r="W42" s="5"/>
       <c r="X42" s="5"/>
       <c r="Y42" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="18:25" x14ac:dyDescent="0.25">
       <c r="S43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="18:25" x14ac:dyDescent="0.25">
       <c r="R44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S44">
         <f>0.02/1000</f>
@@ -4235,23 +4231,23 @@
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="Y44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="18:25" x14ac:dyDescent="0.25">
       <c r="S45" t="s">
+        <v>57</v>
+      </c>
+      <c r="T45" t="s">
         <v>58</v>
       </c>
-      <c r="T45" t="s">
+      <c r="W45" t="s">
         <v>59</v>
-      </c>
-      <c r="W45" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="46" spans="18:25" x14ac:dyDescent="0.25">
       <c r="R46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S46">
         <v>1.1200000000000001</v>
@@ -4263,13 +4259,17 @@
         <v>0.73</v>
       </c>
       <c r="Y46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LUnrestricted</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -4297,13 +4297,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -4318,13 +4318,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -4339,13 +4339,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -5715,6 +5715,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LUnrestricted</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -5742,13 +5746,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -5763,13 +5767,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -5784,13 +5788,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -7160,6 +7164,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LUnrestricted</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -7190,13 +7198,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -7211,13 +7219,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -7232,13 +7240,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -8608,6 +8616,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LUnrestricted</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -8635,13 +8647,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -8656,13 +8668,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -8677,13 +8689,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -10053,6 +10065,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LUnrestricted</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -10080,13 +10096,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -10101,13 +10117,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -10122,13 +10138,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -11498,6 +11514,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LUnrestricted</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -11525,13 +11545,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -11546,13 +11566,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -11567,13 +11587,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -12943,6 +12963,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LUnrestricted</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -12970,13 +12994,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -12991,13 +13015,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -13012,13 +13036,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -14388,6 +14412,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LUnrestricted</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -14415,13 +14443,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -14436,13 +14464,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -14457,13 +14485,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -15833,6 +15861,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LUnrestricted</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -15871,43 +15903,43 @@
         <v>23</v>
       </c>
       <c r="C1" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>78</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -15972,7 +16004,7 @@
     </row>
     <row r="3" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -16023,7 +16055,7 @@
     </row>
     <row r="4" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -16072,7 +16104,7 @@
     </row>
     <row r="5" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -16121,7 +16153,7 @@
     </row>
     <row r="6" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -16168,7 +16200,7 @@
     </row>
     <row r="7" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -16215,7 +16247,7 @@
     </row>
     <row r="8" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -16264,7 +16296,7 @@
     </row>
     <row r="9" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -16312,7 +16344,7 @@
     </row>
     <row r="10" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -16360,7 +16392,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -16411,7 +16443,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -16460,7 +16492,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -16507,7 +16539,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -16556,7 +16588,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -16620,6 +16652,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LUnrestricted</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -16627,8 +16663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16643,7 +16679,7 @@
         <v>22</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -16656,7 +16692,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" s="12">
         <f>0.1*(CAPEX!U3+CAPEX!V3)+0.01*(CAPEX!S3+CAPEX!T3)</f>
@@ -16665,7 +16701,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="12">
         <f>0.1*(CAPEX!U4+CAPEX!V4)+0.01*(CAPEX!S4+CAPEX!T4)</f>
@@ -16674,7 +16710,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" s="12">
         <f>0.1*(CAPEX!U5+CAPEX!V5)+0.01*(CAPEX!S5+CAPEX!T5)</f>
@@ -16683,7 +16719,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" s="12">
         <f>0.1*(CAPEX!U6+CAPEX!V6)+0.01*(CAPEX!S6+CAPEX!T6)</f>
@@ -16692,7 +16728,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" s="12">
         <f>0.1*(CAPEX!U7+CAPEX!V7)+0.01*(CAPEX!S7+CAPEX!T7)</f>
@@ -16701,7 +16737,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" s="12">
         <f>0.1*(CAPEX!U8+CAPEX!V8)+0.01*(CAPEX!S8+CAPEX!T8)</f>
@@ -16710,7 +16746,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9" s="12">
         <f>0.1*(CAPEX!U9+CAPEX!V9)+0.01*(CAPEX!S9+CAPEX!T9)</f>
@@ -16719,7 +16755,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B10" s="12">
         <f>0.1*(CAPEX!U10+CAPEX!V10)+0.01*(CAPEX!S10+CAPEX!T10)</f>
@@ -16728,7 +16764,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="12">
         <f>0.1*(CAPEX!U11+CAPEX!V11)+0.01*(CAPEX!S11+CAPEX!T11)</f>
@@ -16737,7 +16773,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12" s="12">
         <f>0.1*(CAPEX!U12+CAPEX!V12)+0.01*(CAPEX!S12+CAPEX!T12)</f>
@@ -16746,7 +16782,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" s="12">
         <f>0.1*(CAPEX!U13+CAPEX!V13)+0.01*(CAPEX!S13+CAPEX!T13)</f>
@@ -16755,7 +16791,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14" s="12">
         <f>0.1*(CAPEX!U14+CAPEX!V14)+0.01*(CAPEX!S14+CAPEX!T14)</f>
@@ -16764,7 +16800,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15" s="12">
         <f>0.1*(CAPEX!U15+CAPEX!V15)+0.01*(CAPEX!S15+CAPEX!T15)</f>
@@ -16773,7 +16809,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LUnrestricted</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -16781,8 +16821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
-      <selection activeCell="AA54" sqref="AA54"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16829,13 +16869,13 @@
         <v>29</v>
       </c>
       <c r="R1" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="T1" s="10" t="s">
-        <v>46</v>
       </c>
       <c r="U1" s="10" t="s">
         <v>30</v>
@@ -16850,13 +16890,13 @@
         <v>33</v>
       </c>
       <c r="Y1" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="Z1" s="10" t="s">
+      <c r="AA1" s="10" t="s">
         <v>48</v>
-      </c>
-      <c r="AA1" s="10" t="s">
-        <v>49</v>
       </c>
       <c r="AB1" s="10" t="s">
         <v>34</v>
@@ -16871,13 +16911,13 @@
         <v>37</v>
       </c>
       <c r="AF1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="AG1" s="10" t="s">
+      <c r="AH1" s="10" t="s">
         <v>51</v>
-      </c>
-      <c r="AH1" s="10" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
@@ -16897,7 +16937,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="M2" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N2" s="7">
         <v>2018</v>
@@ -16999,7 +17039,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="M3" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N3" s="7">
         <v>2019</v>
@@ -17101,16 +17141,16 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="H4" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="I4" s="10" t="s">
-        <v>85</v>
-      </c>
       <c r="J4" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N4" s="7">
         <v>2020</v>
@@ -17222,7 +17262,7 @@
         <v>3.6</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N5" s="7">
         <v>2021</v>
@@ -17324,7 +17364,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="H6" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I6" s="10">
         <f>30*12/50</f>
@@ -17334,7 +17374,7 @@
         <v>12</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N6" s="7">
         <v>2022</v>
@@ -17436,7 +17476,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="H7" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I7" s="10">
         <f>40*12/50</f>
@@ -17446,7 +17486,7 @@
         <v>24</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N7" s="7">
         <v>2023</v>
@@ -17548,7 +17588,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="H8" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I8" s="10">
         <f>40*12/50</f>
@@ -17558,7 +17598,7 @@
         <v>24</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N8" s="7">
         <v>2024</v>
@@ -17660,7 +17700,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="H9" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I9" s="10">
         <v>12</v>
@@ -17669,7 +17709,7 @@
         <v>36</v>
       </c>
       <c r="M9" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N9" s="7">
         <v>2025</v>
@@ -17771,7 +17811,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="H10" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I10" s="10">
         <v>12</v>
@@ -17780,7 +17820,7 @@
         <v>36</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N10" s="7">
         <v>2026</v>
@@ -17882,7 +17922,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="H11" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I11" s="10">
         <v>12</v>
@@ -17891,7 +17931,7 @@
         <v>36</v>
       </c>
       <c r="M11" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N11" s="7">
         <v>2027</v>
@@ -17993,7 +18033,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="H12" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I12" s="10">
         <f>50*12/50</f>
@@ -18003,7 +18043,7 @@
         <v>36</v>
       </c>
       <c r="M12" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N12" s="7">
         <v>2028</v>
@@ -18105,7 +18145,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="H13" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I13" s="10">
         <v>12</v>
@@ -18114,7 +18154,7 @@
         <v>36</v>
       </c>
       <c r="M13" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N13" s="7">
         <v>2029</v>
@@ -18216,7 +18256,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="H14" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I14" s="10">
         <v>7.2</v>
@@ -18225,7 +18265,7 @@
         <v>12</v>
       </c>
       <c r="M14" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N14" s="7">
         <v>2030</v>
@@ -18327,7 +18367,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="H15" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I15" s="10">
         <v>9.6</v>
@@ -18336,7 +18376,7 @@
         <v>24</v>
       </c>
       <c r="M15" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N15" s="7">
         <v>2031</v>
@@ -18438,7 +18478,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="H16" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I16" s="10">
         <v>12</v>
@@ -18447,7 +18487,7 @@
         <v>36</v>
       </c>
       <c r="M16" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N16" s="7">
         <v>2032</v>
@@ -18549,7 +18589,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="H17" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I17" s="10">
         <v>12</v>
@@ -18558,7 +18598,7 @@
         <v>36</v>
       </c>
       <c r="M17" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N17" s="7">
         <v>2033</v>
@@ -18660,7 +18700,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="H18" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I18" s="10">
         <v>12</v>
@@ -18669,7 +18709,7 @@
         <v>36</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N18" s="7">
         <v>2034</v>
@@ -18771,7 +18811,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="M19" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N19" s="7">
         <v>2035</v>
@@ -18873,7 +18913,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="M20" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N20" s="7">
         <v>2036</v>
@@ -18975,7 +19015,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="M21" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N21" s="7">
         <v>2037</v>
@@ -19077,7 +19117,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="M22" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N22" s="7">
         <v>2038</v>
@@ -19176,10 +19216,10 @@
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="R27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
@@ -19196,13 +19236,13 @@
         <v>27</v>
       </c>
       <c r="E28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" t="s">
         <v>42</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>43</v>
-      </c>
-      <c r="G28" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.25">
@@ -19234,10 +19274,10 @@
         <v>80</v>
       </c>
       <c r="J29" t="s">
+        <v>79</v>
+      </c>
+      <c r="K29" t="s">
         <v>80</v>
-      </c>
-      <c r="K29" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.25">
@@ -19842,7 +19882,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -19859,13 +19899,13 @@
         <v>27</v>
       </c>
       <c r="E53" t="s">
+        <v>41</v>
+      </c>
+      <c r="F53" t="s">
         <v>42</v>
       </c>
-      <c r="F53" t="s">
+      <c r="G53" t="s">
         <v>43</v>
-      </c>
-      <c r="G53" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -20480,6 +20520,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LUnrestricted</oddFooter>
+  </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -20511,13 +20554,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -20532,13 +20575,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -20553,13 +20596,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -21930,6 +21973,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LUnrestricted</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -21957,13 +22003,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -21978,13 +22024,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -21999,13 +22045,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -23375,6 +23421,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LUnrestricted</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -23402,13 +23452,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -23423,13 +23473,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -23444,13 +23494,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -24820,6 +24870,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LUnrestricted</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -24847,13 +24901,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -24868,13 +24922,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -24889,13 +24943,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -26265,6 +26319,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LUnrestricted</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -26292,13 +26350,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -26313,13 +26371,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -26334,13 +26392,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -27710,6 +27768,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LUnrestricted</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -27737,13 +27799,13 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -27758,13 +27820,13 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -27779,13 +27841,13 @@
         <v>37</v>
       </c>
       <c r="S1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>51</v>
-      </c>
-      <c r="U1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -29155,6 +29217,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LUnrestricted</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Real time Present value generation working for residential and business
</commit_message>
<xml_diff>
--- a/tumlknexpectimax/excel_data/input_data_business.xlsx
+++ b/tumlknexpectimax/excel_data/input_data_business.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmadzay\PycharmProjects\mt_code\tumlknexpectimax\tumlknexpectimax\excel_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="645" windowWidth="13680" windowHeight="11250" tabRatio="847" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="648" windowWidth="13680" windowHeight="11256" tabRatio="847" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CAPEX" sheetId="1" r:id="rId1"/>
@@ -26,7 +31,7 @@
     <sheet name="FTTB_Hybridpon_100" sheetId="19" r:id="rId17"/>
     <sheet name="MIG_MATRIX" sheetId="11" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -36,7 +41,7 @@
     <author>Patri, Sai Kireet</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -61,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -86,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H4" authorId="0">
+    <comment ref="H4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -112,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0">
+    <comment ref="H5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -136,7 +141,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H6" authorId="0">
+    <comment ref="H6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -161,7 +166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H7" authorId="0">
+    <comment ref="H7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -186,7 +191,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0">
+    <comment ref="C8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -542,7 +547,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000000%"/>
   </numFmts>
@@ -759,12 +764,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -912,6 +920,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F92B-4BDB-8C8A-80B4841F7958}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1023,6 +1036,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F92B-4BDB-8C8A-80B4841F7958}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1134,6 +1152,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F92B-4BDB-8C8A-80B4841F7958}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1245,6 +1268,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F92B-4BDB-8C8A-80B4841F7958}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1284,6 +1312,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1346,7 +1375,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1375,7 +1404,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1501,6 +1529,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3350-48DF-A99C-6FB4100C1476}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1521,6 +1554,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1555,7 +1589,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1580,7 +1613,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1747,6 +1780,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-41B7-4161-A3FD-A74535C0EF25}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1871,6 +1909,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-41B7-4161-A3FD-A74535C0EF25}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1891,6 +1934,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1935,7 +1979,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2010,7 +2053,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2189,6 +2232,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-111F-41C6-80A4-5A2D634965A5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2349,6 +2397,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-111F-41C6-80A4-5A2D634965A5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2509,6 +2562,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-111F-41C6-80A4-5A2D634965A5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2590,7 +2648,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2625,7 +2689,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2660,7 +2730,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2695,7 +2771,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2756,7 +2838,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2789,9 +2871,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2824,6 +2923,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3006,27 +3122,27 @@
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="10" width="19.140625" customWidth="1"/>
+    <col min="1" max="2" width="29.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" customWidth="1"/>
+    <col min="9" max="10" width="19.109375" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" customWidth="1"/>
-    <col min="15" max="15" width="22.140625" customWidth="1"/>
-    <col min="16" max="16" width="13.5703125" customWidth="1"/>
-    <col min="17" max="18" width="11.7109375" customWidth="1"/>
-    <col min="24" max="24" width="13.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.44140625" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" customWidth="1"/>
+    <col min="14" max="14" width="16.44140625" customWidth="1"/>
+    <col min="15" max="15" width="22.109375" customWidth="1"/>
+    <col min="16" max="16" width="13.5546875" customWidth="1"/>
+    <col min="17" max="18" width="11.6640625" customWidth="1"/>
+    <col min="24" max="24" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -3100,7 +3216,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
@@ -3140,7 +3256,7 @@
       </c>
       <c r="X2" s="13"/>
     </row>
-    <row r="3" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>73</v>
       </c>
@@ -3223,7 +3339,7 @@
         <v>152933.91443632296</v>
       </c>
     </row>
-    <row r="4" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>66</v>
       </c>
@@ -3305,7 +3421,7 @@
         <v>159421.04879802052</v>
       </c>
     </row>
-    <row r="5" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>67</v>
       </c>
@@ -3383,7 +3499,7 @@
         <v>95175.878673873827</v>
       </c>
     </row>
-    <row r="6" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>68</v>
       </c>
@@ -3465,7 +3581,7 @@
         <v>195739.6186738738</v>
       </c>
     </row>
-    <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>69</v>
       </c>
@@ -3547,7 +3663,7 @@
         <v>224772.84879802051</v>
       </c>
     </row>
-    <row r="8" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>70</v>
       </c>
@@ -3627,7 +3743,7 @@
         <v>165279.47443632298</v>
       </c>
     </row>
-    <row r="9" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>71</v>
       </c>
@@ -3707,7 +3823,7 @@
         <v>163225.10879802052</v>
       </c>
     </row>
-    <row r="10" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>72</v>
       </c>
@@ -3786,7 +3902,7 @@
         <v>95273.418673873821</v>
       </c>
     </row>
-    <row r="11" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>74</v>
       </c>
@@ -3867,7 +3983,7 @@
         <v>120488.03413371182</v>
       </c>
     </row>
-    <row r="12" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>75</v>
       </c>
@@ -3947,7 +4063,7 @@
         <v>133197.42073992686</v>
       </c>
     </row>
-    <row r="13" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>76</v>
       </c>
@@ -4028,7 +4144,7 @@
         <v>230247.84071821815</v>
       </c>
     </row>
-    <row r="14" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>77</v>
       </c>
@@ -4108,7 +4224,7 @@
         <v>129617.49413371182</v>
       </c>
     </row>
-    <row r="15" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>78</v>
       </c>
@@ -4189,13 +4305,13 @@
         <v>134657.82111821815</v>
       </c>
     </row>
-    <row r="27" spans="17:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="17:17" x14ac:dyDescent="0.3">
       <c r="Q27">
         <f>0.02/1000</f>
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="42" spans="18:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="18:25" x14ac:dyDescent="0.3">
       <c r="R42" s="5" t="s">
         <v>52</v>
       </c>
@@ -4209,12 +4325,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="18:25" x14ac:dyDescent="0.25">
+    <row r="43" spans="18:25" x14ac:dyDescent="0.3">
       <c r="S43" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="18:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="18:25" x14ac:dyDescent="0.3">
       <c r="R44" t="s">
         <v>55</v>
       </c>
@@ -4234,7 +4350,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="18:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="18:25" x14ac:dyDescent="0.3">
       <c r="S45" t="s">
         <v>57</v>
       </c>
@@ -4245,7 +4361,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="18:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="18:25" x14ac:dyDescent="0.3">
       <c r="R46" t="s">
         <v>60</v>
       </c>
@@ -4281,9 +4397,9 @@
       <selection sqref="A1:U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -4348,7 +4464,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -4413,7 +4529,7 @@
         <v>-1373.815837057527</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -4478,7 +4594,7 @@
         <v>-321.65076096138819</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -4543,7 +4659,7 @@
         <v>1353.871209043366</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -4608,7 +4724,7 @@
         <v>4205.9986197914886</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -4673,7 +4789,7 @@
         <v>9052.7861231763327</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -4738,7 +4854,7 @@
         <v>17327.544791986678</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -4803,7 +4919,7 @@
         <v>30945.693748588084</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -4868,7 +4984,7 @@
         <v>51600.195925279462</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -4933,7 +5049,7 @@
         <v>77844.306419449145</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -4998,7 +5114,7 @@
         <v>100829.28687112352</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -5063,7 +5179,7 @@
         <v>108068.62611646316</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -5128,7 +5244,7 @@
         <v>101444.91585048511</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -5193,7 +5309,7 @@
         <v>92345.005007169064</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -5258,7 +5374,7 @@
         <v>83974.336359869762</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -5323,7 +5439,7 @@
         <v>76346.625731803113</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -5388,7 +5504,7 @@
         <v>69411.768801733138</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -5453,7 +5569,7 @@
         <v>63104.21955120506</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -5518,7 +5634,7 @@
         <v>57369.846455304127</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -5583,7 +5699,7 @@
         <v>52154.405868458292</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -5648,7 +5764,7 @@
         <v>47413.096244052984</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -5730,9 +5846,9 @@
       <selection activeCell="S46" sqref="S46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -5797,7 +5913,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -5862,7 +5978,7 @@
         <v>-1237.5328644674091</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -5927,7 +6043,7 @@
         <v>-197.75714951582648</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -5992,7 +6108,7 @@
         <v>1466.5017649029676</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -6057,7 +6173,7 @@
         <v>4308.3900342093084</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -6122,7 +6238,7 @@
         <v>9145.8692271925338</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -6187,7 +6303,7 @@
         <v>17412.165795637768</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -6252,7 +6368,7 @@
         <v>31022.621933725437</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -6317,7 +6433,7 @@
         <v>51670.13063904069</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -6382,7 +6498,7 @@
         <v>77907.883431959359</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -6447,7 +6563,7 @@
         <v>100887.08415522371</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -6512,7 +6628,7 @@
         <v>108121.16910200879</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -6577,7 +6693,7 @@
         <v>101492.68220098114</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -6642,7 +6758,7 @@
         <v>92388.428962165461</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -6707,7 +6823,7 @@
         <v>84013.812682593751</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -6772,7 +6888,7 @@
         <v>76382.513297915822</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -6837,7 +6953,7 @@
         <v>69444.393861835604</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -6902,7 +7018,7 @@
         <v>63133.878696752763</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -6967,7 +7083,7 @@
         <v>57396.809314892947</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -7032,7 +7148,7 @@
         <v>52178.917558993584</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -7097,7 +7213,7 @@
         <v>47435.379599085063</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -7179,12 +7295,12 @@
       <selection sqref="A1:U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="19" max="19" width="16.85546875" customWidth="1"/>
+    <col min="19" max="19" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -7249,7 +7365,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -7314,7 +7430,7 @@
         <v>-1298.1283124115794</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -7379,7 +7495,7 @@
         <v>-252.84392037416305</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -7444,7 +7560,7 @@
         <v>1416.4228823044798</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -7509,7 +7625,7 @@
         <v>4262.8637773015917</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -7574,7 +7690,7 @@
         <v>9104.4817209127905</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -7639,7 +7755,7 @@
         <v>17374.540789928909</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -7704,7 +7820,7 @@
         <v>30988.417383081021</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -7769,7 +7885,7 @@
         <v>51639.035593000321</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -7834,7 +7950,7 @@
         <v>77879.615208286297</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -7899,7 +8015,7 @@
         <v>100861.38577006638</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -7964,7 +8080,7 @@
         <v>108097.80693368394</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -8029,7 +8145,7 @@
         <v>101471.44386614037</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -8094,7 +8210,7 @@
         <v>92369.121385037477</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -8159,7 +8275,7 @@
         <v>83996.260339750137</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -8224,7 +8340,7 @@
         <v>76366.556622603443</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -8289,7 +8405,7 @@
         <v>69429.88779336981</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -8354,7 +8470,7 @@
         <v>63120.691361783851</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -8419,7 +8535,7 @@
         <v>57384.820828557575</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -8484,7 +8600,7 @@
         <v>52168.018935052336</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -8549,7 +8665,7 @@
         <v>47425.471759138476</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -8631,9 +8747,9 @@
       <selection sqref="A1:U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -8698,7 +8814,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -8763,7 +8879,7 @@
         <v>-1072.7975413371182</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -8828,7 +8944,7 @@
         <v>-462.5432193973802</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -8893,7 +9009,7 @@
         <v>487.9359162503157</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -8958,7 +9074,7 @@
         <v>2077.2370087624954</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -9023,7 +9139,7 @@
         <v>4770.1676515694826</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -9088,7 +9204,7 @@
         <v>9348.0962295563986</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -9153,7 +9269,7 @@
         <v>16866.482417857962</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -9218,7 +9334,7 @@
         <v>28261.05567537887</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -9283,7 +9399,7 @@
         <v>42734.689615525116</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -9348,7 +9464,7 @@
         <v>55408.863800220242</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -9413,7 +9529,7 @@
         <v>59408.21219880171</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -9478,7 +9594,7 @@
         <v>55769.74896186671</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -9543,7 +9659,7 @@
         <v>50770.125468065649</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -9608,7 +9724,7 @@
         <v>46166.477823116569</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -9673,7 +9789,7 @@
         <v>41973.317263804332</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -9738,7 +9854,7 @@
         <v>38161.008394423945</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -9803,7 +9919,7 @@
         <v>34693.392742890363</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -9868,7 +9984,7 @@
         <v>31540.872429698233</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -9933,7 +10049,7 @@
         <v>28673.520390634752</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -9998,7 +10114,7 @@
         <v>26066.836718758859</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -10080,9 +10196,9 @@
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -10147,7 +10263,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -10212,7 +10328,7 @@
         <v>-2032.9008073992691</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -10277,7 +10393,7 @@
         <v>-1128.0916430902446</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -10342,7 +10458,7 @@
         <v>251.8175145460585</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -10407,7 +10523,7 @@
         <v>2533.3577705490084</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -10472,7 +10588,7 @@
         <v>6358.5132112565598</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -10537,7 +10653,7 @@
         <v>12835.126259756675</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -10602,7 +10718,7 @@
         <v>23449.093309573149</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -10667,7 +10783,7 @@
         <v>39515.176006102003</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -10732,7 +10848,7 @@
         <v>59911.816386371538</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -10797,7 +10913,7 @@
         <v>77775.728398294057</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -10862,7 +10978,7 @@
         <v>83426.285578198047</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -10927,7 +11043,7 @@
         <v>78323.574606690105</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -10992,7 +11108,7 @@
         <v>71299.603601721174</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -11057,7 +11173,7 @@
         <v>64835.896513405729</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -11122,7 +11238,7 @@
         <v>58946.780063178769</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -11187,7 +11303,7 @@
         <v>53592.578202964956</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -11252,7 +11368,7 @@
         <v>48722.614878762637</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -11317,7 +11433,7 @@
         <v>44295.185562242019</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -11382,7 +11498,7 @@
         <v>40268.350511129102</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -11447,7 +11563,7 @@
         <v>36607.591373753719</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -11529,9 +11645,9 @@
       <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -11596,7 +11712,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -11661,7 +11777,7 @@
         <v>-11486.239659399269</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -11726,7 +11842,7 @@
         <v>-9514.7633267266083</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -11791,7 +11907,7 @@
         <v>-7003.5038507431964</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -11856,7 +11972,7 @@
         <v>-3391.6150709235671</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -11921,7 +12037,7 @@
         <v>2145.864586162646</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -11986,7 +12102,7 @@
         <v>11048.525212883327</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -12051,7 +12167,7 @@
         <v>25237.4941312214</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -12116,7 +12232,7 @@
         <v>46410.923545855207</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -12181,7 +12297,7 @@
         <v>73126.786074518022</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -12246,7 +12362,7 @@
         <v>96540.632012095215</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -12311,7 +12427,7 @@
         <v>104169.84897189197</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -12376,7 +12492,7 @@
         <v>97900.572991784036</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -12441,7 +12557,7 @@
         <v>89122.875135622628</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -12506,7 +12622,7 @@
         <v>81045.127385736647</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -12571,7 +12687,7 @@
         <v>73683.708482591188</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -12636,7 +12752,7 @@
         <v>66990.93493881321</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -12701,7 +12817,7 @@
         <v>60903.461494005125</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -12766,7 +12882,7 @@
         <v>55369.157312395095</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -12831,7 +12947,7 @@
         <v>50335.597556722809</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -12896,7 +13012,7 @@
         <v>45759.634142475268</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -12978,9 +13094,9 @@
       <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -13045,7 +13161,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -13110,7 +13226,7 @@
         <v>-1481.7435413371186</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -13175,7 +13291,7 @@
         <v>-419.76685576101687</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -13240,7 +13356,7 @@
         <v>1264.6747592255217</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -13305,7 +13421,7 @@
         <v>4124.9109381389026</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -13370,7 +13486,7 @@
         <v>8979.0700489467108</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -13435,7 +13551,7 @@
         <v>17260.530179050653</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -13500,7 +13616,7 @@
         <v>30884.771373191699</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -13565,7 +13681,7 @@
         <v>51544.811947646391</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -13630,7 +13746,7 @@
         <v>77793.957348873635</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -13695,7 +13811,7 @@
         <v>100783.51498878215</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -13760,7 +13876,7 @@
         <v>108027.01531433463</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -13825,7 +13941,7 @@
         <v>101407.08784855009</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -13890,7 +14006,7 @@
         <v>92310.615914500857</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -13955,7 +14071,7 @@
         <v>83943.073548353204</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -14020,7 +14136,7 @@
         <v>76318.204994060783</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -14085,7 +14201,7 @@
         <v>69385.931767421935</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -14150,7 +14266,7 @@
         <v>63080.731338194877</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -14215,7 +14331,7 @@
         <v>57348.49353438578</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -14280,7 +14396,7 @@
         <v>52134.994122168886</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -14345,7 +14461,7 @@
         <v>47395.4492019717</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -14427,9 +14543,9 @@
       <selection activeCell="R39" sqref="R39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -14494,7 +14610,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -14559,7 +14675,7 @@
         <v>-1927.2108073992695</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -14624,7 +14740,7 @@
         <v>-824.73709763569946</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -14689,7 +14805,7 @@
         <v>896.51999388490117</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -14754,7 +14870,7 @@
         <v>3790.2247878292478</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -14819,7 +14935,7 @@
         <v>8674.8099123015691</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -14884,7 +15000,7 @@
         <v>16983.930054827797</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -14949,7 +15065,7 @@
         <v>30633.316714807286</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -15014,7 +15130,7 @@
         <v>51316.216803660558</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -15079,7 +15195,7 @@
         <v>77586.143581613782</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -15144,7 +15260,7 @@
         <v>100594.59338218228</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -15209,7 +15325,7 @@
         <v>107855.26839924385</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -15274,7 +15390,7 @@
         <v>101250.95428937666</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -15339,7 +15455,7 @@
         <v>92168.676315252291</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -15404,7 +15520,7 @@
         <v>83814.037549036337</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -15469,7 +15585,7 @@
         <v>76200.89954013635</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -15534,7 +15650,7 @@
         <v>69279.29044567245</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -15599,7 +15715,7 @@
         <v>62983.784682058984</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -15664,7 +15780,7 @@
         <v>57260.360210625877</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -15729,7 +15845,7 @@
         <v>52054.872918750792</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -15794,7 +15910,7 @@
         <v>47322.611744318885</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -15876,26 +15992,26 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="1" max="1" width="30.88671875" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="34.5546875" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" customWidth="1"/>
-    <col min="15" max="15" width="25.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.88671875" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" customWidth="1"/>
+    <col min="14" max="14" width="16.44140625" customWidth="1"/>
+    <col min="15" max="15" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -15942,7 +16058,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -16002,7 +16118,7 @@
         <v>134657.82111821815</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -16053,7 +16169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -16102,7 +16218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -16151,7 +16267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -16198,7 +16314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -16245,7 +16361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -16294,7 +16410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -16342,7 +16458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -16390,7 +16506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>74</v>
       </c>
@@ -16441,7 +16557,7 @@
         <v>14169.78698450634</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>75</v>
       </c>
@@ -16490,7 +16606,7 @@
         <v>1460.4003782912914</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>76</v>
       </c>
@@ -16537,7 +16653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -16586,7 +16702,7 @@
         <v>5040.3269845063332</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>78</v>
       </c>
@@ -16634,7 +16750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
@@ -16667,14 +16783,14 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="39.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>22</v>
       </c>
@@ -16682,7 +16798,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
@@ -16690,7 +16806,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>73</v>
       </c>
@@ -16699,7 +16815,7 @@
         <v>2121.2871443632298</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>66</v>
       </c>
@@ -16708,7 +16824,7 @@
         <v>2770.5428879802053</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>67</v>
       </c>
@@ -16717,7 +16833,7 @@
         <v>2417.7849867387386</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>68</v>
       </c>
@@ -16726,7 +16842,7 @@
         <v>12474.158986738737</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>69</v>
       </c>
@@ -16735,7 +16851,7 @@
         <v>9305.722887980206</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>70</v>
       </c>
@@ -16744,7 +16860,7 @@
         <v>3355.8431443632298</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>71</v>
       </c>
@@ -16753,7 +16869,7 @@
         <v>3150.9488879802052</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>72</v>
       </c>
@@ -16762,7 +16878,7 @@
         <v>2427.5389867387385</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>74</v>
       </c>
@@ -16771,7 +16887,7 @@
         <v>1708.7975413371182</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>75</v>
       </c>
@@ -16780,7 +16896,7 @@
         <v>2920.9008073992691</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>76</v>
       </c>
@@ -16789,7 +16905,7 @@
         <v>12626.112007182181</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>77</v>
       </c>
@@ -16798,7 +16914,7 @@
         <v>2621.7435413371186</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>78</v>
       </c>
@@ -16825,22 +16941,22 @@
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" customWidth="1"/>
+    <col min="7" max="7" width="23.5546875" customWidth="1"/>
     <col min="8" max="8" width="23" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" customWidth="1"/>
-    <col min="34" max="34" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
+    <col min="34" max="34" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -16920,7 +17036,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2018</v>
       </c>
@@ -17023,7 +17139,7 @@
         <v>-1927.1838111821821</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2019</v>
       </c>
@@ -17125,7 +17241,7 @@
         <v>-824.71255562016552</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2020</v>
       </c>
@@ -17236,7 +17352,7 @@
         <v>896.54230480811384</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2021</v>
       </c>
@@ -17348,7 +17464,7 @@
         <v>3790.2450704867142</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2022</v>
       </c>
@@ -17460,7 +17576,7 @@
         <v>8674.8283510810834</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2023</v>
       </c>
@@ -17572,7 +17688,7 @@
         <v>16983.94681735463</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2024</v>
       </c>
@@ -17684,7 +17800,7 @@
         <v>30633.331953468041</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>2025</v>
       </c>
@@ -17795,7 +17911,7 @@
         <v>51316.230656988519</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>2026</v>
       </c>
@@ -17906,7 +18022,7 @@
         <v>77586.156175548298</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2027</v>
       </c>
@@ -18017,7 +18133,7 @@
         <v>100594.60483121366</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>2028</v>
       </c>
@@ -18129,7 +18245,7 @@
         <v>107855.2788074542</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2029</v>
       </c>
@@ -18240,7 +18356,7 @@
         <v>101250.96375138607</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2030</v>
       </c>
@@ -18351,7 +18467,7 @@
         <v>92168.684917079023</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2031</v>
       </c>
@@ -18462,7 +18578,7 @@
         <v>83814.045368878811</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2032</v>
       </c>
@@ -18573,7 +18689,7 @@
         <v>76200.906649084063</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2033</v>
       </c>
@@ -18684,7 +18800,7 @@
         <v>69279.296908352189</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2034</v>
       </c>
@@ -18795,7 +18911,7 @@
         <v>62983.790557222375</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2035</v>
       </c>
@@ -18897,7 +19013,7 @@
         <v>57260.365551683506</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>2036</v>
       </c>
@@ -18999,7 +19115,7 @@
         <v>52054.877774257729</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>2037</v>
       </c>
@@ -19101,7 +19217,7 @@
         <v>47322.616158416102</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>2038</v>
       </c>
@@ -19203,7 +19319,7 @@
         <v>43020.560144014649</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
       <c r="J25" s="3">
         <v>29262</v>
       </c>
@@ -19214,7 +19330,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -19222,7 +19338,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -19245,7 +19361,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>2018</v>
       </c>
@@ -19280,7 +19396,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>2019</v>
       </c>
@@ -19315,7 +19431,7 @@
         <v>2049</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>2020</v>
       </c>
@@ -19344,7 +19460,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>2021</v>
       </c>
@@ -19373,7 +19489,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>2022</v>
       </c>
@@ -19402,7 +19518,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>2023</v>
       </c>
@@ -19431,7 +19547,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>2024</v>
       </c>
@@ -19474,7 +19590,7 @@
       <c r="AC35" s="10"/>
       <c r="AD35" s="10"/>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>2025</v>
       </c>
@@ -19503,7 +19619,7 @@
         <v>7008</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>2026</v>
       </c>
@@ -19532,7 +19648,7 @@
         <v>11517</v>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>2027</v>
       </c>
@@ -19561,7 +19677,7 @@
         <v>16335</v>
       </c>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>2028</v>
       </c>
@@ -19590,7 +19706,7 @@
         <v>19227</v>
       </c>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>2029</v>
       </c>
@@ -19619,7 +19735,7 @@
         <v>19847</v>
       </c>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>2030</v>
       </c>
@@ -19648,7 +19764,7 @@
         <v>19876</v>
       </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>2031</v>
       </c>
@@ -19677,7 +19793,7 @@
         <v>19880</v>
       </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>2032</v>
       </c>
@@ -19706,7 +19822,7 @@
         <v>19882</v>
       </c>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>2033</v>
       </c>
@@ -19735,7 +19851,7 @@
         <v>19884</v>
       </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>2034</v>
       </c>
@@ -19764,7 +19880,7 @@
         <v>19885</v>
       </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>2035</v>
       </c>
@@ -19793,7 +19909,7 @@
         <v>19886</v>
       </c>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>2036</v>
       </c>
@@ -19822,7 +19938,7 @@
         <v>19886</v>
       </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>2037</v>
       </c>
@@ -19851,7 +19967,7 @@
         <v>19886</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>2038</v>
       </c>
@@ -19880,12 +19996,12 @@
         <v>19886</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>24</v>
       </c>
@@ -19908,7 +20024,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>2018</v>
       </c>
@@ -19937,7 +20053,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>2019</v>
       </c>
@@ -19966,7 +20082,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>2020</v>
       </c>
@@ -19995,7 +20111,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>2021</v>
       </c>
@@ -20024,7 +20140,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>2022</v>
       </c>
@@ -20053,7 +20169,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>2023</v>
       </c>
@@ -20082,7 +20198,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>2024</v>
       </c>
@@ -20111,7 +20227,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>2025</v>
       </c>
@@ -20140,7 +20256,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>2026</v>
       </c>
@@ -20169,7 +20285,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>2027</v>
       </c>
@@ -20198,7 +20314,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>2028</v>
       </c>
@@ -20227,7 +20343,7 @@
         <v>1447</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>2029</v>
       </c>
@@ -20256,7 +20372,7 @@
         <v>1494</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>2030</v>
       </c>
@@ -20285,7 +20401,7 @@
         <v>1495</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>2031</v>
       </c>
@@ -20314,7 +20430,7 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>2032</v>
       </c>
@@ -20343,7 +20459,7 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>2033</v>
       </c>
@@ -20372,7 +20488,7 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>2034</v>
       </c>
@@ -20401,7 +20517,7 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>2035</v>
       </c>
@@ -20430,7 +20546,7 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>2036</v>
       </c>
@@ -20459,7 +20575,7 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>2037</v>
       </c>
@@ -20488,7 +20604,7 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>2038</v>
       </c>
@@ -20535,12 +20651,12 @@
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="19" max="19" width="14.85546875" customWidth="1"/>
+    <col min="19" max="19" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -20605,7 +20721,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -20670,7 +20786,7 @@
         <v>-2190.4</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -20735,7 +20851,7 @@
         <v>-1745.8181818181818</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -20800,7 +20916,7 @@
         <v>-1152.7272727272725</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -20865,7 +20981,7 @@
         <v>-271.6754320060104</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -20930,7 +21046,7 @@
         <v>1132.4363089952869</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -20995,7 +21111,7 @@
         <v>3421.2764900559437</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -21060,7 +21176,7 @@
         <v>7111.4683603895064</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -21125,7 +21241,7 @@
         <v>12637.031819549376</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -21190,7 +21306,7 @@
         <v>19631.750176938076</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -21255,7 +21371,7 @@
         <v>25757.144754234483</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -21320,7 +21436,7 @@
         <v>27732.128808666199</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -21385,7 +21501,7 @@
         <v>26051.37036309313</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -21450,7 +21566,7 @@
         <v>23718.623165704772</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -21515,7 +21631,7 @@
         <v>21567.598654930509</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -21580,7 +21696,7 @@
         <v>19609.751845665145</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -21645,7 +21761,7 @@
         <v>17828.770755178317</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -21710,7 +21826,7 @@
         <v>16208.756878687314</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -21775,7 +21891,7 @@
         <v>14735.233526079377</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -21840,7 +21956,7 @@
         <v>13396.314333534016</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -21905,7 +22021,7 @@
         <v>12178.467575940011</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -21987,9 +22103,9 @@
       <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -22054,7 +22170,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -22119,7 +22235,7 @@
         <v>-643.25983705752697</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -22184,7 +22300,7 @@
         <v>-72.05439732502451</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -22249,7 +22365,7 @@
         <v>842.92575449791173</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -22314,7 +22430,7 @@
         <v>2399.955043533037</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -22379,7 +22495,7 @@
         <v>5063.5476831790656</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -22444,7 +22560,7 @@
         <v>9614.8053492014751</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -22509,7 +22625,7 @@
         <v>17108.945253898943</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -22574,7 +22690,7 @@
         <v>28481.47643541612</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -22639,7 +22755,7 @@
         <v>42935.072124649887</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -22704,7 +22820,7 @@
         <v>55591.029717606398</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -22769,7 +22885,7 @@
         <v>59573.817578243667</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -22834,7 +22950,7 @@
         <v>55920.299306813948</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -22899,7 +23015,7 @@
         <v>50906.989418017678</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -22964,7 +23080,7 @@
         <v>46290.899595800242</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -23029,7 +23145,7 @@
         <v>42086.427966244024</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -23094,7 +23210,7 @@
         <v>38263.836305732766</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -23159,7 +23275,7 @@
         <v>34786.872662262016</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -23224,7 +23340,7 @@
         <v>31625.854174581553</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -23289,7 +23405,7 @@
         <v>28750.776522346863</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -23354,7 +23470,7 @@
         <v>26137.069565769867</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -23436,9 +23552,9 @@
       <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -23503,7 +23619,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -23568,7 +23684,7 @@
         <v>-1109.126864467409</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -23633,7 +23749,7 @@
         <v>-288.29714951582633</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -23698,7 +23814,7 @@
         <v>1015.2670541591659</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -23763,7 +23879,7 @@
         <v>3227.4028065609241</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -23828,7 +23944,7 @@
         <v>6989.4632439946645</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -23893,7 +24009,7 @@
         <v>13408.717198609498</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -23958,7 +24074,7 @@
         <v>23970.539617621173</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -24023,7 +24139,7 @@
         <v>39989.218104327483</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -24088,7 +24204,7 @@
         <v>60342.763748394696</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -24153,7 +24269,7 @@
         <v>78167.498727406026</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -24218,7 +24334,7 @@
         <v>83782.440422845291</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -24283,7 +24399,7 @@
         <v>78647.351738187601</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -24348,7 +24464,7 @@
         <v>71593.946448537085</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -24413,7 +24529,7 @@
         <v>65103.480919602007</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -24478,7 +24594,7 @@
         <v>59190.038614266297</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -24543,7 +24659,7 @@
         <v>53813.722340317247</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -24608,7 +24724,7 @@
         <v>48923.655003628359</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -24673,7 +24789,7 @@
         <v>44477.949312119948</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -24738,7 +24854,7 @@
         <v>40434.499374654493</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -24803,7 +24919,7 @@
         <v>36758.635795140442</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -24885,9 +25001,9 @@
       <selection sqref="A1:U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -24952,7 +25068,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -25017,7 +25133,7 @@
         <v>-1540.4913604115791</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -25082,7 +25198,7 @@
         <v>-680.4466912832537</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -25147,7 +25263,7 @@
         <v>658.76747073423201</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -25212,7 +25328,7 @@
         <v>2903.3122761746204</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -25277,7 +25393,7 @@
         <v>6694.8354890980245</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -25342,7 +25458,7 @@
         <v>13140.873785067099</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -25407,7 +25523,7 @@
         <v>23727.045605309897</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -25472,7 +25588,7 @@
         <v>39767.859911317231</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -25537,7 +25653,7 @@
         <v>60141.529027476296</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -25602,7 +25718,7 @@
         <v>77984.558072025655</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -25667,7 +25783,7 @@
         <v>83616.130736135863</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -25732,7 +25848,7 @@
         <v>78496.161113906302</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -25797,7 +25913,7 @@
         <v>71456.500426463172</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -25862,7 +25978,7 @@
         <v>64978.529990443909</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -25927,7 +26043,7 @@
         <v>59076.446860486205</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -25992,7 +26108,7 @@
         <v>53710.457109608076</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -26057,7 +26173,7 @@
         <v>48829.777521165473</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -26122,7 +26238,7 @@
         <v>44392.606146244601</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -26187,7 +26303,7 @@
         <v>40356.91467840418</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -26252,7 +26368,7 @@
         <v>36688.104253094702</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -26334,9 +26450,9 @@
       <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -26401,7 +26517,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -26466,7 +26582,7 @@
         <v>-11344.748312411579</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -26531,7 +26647,7 @@
         <v>-9386.1348294650707</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -26596,7 +26712,7 @@
         <v>-6886.5688532327094</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -26661,7 +26777,7 @@
         <v>-3285.3105277322147</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -26726,7 +26842,7 @@
         <v>2242.5050799729665</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -26791,7 +26907,7 @@
         <v>11136.380207256343</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -26856,7 +26972,7 @@
         <v>25317.362307924141</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -26921,7 +27037,7 @@
         <v>46483.530979221337</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -26986,7 +27102,7 @@
         <v>73192.792832123596</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -27051,7 +27167,7 @@
         <v>96600.638155373017</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -27116,7 +27232,7 @@
         <v>104224.40001123541</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -27181,7 +27297,7 @@
         <v>97950.164845732623</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -27246,7 +27362,7 @@
         <v>89167.958639212258</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -27311,7 +27427,7 @@
         <v>81086.112388999929</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -27376,7 +27492,7 @@
         <v>73720.967576466894</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -27441,7 +27557,7 @@
         <v>67024.806842336591</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -27506,7 +27622,7 @@
         <v>60934.254133571834</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -27571,7 +27687,7 @@
         <v>55397.1506210921</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -27636,7 +27752,7 @@
         <v>50361.046019174632</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -27701,7 +27817,7 @@
         <v>45782.769108340566</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -27783,9 +27899,9 @@
       <selection sqref="A1:U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -27850,7 +27966,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -27915,7 +28031,7 @@
         <v>-7392.4157164674089</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -27980,7 +28096,7 @@
         <v>-5793.1051967885533</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -28045,7 +28161,7 @@
         <v>-3620.1782780722383</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -28110,7 +28226,7 @@
         <v>-315.86455031360538</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -28175,7 +28291,7 @@
         <v>4942.0014230807928</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -28240,7 +28356,7 @@
         <v>13590.46779189982</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -28305,7 +28421,7 @@
         <v>27548.351021236394</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -28370,7 +28486,7 @@
         <v>48511.702536777928</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -28435,7 +28551,7 @@
         <v>75036.585157175039</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -28500,7 +28616,7 @@
         <v>98276.812996328881</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -28565,7 +28681,7 @@
         <v>105748.19532119529</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -28630,7 +28746,7 @@
         <v>99335.433309332511</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -28695,7 +28811,7 @@
         <v>90427.293606121239</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -28760,7 +28876,7 @@
         <v>82230.962358917197</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -28825,7 +28941,7 @@
         <v>74761.740276391676</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -28890,7 +29006,7 @@
         <v>67970.963842268204</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -28955,7 +29071,7 @@
         <v>61794.396860782392</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -29020,7 +29136,7 @@
         <v>56179.098554919889</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -29085,7 +29201,7 @@
         <v>51071.907777199893</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -29150,7 +29266,7 @@
         <v>46429.007070181709</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2038</v>
       </c>

</xml_diff>

<commit_message>
opex without building rent
</commit_message>
<xml_diff>
--- a/tumlknexpectimax/excel_data/input_data_business.xlsx
+++ b/tumlknexpectimax/excel_data/input_data_business.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmadzay\LRZ Sync+Share\PycharmProjects\mt_branch_new_code\tumlknexpectimax\tumlknexpectimax\excel_data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="828" windowWidth="13680" windowHeight="11076" tabRatio="847" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="825" windowWidth="13680" windowHeight="11070" tabRatio="847" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CAPEX" sheetId="1" r:id="rId1"/>
@@ -31,7 +26,7 @@
     <sheet name="FTTB_Hybridpon_100" sheetId="19" r:id="rId17"/>
     <sheet name="MIG_MATRIX" sheetId="11" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -41,7 +36,7 @@
     <author>Patri, Sai Kireet</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0" shapeId="0">
+    <comment ref="B3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -66,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="C3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -91,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H4" authorId="0" shapeId="0">
+    <comment ref="H4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -117,7 +112,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0">
+    <comment ref="H5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -141,7 +136,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H6" authorId="0" shapeId="0">
+    <comment ref="H6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -166,7 +161,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H7" authorId="0" shapeId="0">
+    <comment ref="H7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -191,7 +186,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0" shapeId="0">
+    <comment ref="C8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -547,7 +542,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000000%"/>
   </numFmts>
@@ -772,9 +767,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -920,7 +915,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F92B-4BDB-8C8A-80B4841F7958}"/>
             </c:ext>
@@ -1036,7 +1031,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-F92B-4BDB-8C8A-80B4841F7958}"/>
             </c:ext>
@@ -1152,7 +1147,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-F92B-4BDB-8C8A-80B4841F7958}"/>
             </c:ext>
@@ -1268,7 +1263,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-F92B-4BDB-8C8A-80B4841F7958}"/>
             </c:ext>
@@ -1284,11 +1279,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="219419136"/>
-        <c:axId val="220160576"/>
+        <c:axId val="152826880"/>
+        <c:axId val="152840448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="219419136"/>
+        <c:axId val="152826880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1316,7 +1311,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="220160576"/>
+        <c:crossAx val="152840448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1324,7 +1319,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="220160576"/>
+        <c:axId val="152840448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1353,7 +1348,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="219419136"/>
+        <c:crossAx val="152826880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1375,9 +1370,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1404,6 +1399,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1485,51 +1481,51 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>51114.587309311035</c:v>
+                  <c:v>36062.342937580564</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30429.282118970365</c:v>
+                  <c:v>19283.042118970367</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>66109.823692218881</c:v>
+                  <c:v>43709.823692218881</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>66648.422052537615</c:v>
+                  <c:v>44248.4220525376</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8108.705667292159</c:v>
+                  <c:v>10540.776519765759</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8798.3519740095981</c:v>
+                  <c:v>11938.918689039821</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69659.850521829372</c:v>
+                  <c:v>50983.71612182937</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70126.863400003014</c:v>
+                  <c:v>47726.863400003029</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>70620.289169209602</c:v>
+                  <c:v>48220.289169209609</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>51210.227713520049</c:v>
+                  <c:v>37682.867713520049</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>67227.8721002112</c:v>
+                  <c:v>44827.8721002112</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>12139.814930199653</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>70921.654760442281</c:v>
+                  <c:v>47419.574760442287</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>72488.476920599642</c:v>
+                  <c:v>50088.476920599649</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3350-48DF-A99C-6FB4100C1476}"/>
             </c:ext>
@@ -1544,11 +1540,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="220253184"/>
-        <c:axId val="220162880"/>
+        <c:axId val="153448960"/>
+        <c:axId val="152842752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="220253184"/>
+        <c:axId val="153448960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1558,7 +1554,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="220162880"/>
+        <c:crossAx val="152842752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1566,7 +1562,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="220162880"/>
+        <c:axId val="152842752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1589,13 +1585,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="220253184"/>
+        <c:crossAx val="153448960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1613,9 +1610,9 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1780,7 +1777,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-41B7-4161-A3FD-A74535C0EF25}"/>
             </c:ext>
@@ -1909,7 +1906,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-41B7-4161-A3FD-A74535C0EF25}"/>
             </c:ext>
@@ -1924,11 +1921,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="221506048"/>
-        <c:axId val="220164608"/>
+        <c:axId val="153451520"/>
+        <c:axId val="152844480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="221506048"/>
+        <c:axId val="153451520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1945,10 +1942,10 @@
             <a:pPr>
               <a:defRPr sz="1200"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="220164608"/>
+        <c:crossAx val="152844480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1956,7 +1953,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="220164608"/>
+        <c:axId val="152844480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1992,10 +1989,10 @@
             <a:pPr>
               <a:defRPr sz="1200"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221506048"/>
+        <c:crossAx val="153451520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2011,7 +2008,7 @@
             <a:pPr>
               <a:defRPr sz="1400"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
       </c:legendEntry>
@@ -2024,7 +2021,7 @@
             <a:pPr>
               <a:defRPr sz="1400"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
       </c:legendEntry>
@@ -2053,9 +2050,9 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2232,7 +2229,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-111F-41C6-80A4-5A2D634965A5}"/>
             </c:ext>
@@ -2397,7 +2394,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-111F-41C6-80A4-5A2D634965A5}"/>
             </c:ext>
@@ -2562,7 +2559,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-111F-41C6-80A4-5A2D634965A5}"/>
             </c:ext>
@@ -2577,11 +2574,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="221744640"/>
-        <c:axId val="220166912"/>
+        <c:axId val="164004864"/>
+        <c:axId val="163693120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="221744640"/>
+        <c:axId val="164004864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2591,7 +2588,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="220166912"/>
+        <c:crossAx val="163693120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2599,7 +2596,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="220166912"/>
+        <c:axId val="163693120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2610,7 +2607,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="221744640"/>
+        <c:crossAx val="164004864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2651,7 +2648,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2692,7 +2689,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2733,7 +2730,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2774,7 +2771,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0800-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2838,7 +2835,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2871,26 +2868,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2923,23 +2903,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3122,27 +3085,27 @@
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="29.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" customWidth="1"/>
-    <col min="9" max="10" width="19.109375" customWidth="1"/>
+    <col min="1" max="2" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="9" max="10" width="19.140625" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="13.44140625" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" customWidth="1"/>
-    <col min="14" max="14" width="16.44140625" customWidth="1"/>
-    <col min="15" max="15" width="22.109375" customWidth="1"/>
-    <col min="16" max="16" width="13.5546875" customWidth="1"/>
-    <col min="17" max="18" width="11.6640625" customWidth="1"/>
-    <col min="24" max="24" width="13.44140625" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" customWidth="1"/>
+    <col min="15" max="15" width="22.140625" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" customWidth="1"/>
+    <col min="17" max="18" width="11.7109375" customWidth="1"/>
+    <col min="24" max="24" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" s="9" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -3216,7 +3179,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
@@ -3258,7 +3221,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>73</v>
       </c>
@@ -3337,7 +3300,7 @@
         <v>307967.22911888885</v>
       </c>
     </row>
-    <row r="4" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>66</v>
       </c>
@@ -3415,7 +3378,7 @@
         <v>216506.84792333335</v>
       </c>
     </row>
-    <row r="5" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>67</v>
       </c>
@@ -3489,7 +3452,7 @@
         <v>145045.86878666666</v>
       </c>
     </row>
-    <row r="6" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>68</v>
       </c>
@@ -3567,7 +3530,7 @@
         <v>218092.13545333332</v>
       </c>
     </row>
-    <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>69</v>
       </c>
@@ -3645,7 +3608,7 @@
         <v>288249.58125666669</v>
       </c>
     </row>
-    <row r="8" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>70</v>
       </c>
@@ -3721,7 +3684,7 @@
         <v>347869.80689666665</v>
       </c>
     </row>
-    <row r="9" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>71</v>
       </c>
@@ -3797,7 +3760,7 @@
         <v>221159.28125666664</v>
       </c>
     </row>
-    <row r="10" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>72</v>
       </c>
@@ -3872,7 +3835,7 @@
         <v>147813.53545333334</v>
       </c>
     </row>
-    <row r="11" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>74</v>
       </c>
@@ -3949,7 +3912,7 @@
         <v>215033.99423000001</v>
       </c>
     </row>
-    <row r="12" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>75</v>
       </c>
@@ -4025,7 +3988,7 @@
         <v>178789.21166999999</v>
       </c>
     </row>
-    <row r="13" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>76</v>
       </c>
@@ -4102,7 +4065,7 @@
         <v>298182.08727000002</v>
       </c>
     </row>
-    <row r="14" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>77</v>
       </c>
@@ -4178,7 +4141,7 @@
         <v>235044.99423000001</v>
       </c>
     </row>
-    <row r="15" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>78</v>
       </c>
@@ -4255,13 +4218,13 @@
         <v>196669.21166999999</v>
       </c>
     </row>
-    <row r="27" spans="17:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="17:17" ht="14.45" x14ac:dyDescent="0.3">
       <c r="Q27">
         <f>0.02/1000</f>
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="42" spans="18:25" x14ac:dyDescent="0.3">
+    <row r="42" spans="18:25" x14ac:dyDescent="0.25">
       <c r="R42" s="5" t="s">
         <v>52</v>
       </c>
@@ -4275,12 +4238,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="18:25" x14ac:dyDescent="0.3">
+    <row r="43" spans="18:25" x14ac:dyDescent="0.25">
       <c r="S43" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="18:25" x14ac:dyDescent="0.3">
+    <row r="44" spans="18:25" x14ac:dyDescent="0.25">
       <c r="R44" t="s">
         <v>55</v>
       </c>
@@ -4300,7 +4263,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="18:25" x14ac:dyDescent="0.3">
+    <row r="45" spans="18:25" x14ac:dyDescent="0.25">
       <c r="S45" t="s">
         <v>57</v>
       </c>
@@ -4311,7 +4274,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="18:25" x14ac:dyDescent="0.3">
+    <row r="46" spans="18:25" x14ac:dyDescent="0.25">
       <c r="R46" t="s">
         <v>60</v>
       </c>
@@ -4347,7 +4310,7 @@
       <selection sqref="A1:U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -5796,7 +5759,7 @@
       <selection activeCell="S46" sqref="S46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -7245,9 +7208,9 @@
       <selection sqref="A1:U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="19" max="19" width="16.88671875" customWidth="1"/>
+    <col min="19" max="19" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
@@ -8697,7 +8660,7 @@
       <selection sqref="A1:U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -10146,7 +10109,7 @@
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -11595,7 +11558,7 @@
       <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -13044,7 +13007,7 @@
       <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -14493,7 +14456,7 @@
       <selection activeCell="R39" sqref="R39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -15942,23 +15905,23 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" customWidth="1"/>
-    <col min="6" max="6" width="34.5546875" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="16.88671875" customWidth="1"/>
-    <col min="12" max="12" width="12.5546875" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" customWidth="1"/>
-    <col min="14" max="14" width="16.44140625" customWidth="1"/>
-    <col min="15" max="15" width="25.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" customWidth="1"/>
+    <col min="15" max="15" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -16730,17 +16693,17 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="39.88671875" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>22</v>
       </c>
@@ -16748,96 +16711,96 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="12">
         <f>AVERAGE(B3:B15)</f>
-        <v>51114.587309311035</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>36062.342937580564</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>73</v>
       </c>
       <c r="B3" s="12">
-        <v>30429.282118970365</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>19283.042118970367</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>66</v>
       </c>
       <c r="B4" s="12">
-        <v>66109.823692218881</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>43709.823692218881</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>67</v>
       </c>
       <c r="B5" s="12">
-        <v>66648.422052537615</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>44248.4220525376</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>68</v>
       </c>
       <c r="B6" s="12">
-        <v>8108.705667292159</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>10540.776519765759</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>69</v>
       </c>
       <c r="B7" s="12">
-        <v>8798.3519740095981</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>11938.918689039821</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>70</v>
       </c>
       <c r="B8" s="12">
-        <v>69659.850521829372</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>50983.71612182937</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B9" s="12">
-        <v>70126.863400003014</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>47726.863400003029</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>72</v>
       </c>
       <c r="B10" s="12">
-        <v>70620.289169209602</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>48220.289169209609</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>74</v>
       </c>
       <c r="B11" s="12">
-        <v>51210.227713520049</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <v>37682.867713520049</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>75</v>
       </c>
       <c r="B12" s="12">
-        <v>67227.8721002112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>44827.8721002112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>76</v>
       </c>
@@ -16845,20 +16808,20 @@
         <v>12139.814930199653</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>77</v>
       </c>
       <c r="B14" s="12">
-        <v>70921.654760442281</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+        <v>47419.574760442287</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>78</v>
       </c>
       <c r="B15" s="12">
-        <v>72488.476920599642</v>
+        <v>50088.476920599649</v>
       </c>
     </row>
   </sheetData>
@@ -16879,19 +16842,19 @@
       <selection activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" customWidth="1"/>
-    <col min="7" max="7" width="23.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" customWidth="1"/>
     <col min="8" max="8" width="23" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" customWidth="1"/>
-    <col min="34" max="34" width="17.88671875" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="34" max="34" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.3">
@@ -17022,31 +16985,31 @@
       </c>
       <c r="U2" s="7">
         <f>OPEX!$B$15</f>
-        <v>72488.476920599642</v>
+        <v>50088.476920599649</v>
       </c>
       <c r="V2" s="11">
         <f>O2-U2</f>
-        <v>-71204.476920599642</v>
+        <v>-48804.476920599649</v>
       </c>
       <c r="W2" s="11">
         <f>P2-U2</f>
-        <v>-71204.476920599642</v>
+        <v>-48804.476920599649</v>
       </c>
       <c r="X2" s="11">
         <f t="shared" ref="X2:X22" si="1">Q2-U2</f>
-        <v>-71204.476920599642</v>
+        <v>-48804.476920599649</v>
       </c>
       <c r="Y2" s="11">
         <f>R2-$U2</f>
-        <v>-71348.476920599642</v>
+        <v>-48948.476920599649</v>
       </c>
       <c r="Z2" s="11">
         <f>S2-$U2</f>
-        <v>-71348.476920599642</v>
+        <v>-48948.476920599649</v>
       </c>
       <c r="AA2" s="11">
         <f>T2-$U2</f>
-        <v>-71348.476920599642</v>
+        <v>-48948.476920599649</v>
       </c>
       <c r="AB2" s="11">
         <f>1/POWER(1+$L$25,N2-2018)</f>
@@ -17054,27 +17017,27 @@
       </c>
       <c r="AC2" s="12">
         <f>V2*AB2</f>
-        <v>-71204.476920599642</v>
+        <v>-48804.476920599649</v>
       </c>
       <c r="AD2" s="12">
         <f>W2*AB2</f>
-        <v>-71204.476920599642</v>
+        <v>-48804.476920599649</v>
       </c>
       <c r="AE2" s="12">
         <f>X2*AB2</f>
-        <v>-71204.476920599642</v>
+        <v>-48804.476920599649</v>
       </c>
       <c r="AF2" s="12">
         <f>Y2*$AB2</f>
-        <v>-71348.476920599642</v>
+        <v>-48948.476920599649</v>
       </c>
       <c r="AG2" s="12">
         <f>Z2*$AB2</f>
-        <v>-71348.476920599642</v>
+        <v>-48948.476920599649</v>
       </c>
       <c r="AH2" s="12">
         <f>AA2*$AB2</f>
-        <v>-71348.476920599642</v>
+        <v>-48948.476920599649</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.3">
@@ -17124,31 +17087,31 @@
       </c>
       <c r="U3" s="7">
         <f>OPEX!$B$15</f>
-        <v>72488.476920599642</v>
+        <v>50088.476920599649</v>
       </c>
       <c r="V3" s="11">
         <f t="shared" ref="V3:V22" si="8">O3-U3</f>
-        <v>-70772.476920599642</v>
+        <v>-48372.476920599649</v>
       </c>
       <c r="W3" s="11">
         <f t="shared" ref="W3:W22" si="9">P3-U3</f>
-        <v>-70688.476920599642</v>
+        <v>-48288.476920599649</v>
       </c>
       <c r="X3" s="11">
         <f t="shared" si="1"/>
-        <v>-70052.476920599642</v>
+        <v>-47652.476920599649</v>
       </c>
       <c r="Y3" s="11">
         <f t="shared" ref="Y3:Y22" si="10">R3-$U3</f>
-        <v>-70952.476920599642</v>
+        <v>-48552.476920599649</v>
       </c>
       <c r="Z3" s="11">
         <f t="shared" ref="Z3:Z22" si="11">S3-$U3</f>
-        <v>-70880.476920599642</v>
+        <v>-48480.476920599649</v>
       </c>
       <c r="AA3" s="11">
         <f t="shared" ref="AA3:AA22" si="12">T3-$U3</f>
-        <v>-70328.476920599642</v>
+        <v>-47928.476920599649</v>
       </c>
       <c r="AB3" s="11">
         <f t="shared" ref="AB3:AB22" si="13">1/POWER(1+$L$25,N3-2018)</f>
@@ -17156,27 +17119,27 @@
       </c>
       <c r="AC3" s="12">
         <f t="shared" ref="AC3:AC22" si="14">V3*AB3</f>
-        <v>-64338.615382363307</v>
+        <v>-43974.979018726954</v>
       </c>
       <c r="AD3" s="12">
         <f t="shared" ref="AD3:AD22" si="15">W3*AB3</f>
-        <v>-64262.251745999674</v>
+        <v>-43898.615382363314</v>
       </c>
       <c r="AE3" s="12">
         <f t="shared" ref="AE3:AE22" si="16">X3*AB3</f>
-        <v>-63684.069927817851</v>
+        <v>-43320.433564181498</v>
       </c>
       <c r="AF3" s="12">
         <f t="shared" ref="AF3:AF22" si="17">Y3*$AB3</f>
-        <v>-64502.251745999674</v>
+        <v>-44138.615382363314</v>
       </c>
       <c r="AG3" s="12">
         <f t="shared" ref="AG3:AG22" si="18">Z3*$AB3</f>
-        <v>-64436.79720054513</v>
+        <v>-44073.16083690877</v>
       </c>
       <c r="AH3" s="12">
         <f t="shared" ref="AH3:AH22" si="19">AA3*$AB3</f>
-        <v>-63934.979018726946</v>
+        <v>-43571.342655090586</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.3">
@@ -17235,31 +17198,31 @@
       </c>
       <c r="U4" s="7">
         <f>OPEX!$B$15</f>
-        <v>72488.476920599642</v>
+        <v>50088.476920599649</v>
       </c>
       <c r="V4" s="11">
         <f t="shared" si="8"/>
-        <v>-70136.476920599642</v>
+        <v>-47736.476920599649</v>
       </c>
       <c r="W4" s="11">
         <f t="shared" si="9"/>
-        <v>-70016.476920599642</v>
+        <v>-47616.476920599649</v>
       </c>
       <c r="X4" s="11">
         <f t="shared" si="1"/>
-        <v>-67844.476920599642</v>
+        <v>-45444.476920599649</v>
       </c>
       <c r="Y4" s="11">
         <f t="shared" si="10"/>
-        <v>-70400.476920599642</v>
+        <v>-48000.476920599649</v>
       </c>
       <c r="Z4" s="11">
         <f t="shared" si="11"/>
-        <v>-70292.476920599642</v>
+        <v>-47892.476920599649</v>
       </c>
       <c r="AA4" s="11">
         <f t="shared" si="12"/>
-        <v>-68336.476920599642</v>
+        <v>-45936.476920599649</v>
       </c>
       <c r="AB4" s="11">
         <f t="shared" si="13"/>
@@ -17267,27 +17230,27 @@
       </c>
       <c r="AC4" s="12">
         <f t="shared" si="14"/>
-        <v>-57964.030512892263</v>
+        <v>-39451.633818677394</v>
       </c>
       <c r="AD4" s="12">
         <f t="shared" si="15"/>
-        <v>-57864.856959173252</v>
+        <v>-39352.460264958383</v>
       </c>
       <c r="AE4" s="12">
         <f t="shared" si="16"/>
-        <v>-56069.815636859203</v>
+        <v>-37557.418942644334</v>
       </c>
       <c r="AF4" s="12">
         <f t="shared" si="17"/>
-        <v>-58182.212331074079</v>
+        <v>-39669.81563685921</v>
       </c>
       <c r="AG4" s="12">
         <f t="shared" si="18"/>
-        <v>-58092.956132726969</v>
+        <v>-39580.5594385121</v>
       </c>
       <c r="AH4" s="12">
         <f t="shared" si="19"/>
-        <v>-56476.427207107139</v>
+        <v>-37964.03051289227</v>
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.3">
@@ -17347,31 +17310,31 @@
       </c>
       <c r="U5" s="7">
         <f>OPEX!$B$15</f>
-        <v>72488.476920599642</v>
+        <v>50088.476920599649</v>
       </c>
       <c r="V5" s="11">
         <f t="shared" si="8"/>
-        <v>-69308.476920599642</v>
+        <v>-46908.476920599649</v>
       </c>
       <c r="W5" s="11">
         <f t="shared" si="9"/>
-        <v>-68972.476920599642</v>
+        <v>-46572.476920599649</v>
       </c>
       <c r="X5" s="11">
         <f t="shared" si="1"/>
-        <v>-63452.476920599642</v>
+        <v>-41052.476920599649</v>
       </c>
       <c r="Y5" s="11">
         <f t="shared" si="10"/>
-        <v>-69644.476920599642</v>
+        <v>-47244.476920599649</v>
       </c>
       <c r="Z5" s="11">
         <f t="shared" si="11"/>
-        <v>-69332.476920599642</v>
+        <v>-46932.476920599649</v>
       </c>
       <c r="AA5" s="11">
         <f t="shared" si="12"/>
-        <v>-64376.476920599642</v>
+        <v>-41976.476920599649</v>
       </c>
       <c r="AB5" s="11">
         <f t="shared" si="13"/>
@@ -17379,27 +17342,27 @@
       </c>
       <c r="AC5" s="12">
         <f t="shared" si="14"/>
-        <v>-52072.484538391902</v>
+        <v>-35243.03299819657</v>
       </c>
       <c r="AD5" s="12">
         <f t="shared" si="15"/>
-        <v>-51820.04276528897</v>
+        <v>-34990.591225093638</v>
       </c>
       <c r="AE5" s="12">
         <f t="shared" si="16"/>
-        <v>-47672.785064312266</v>
+        <v>-30843.333524116933</v>
       </c>
       <c r="AF5" s="12">
         <f t="shared" si="17"/>
-        <v>-52324.926311494833</v>
+        <v>-35495.474771299501</v>
       </c>
       <c r="AG5" s="12">
         <f t="shared" si="18"/>
-        <v>-52090.516093613536</v>
+        <v>-35261.064553418211</v>
       </c>
       <c r="AH5" s="12">
         <f t="shared" si="19"/>
-        <v>-48366.999940345318</v>
+        <v>-31537.54840014999</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.3">
@@ -17459,31 +17422,31 @@
       </c>
       <c r="U6" s="7">
         <f>OPEX!$B$15</f>
-        <v>72488.476920599642</v>
+        <v>50088.476920599649</v>
       </c>
       <c r="V6" s="11">
         <f t="shared" si="8"/>
-        <v>-68144.476920599642</v>
+        <v>-45744.476920599649</v>
       </c>
       <c r="W6" s="11">
         <f t="shared" si="9"/>
-        <v>-67532.476920599642</v>
+        <v>-45132.476920599649</v>
       </c>
       <c r="X6" s="11">
         <f t="shared" si="1"/>
-        <v>-54956.476920599642</v>
+        <v>-32556.476920599649</v>
       </c>
       <c r="Y6" s="11">
         <f t="shared" si="10"/>
-        <v>-68612.476920599642</v>
+        <v>-46212.476920599649</v>
       </c>
       <c r="Z6" s="11">
         <f t="shared" si="11"/>
-        <v>-68048.476920599642</v>
+        <v>-45648.476920599649</v>
       </c>
       <c r="AA6" s="11">
         <f t="shared" si="12"/>
-        <v>-56720.476920599642</v>
+        <v>-34320.476920599649</v>
       </c>
       <c r="AB6" s="11">
         <f t="shared" si="13"/>
@@ -17491,27 +17454,27 @@
       </c>
       <c r="AC6" s="12">
         <f t="shared" si="14"/>
-        <v>-46543.59464558406</v>
+        <v>-31244.093245406486</v>
       </c>
       <c r="AD6" s="12">
         <f t="shared" si="15"/>
-        <v>-46125.590410900637</v>
+        <v>-30826.089010723063</v>
       </c>
       <c r="AE6" s="12">
         <f t="shared" si="16"/>
-        <v>-37536.013196229513</v>
+        <v>-22236.511796051938</v>
       </c>
       <c r="AF6" s="12">
         <f t="shared" si="17"/>
-        <v>-46863.244942694917</v>
+        <v>-31563.743542517339</v>
       </c>
       <c r="AG6" s="12">
         <f t="shared" si="18"/>
-        <v>-46478.025353869016</v>
+        <v>-31178.523953691441</v>
       </c>
       <c r="AH6" s="12">
         <f t="shared" si="19"/>
-        <v>-38740.8489314935</v>
+        <v>-23441.347531315922</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.3">
@@ -17571,31 +17534,31 @@
       </c>
       <c r="U7" s="7">
         <f>OPEX!$B$15</f>
-        <v>72488.476920599642</v>
+        <v>50088.476920599649</v>
       </c>
       <c r="V7" s="11">
         <f t="shared" si="8"/>
-        <v>-66560.476920599642</v>
+        <v>-44160.476920599649</v>
       </c>
       <c r="W7" s="11">
         <f t="shared" si="9"/>
-        <v>-65492.476920599642</v>
+        <v>-43092.476920599649</v>
       </c>
       <c r="X7" s="11">
         <f t="shared" si="1"/>
-        <v>-38660.476920599642</v>
+        <v>-16260.476920599649</v>
       </c>
       <c r="Y7" s="11">
         <f t="shared" si="10"/>
-        <v>-67160.476920599642</v>
+        <v>-44760.476920599649</v>
       </c>
       <c r="Z7" s="11">
         <f t="shared" si="11"/>
-        <v>-66212.476920599642</v>
+        <v>-43812.476920599649</v>
       </c>
       <c r="AA7" s="11">
         <f t="shared" si="12"/>
-        <v>-42068.476920599642</v>
+        <v>-19668.476920599649</v>
       </c>
       <c r="AB7" s="11">
         <f t="shared" si="13"/>
@@ -17603,27 +17566,27 @@
       </c>
       <c r="AC7" s="12">
         <f t="shared" si="14"/>
-        <v>-41328.819392987076</v>
+        <v>-27420.181756462011</v>
       </c>
       <c r="AD7" s="12">
         <f t="shared" si="15"/>
-        <v>-40665.675419959902</v>
+        <v>-26757.037783434833</v>
       </c>
       <c r="AE7" s="12">
         <f t="shared" si="16"/>
-        <v>-24005.114479636653</v>
+        <v>-10096.476843111588</v>
       </c>
       <c r="AF7" s="12">
         <f t="shared" si="17"/>
-        <v>-41701.372186822569</v>
+        <v>-27792.734550297504</v>
       </c>
       <c r="AG7" s="12">
         <f t="shared" si="18"/>
-        <v>-41112.738772562487</v>
+        <v>-27204.101136037425</v>
       </c>
       <c r="AH7" s="12">
         <f t="shared" si="19"/>
-        <v>-26121.214348622252</v>
+        <v>-12212.576712097187</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.3">
@@ -17683,31 +17646,31 @@
       </c>
       <c r="U8" s="7">
         <f>OPEX!$B$15</f>
-        <v>72488.476920599642</v>
+        <v>50088.476920599649</v>
       </c>
       <c r="V8" s="11">
         <f t="shared" si="8"/>
-        <v>-64376.476920599642</v>
+        <v>-41976.476920599649</v>
       </c>
       <c r="W8" s="11">
         <f t="shared" si="9"/>
-        <v>-62576.476920599642</v>
+        <v>-40176.476920599649</v>
       </c>
       <c r="X8" s="11">
         <f t="shared" si="1"/>
-        <v>-8756.4769205996417</v>
+        <v>13643.523079400351</v>
       </c>
       <c r="Y8" s="11">
         <f t="shared" si="10"/>
-        <v>-65228.476920599642</v>
+        <v>-42828.476920599649</v>
       </c>
       <c r="Z8" s="11">
         <f t="shared" si="11"/>
-        <v>-63572.476920599642</v>
+        <v>-41172.476920599649</v>
       </c>
       <c r="AA8" s="11">
         <f t="shared" si="12"/>
-        <v>-15152.476920599642</v>
+        <v>7247.523079400351</v>
       </c>
       <c r="AB8" s="11">
         <f t="shared" si="13"/>
@@ -17715,27 +17678,27 @@
       </c>
       <c r="AC8" s="12">
         <f t="shared" si="14"/>
-        <v>-36338.842930387167</v>
+        <v>-23694.626897182559</v>
       </c>
       <c r="AD8" s="12">
         <f t="shared" si="15"/>
-        <v>-35322.789856290365</v>
+        <v>-22678.573823085761</v>
       </c>
       <c r="AE8" s="12">
         <f t="shared" si="16"/>
-        <v>-4942.8029407960767</v>
+        <v>7701.4130924085284</v>
       </c>
       <c r="AF8" s="12">
         <f t="shared" si="17"/>
-        <v>-36819.774718792985</v>
+        <v>-24175.558685588378</v>
       </c>
       <c r="AG8" s="12">
         <f t="shared" si="18"/>
-        <v>-35885.005890623928</v>
+        <v>-23240.789857419324</v>
       </c>
       <c r="AH8" s="12">
         <f t="shared" si="19"/>
-        <v>-8553.1781974200367</v>
+        <v>4091.0378357845698</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.3">
@@ -17794,31 +17757,31 @@
       </c>
       <c r="U9" s="7">
         <f>OPEX!$B$15</f>
-        <v>72488.476920599642</v>
+        <v>50088.476920599649</v>
       </c>
       <c r="V9" s="11">
         <f t="shared" si="8"/>
-        <v>-61400.476920599642</v>
+        <v>-39000.476920599649</v>
       </c>
       <c r="W9" s="11">
         <f t="shared" si="9"/>
-        <v>-58472.476920599642</v>
+        <v>-36072.476920599649</v>
       </c>
       <c r="X9" s="11">
         <f t="shared" si="1"/>
-        <v>42051.523079400358</v>
+        <v>64451.523079400351</v>
       </c>
       <c r="Y9" s="11">
         <f t="shared" si="10"/>
-        <v>-62528.476920599642</v>
+        <v>-40128.476920599649</v>
       </c>
       <c r="Z9" s="11">
         <f t="shared" si="11"/>
-        <v>-59912.476920599642</v>
+        <v>-37512.476920599649</v>
       </c>
       <c r="AA9" s="11">
         <f t="shared" si="12"/>
-        <v>30579.523079400358</v>
+        <v>52979.523079400351</v>
       </c>
       <c r="AB9" s="11">
         <f t="shared" si="13"/>
@@ -17826,27 +17789,27 @@
       </c>
       <c r="AC9" s="12">
         <f t="shared" si="14"/>
-        <v>-31508.153195042833</v>
+        <v>-20013.411346675013</v>
       </c>
       <c r="AD9" s="12">
         <f t="shared" si="15"/>
-        <v>-30005.626224863325</v>
+        <v>-18510.884376495505</v>
       </c>
       <c r="AE9" s="12">
         <f t="shared" si="16"/>
-        <v>21579.080452160211</v>
+        <v>33073.822300528031</v>
       </c>
       <c r="AF9" s="12">
         <f t="shared" si="17"/>
-        <v>-32086.995552407072</v>
+        <v>-20592.253704039249</v>
       </c>
       <c r="AG9" s="12">
         <f t="shared" si="18"/>
-        <v>-30744.573915115543</v>
+        <v>-19249.83206674772</v>
       </c>
       <c r="AH9" s="12">
         <f t="shared" si="19"/>
-        <v>15692.130519817545</v>
+        <v>27186.872368185366</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.3">
@@ -17905,31 +17868,31 @@
       </c>
       <c r="U10" s="7">
         <f>OPEX!$B$15</f>
-        <v>72488.476920599642</v>
+        <v>50088.476920599649</v>
       </c>
       <c r="V10" s="11">
         <f t="shared" si="8"/>
-        <v>-57344.476920599642</v>
+        <v>-34944.476920599649</v>
       </c>
       <c r="W10" s="11">
         <f t="shared" si="9"/>
-        <v>-52712.476920599642</v>
+        <v>-30312.476920599649</v>
       </c>
       <c r="X10" s="11">
         <f t="shared" si="1"/>
-        <v>115743.52307940036</v>
+        <v>138143.52307940036</v>
       </c>
       <c r="Y10" s="11">
         <f t="shared" si="10"/>
-        <v>-58880.476920599642</v>
+        <v>-36480.476920599649</v>
       </c>
       <c r="Z10" s="11">
         <f t="shared" si="11"/>
-        <v>-54728.476920599642</v>
+        <v>-32328.476920599649</v>
       </c>
       <c r="AA10" s="11">
         <f t="shared" si="12"/>
-        <v>96891.523079400358</v>
+        <v>119291.52307940036</v>
       </c>
       <c r="AB10" s="11">
         <f t="shared" si="13"/>
@@ -17937,27 +17900,27 @@
       </c>
       <c r="AC10" s="12">
         <f t="shared" si="14"/>
-        <v>-26751.621697726445</v>
+        <v>-16301.856381028425</v>
       </c>
       <c r="AD10" s="12">
         <f t="shared" si="15"/>
-        <v>-24590.759512594959</v>
+        <v>-14140.994195896941</v>
       </c>
       <c r="AE10" s="12">
         <f t="shared" si="16"/>
-        <v>53995.207728015848</v>
+        <v>64444.973044713872</v>
       </c>
       <c r="AF10" s="12">
         <f t="shared" si="17"/>
-        <v>-27468.177033728596</v>
+        <v>-17018.411717030576</v>
       </c>
       <c r="AG10" s="12">
         <f t="shared" si="18"/>
-        <v>-25531.238391097784</v>
+        <v>-15081.473074399764</v>
       </c>
       <c r="AH10" s="12">
         <f t="shared" si="19"/>
-        <v>45200.610596301958</v>
+        <v>55650.375912999982</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.3">
@@ -18016,31 +17979,31 @@
       </c>
       <c r="U11" s="7">
         <f>OPEX!$B$15</f>
-        <v>72488.476920599642</v>
+        <v>50088.476920599649</v>
       </c>
       <c r="V11" s="11">
         <f t="shared" si="8"/>
-        <v>-51872.476920599642</v>
+        <v>-29472.476920599649</v>
       </c>
       <c r="W11" s="11">
         <f t="shared" si="9"/>
-        <v>-44744.476920599642</v>
+        <v>-22344.476920599649</v>
       </c>
       <c r="X11" s="11">
         <f t="shared" si="1"/>
-        <v>194487.52307940036</v>
+        <v>216887.52307940036</v>
       </c>
       <c r="Y11" s="11">
         <f t="shared" si="10"/>
-        <v>-53960.476920599642</v>
+        <v>-31560.476920599649</v>
       </c>
       <c r="Z11" s="11">
         <f t="shared" si="11"/>
-        <v>-47552.476920599642</v>
+        <v>-25152.476920599649</v>
       </c>
       <c r="AA11" s="11">
         <f t="shared" si="12"/>
-        <v>167775.52307940036</v>
+        <v>190175.52307940036</v>
       </c>
       <c r="AB11" s="11">
         <f t="shared" si="13"/>
@@ -18048,27 +18011,27 @@
       </c>
       <c r="AC11" s="12">
         <f t="shared" si="14"/>
-        <v>-21998.993921107984</v>
+        <v>-12499.207269564333</v>
       </c>
       <c r="AD11" s="12">
         <f t="shared" si="15"/>
-        <v>-18976.026097348913</v>
+        <v>-9476.2394458052604</v>
       </c>
       <c r="AE11" s="12">
         <f t="shared" si="16"/>
-        <v>82481.69534113734</v>
+        <v>91981.481992680987</v>
       </c>
       <c r="AF11" s="12">
         <f t="shared" si="17"/>
-        <v>-22884.509748269735</v>
+        <v>-13384.72309672608</v>
       </c>
       <c r="AG11" s="12">
         <f t="shared" si="18"/>
-        <v>-20166.892209738853</v>
+        <v>-10667.105558195199</v>
       </c>
       <c r="AH11" s="12">
         <f t="shared" si="19"/>
-        <v>71153.199759171519</v>
+        <v>80652.986410715181</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.3">
@@ -18128,31 +18091,31 @@
       </c>
       <c r="U12" s="7">
         <f>OPEX!$B$15</f>
-        <v>72488.476920599642</v>
+        <v>50088.476920599649</v>
       </c>
       <c r="V12" s="11">
         <f t="shared" si="8"/>
-        <v>-44528.476920599642</v>
+        <v>-22128.476920599649</v>
       </c>
       <c r="W12" s="11">
         <f t="shared" si="9"/>
-        <v>-33908.476920599642</v>
+        <v>-11508.476920599649</v>
       </c>
       <c r="X12" s="11">
         <f t="shared" si="1"/>
-        <v>241767.52307940036</v>
+        <v>264167.52307940036</v>
       </c>
       <c r="Y12" s="11">
         <f t="shared" si="10"/>
-        <v>-47360.476920599642</v>
+        <v>-24960.476920599649</v>
       </c>
       <c r="Z12" s="11">
         <f t="shared" si="11"/>
-        <v>-37784.476920599642</v>
+        <v>-15384.476920599649</v>
       </c>
       <c r="AA12" s="11">
         <f t="shared" si="12"/>
-        <v>210327.52307940036</v>
+        <v>232727.52307940036</v>
       </c>
       <c r="AB12" s="11">
         <f t="shared" si="13"/>
@@ -18160,27 +18123,27 @@
       </c>
       <c r="AC12" s="12">
         <f t="shared" si="14"/>
-        <v>-17167.65546525496</v>
+        <v>-8531.4857820334582</v>
       </c>
       <c r="AD12" s="12">
         <f t="shared" si="15"/>
-        <v>-13073.185731513337</v>
+        <v>-4437.0160482918336</v>
       </c>
       <c r="AE12" s="12">
         <f t="shared" si="16"/>
-        <v>93211.846125262178</v>
+        <v>101848.01580848369</v>
       </c>
       <c r="AF12" s="12">
         <f t="shared" si="17"/>
-        <v>-18259.514060919395</v>
+        <v>-9623.3443776978911</v>
       </c>
       <c r="AG12" s="12">
         <f t="shared" si="18"/>
-        <v>-14567.5515213422</v>
+        <v>-5931.3818381206975</v>
       </c>
       <c r="AH12" s="12">
         <f t="shared" si="19"/>
-        <v>81090.36510559771</v>
+        <v>89726.534788819219</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.3">
@@ -18239,31 +18202,31 @@
       </c>
       <c r="U13" s="7">
         <f>OPEX!$B$15</f>
-        <v>72488.476920599642</v>
+        <v>50088.476920599649</v>
       </c>
       <c r="V13" s="11">
         <f t="shared" si="8"/>
-        <v>-34880.476920599642</v>
+        <v>-12480.476920599649</v>
       </c>
       <c r="W13" s="11">
         <f t="shared" si="9"/>
-        <v>-19316.476920599642</v>
+        <v>3083.523079400351</v>
       </c>
       <c r="X13" s="11">
         <f t="shared" si="1"/>
-        <v>251907.52307940036</v>
+        <v>274307.52307940036</v>
       </c>
       <c r="Y13" s="11">
         <f t="shared" si="10"/>
-        <v>-38672.476920599642</v>
+        <v>-16272.476920599649</v>
       </c>
       <c r="Z13" s="11">
         <f t="shared" si="11"/>
-        <v>-24668.476920599642</v>
+        <v>-2268.476920599649</v>
       </c>
       <c r="AA13" s="11">
         <f t="shared" si="12"/>
-        <v>219459.52307940036</v>
+        <v>241859.52307940036</v>
       </c>
       <c r="AB13" s="11">
         <f t="shared" si="13"/>
@@ -18271,27 +18234,27 @@
       </c>
       <c r="AC13" s="12">
         <f t="shared" si="14"/>
-        <v>-12225.394371671671</v>
+        <v>-4374.3310232884887</v>
       </c>
       <c r="AD13" s="12">
         <f t="shared" si="15"/>
-        <v>-6770.3073201432835</v>
+        <v>1080.7560282398995</v>
       </c>
       <c r="AE13" s="12">
         <f t="shared" si="16"/>
-        <v>88292.050072797836</v>
+        <v>96143.113421181028</v>
       </c>
       <c r="AF13" s="12">
         <f t="shared" si="17"/>
-        <v>-13554.467238505111</v>
+        <v>-5703.4038901219283</v>
       </c>
       <c r="AG13" s="12">
         <f t="shared" si="18"/>
-        <v>-8646.1506701676935</v>
+        <v>-795.08732178451146</v>
       </c>
       <c r="AH13" s="12">
         <f t="shared" si="19"/>
-        <v>76919.224022425624</v>
+        <v>84770.287370808801</v>
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.3">
@@ -18350,31 +18313,31 @@
       </c>
       <c r="U14" s="7">
         <f>OPEX!$B$15</f>
-        <v>72488.476920599642</v>
+        <v>50088.476920599649</v>
       </c>
       <c r="V14" s="11">
         <f t="shared" si="8"/>
-        <v>-22256.476920599642</v>
+        <v>143.52307940035098</v>
       </c>
       <c r="W14" s="11">
         <f t="shared" si="9"/>
-        <v>-272.47692059964174</v>
+        <v>22127.523079400351</v>
       </c>
       <c r="X14" s="11">
         <f t="shared" si="1"/>
-        <v>252363.52307940036</v>
+        <v>274763.52307940036</v>
       </c>
       <c r="Y14" s="11">
         <f t="shared" si="10"/>
-        <v>-27296.476920599642</v>
+        <v>-4896.476920599649</v>
       </c>
       <c r="Z14" s="11">
         <f t="shared" si="11"/>
-        <v>-7508.4769205996417</v>
+        <v>14891.523079400351</v>
       </c>
       <c r="AA14" s="11">
         <f t="shared" si="12"/>
-        <v>219843.52307940036</v>
+        <v>242243.52307940036</v>
       </c>
       <c r="AB14" s="11">
         <f t="shared" si="13"/>
@@ -18382,27 +18345,27 @@
       </c>
       <c r="AC14" s="12">
         <f t="shared" si="14"/>
-        <v>-7091.5994405623424</v>
+        <v>45.730876149642263</v>
       </c>
       <c r="AD14" s="12">
         <f t="shared" si="15"/>
-        <v>-86.819544017863748</v>
+        <v>7050.5107726941205</v>
       </c>
       <c r="AE14" s="12">
         <f t="shared" si="16"/>
-        <v>80410.795719055779</v>
+        <v>87548.126035767767</v>
       </c>
       <c r="AF14" s="12">
         <f t="shared" si="17"/>
-        <v>-8697.4987618225387</v>
+        <v>-1560.1684451105548</v>
       </c>
       <c r="AG14" s="12">
         <f t="shared" si="18"/>
-        <v>-2392.4321409700037</v>
+        <v>4744.8981757419806</v>
       </c>
       <c r="AH14" s="12">
         <f t="shared" si="19"/>
-        <v>70048.921527114988</v>
+        <v>77186.251843826962</v>
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.3">
@@ -18461,31 +18424,31 @@
       </c>
       <c r="U15" s="7">
         <f>OPEX!$B$15</f>
-        <v>72488.476920599642</v>
+        <v>50088.476920599649</v>
       </c>
       <c r="V15" s="11">
         <f t="shared" si="8"/>
-        <v>-6176.4769205996417</v>
+        <v>16223.523079400351</v>
       </c>
       <c r="W15" s="11">
         <f t="shared" si="9"/>
-        <v>23847.523079400358</v>
+        <v>46247.523079400351</v>
       </c>
       <c r="X15" s="11">
         <f t="shared" si="1"/>
-        <v>252447.52307940036</v>
+        <v>274847.52307940036</v>
       </c>
       <c r="Y15" s="11">
         <f t="shared" si="10"/>
-        <v>-12812.476920599642</v>
+        <v>9587.523079400351</v>
       </c>
       <c r="Z15" s="11">
         <f t="shared" si="11"/>
-        <v>14187.523079400358</v>
+        <v>36587.523079400351</v>
       </c>
       <c r="AA15" s="11">
         <f t="shared" si="12"/>
-        <v>219927.52307940036</v>
+        <v>242327.52307940036</v>
       </c>
       <c r="AB15" s="11">
         <f t="shared" si="13"/>
@@ -18493,27 +18456,27 @@
       </c>
       <c r="AC15" s="12">
         <f t="shared" si="14"/>
-        <v>-1789.1053561634626</v>
+        <v>4699.3767499383421</v>
       </c>
       <c r="AD15" s="12">
         <f t="shared" si="15"/>
-        <v>6907.7779810508518</v>
+        <v>13396.260087152656</v>
       </c>
       <c r="AE15" s="12">
         <f t="shared" si="16"/>
-        <v>73125.055188857688</v>
+        <v>79613.537294959489</v>
       </c>
       <c r="AF15" s="12">
         <f t="shared" si="17"/>
-        <v>-3711.3181800961229</v>
+        <v>2777.1639260056818</v>
       </c>
       <c r="AG15" s="12">
         <f t="shared" si="18"/>
-        <v>4109.6200727944479</v>
+        <v>10598.102178896252</v>
       </c>
       <c r="AH15" s="12">
         <f t="shared" si="19"/>
-        <v>63705.169559820592</v>
+        <v>70193.6516659224</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.3">
@@ -18572,31 +18535,31 @@
       </c>
       <c r="U16" s="7">
         <f>OPEX!$B$15</f>
-        <v>72488.476920599642</v>
+        <v>50088.476920599649</v>
       </c>
       <c r="V16" s="11">
         <f t="shared" si="8"/>
-        <v>13815.523079400358</v>
+        <v>36215.523079400351</v>
       </c>
       <c r="W16" s="11">
         <f t="shared" si="9"/>
-        <v>52875.523079400358</v>
+        <v>75275.523079400358</v>
       </c>
       <c r="X16" s="11">
         <f t="shared" si="1"/>
-        <v>252483.52307940036</v>
+        <v>274883.52307940036</v>
       </c>
       <c r="Y16" s="11">
         <f t="shared" si="10"/>
-        <v>5151.5230794003583</v>
+        <v>27551.523079400351</v>
       </c>
       <c r="Z16" s="11">
         <f t="shared" si="11"/>
-        <v>40299.523079400358</v>
+        <v>62699.523079400351</v>
       </c>
       <c r="AA16" s="11">
         <f t="shared" si="12"/>
-        <v>219951.52307940036</v>
+        <v>242351.52307940036</v>
       </c>
       <c r="AB16" s="11">
         <f t="shared" si="13"/>
@@ -18604,27 +18567,27 @@
       </c>
       <c r="AC16" s="12">
         <f t="shared" si="14"/>
-        <v>3638.0590213930896</v>
+        <v>9536.6791178492731</v>
       </c>
       <c r="AD16" s="12">
         <f t="shared" si="15"/>
-        <v>13923.777814588564</v>
+        <v>19822.397911044751</v>
       </c>
       <c r="AE16" s="12">
         <f t="shared" si="16"/>
-        <v>66486.80282411653</v>
+        <v>72385.422920572717</v>
       </c>
       <c r="AF16" s="12">
         <f t="shared" si="17"/>
-        <v>1356.5570340852148</v>
+        <v>7255.1771305413986</v>
       </c>
       <c r="AG16" s="12">
         <f t="shared" si="18"/>
-        <v>10612.123960435305</v>
+        <v>16510.74405689149</v>
       </c>
       <c r="AH16" s="12">
         <f t="shared" si="19"/>
-        <v>57920.110459031144</v>
+        <v>63818.730555487324</v>
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.3">
@@ -18683,31 +18646,31 @@
       </c>
       <c r="U17" s="7">
         <f>OPEX!$B$15</f>
-        <v>72488.476920599642</v>
+        <v>50088.476920599649</v>
       </c>
       <c r="V17" s="11">
         <f t="shared" si="8"/>
-        <v>37851.523079400358</v>
+        <v>60251.523079400351</v>
       </c>
       <c r="W17" s="11">
         <f t="shared" si="9"/>
-        <v>85899.523079400358</v>
+        <v>108299.52307940036</v>
       </c>
       <c r="X17" s="11">
         <f t="shared" si="1"/>
-        <v>252507.52307940036</v>
+        <v>274907.52307940036</v>
       </c>
       <c r="Y17" s="11">
         <f t="shared" si="10"/>
-        <v>26787.523079400358</v>
+        <v>49187.523079400351</v>
       </c>
       <c r="Z17" s="11">
         <f t="shared" si="11"/>
-        <v>70059.523079400358</v>
+        <v>92459.523079400358</v>
       </c>
       <c r="AA17" s="11">
         <f t="shared" si="12"/>
-        <v>219975.52307940036</v>
+        <v>242375.52307940036</v>
       </c>
       <c r="AB17" s="11">
         <f t="shared" si="13"/>
@@ -18715,27 +18678,27 @@
       </c>
       <c r="AC17" s="12">
         <f t="shared" si="14"/>
-        <v>9061.3536817218373</v>
+        <v>14423.735587591096</v>
       </c>
       <c r="AD17" s="12">
         <f t="shared" si="15"/>
-        <v>20563.6628698114</v>
+        <v>25926.044775680661</v>
       </c>
       <c r="AE17" s="12">
         <f t="shared" si="16"/>
-        <v>60448.293431108978</v>
+        <v>65810.675336978238</v>
       </c>
       <c r="AF17" s="12">
         <f t="shared" si="17"/>
-        <v>6412.7200475014142</v>
+        <v>11775.101953370673</v>
       </c>
       <c r="AG17" s="12">
         <f t="shared" si="18"/>
-        <v>16771.692807803851</v>
+        <v>22134.074713673112</v>
       </c>
       <c r="AH17" s="12">
         <f t="shared" si="19"/>
-        <v>52660.391281031349</v>
+        <v>58022.773186900609</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.3">
@@ -18794,31 +18757,31 @@
       </c>
       <c r="U18" s="7">
         <f>OPEX!$B$15</f>
-        <v>72488.476920599642</v>
+        <v>50088.476920599649</v>
       </c>
       <c r="V18" s="11">
         <f t="shared" si="8"/>
-        <v>65499.523079400358</v>
+        <v>87899.523079400358</v>
       </c>
       <c r="W18" s="11">
         <f t="shared" si="9"/>
-        <v>120759.52307940036</v>
+        <v>143159.52307940036</v>
       </c>
       <c r="X18" s="11">
         <f t="shared" si="1"/>
-        <v>252519.52307940036</v>
+        <v>274919.52307940036</v>
       </c>
       <c r="Y18" s="11">
         <f t="shared" si="10"/>
-        <v>51675.523079400358</v>
+        <v>74075.523079400358</v>
       </c>
       <c r="Z18" s="11">
         <f t="shared" si="11"/>
-        <v>101427.52307940036</v>
+        <v>123827.52307940036</v>
       </c>
       <c r="AA18" s="11">
         <f t="shared" si="12"/>
-        <v>219987.52307940036</v>
+        <v>242387.52307940036</v>
       </c>
       <c r="AB18" s="11">
         <f t="shared" si="13"/>
@@ -18826,27 +18789,27 @@
       </c>
       <c r="AC18" s="12">
         <f t="shared" si="14"/>
-        <v>14254.604602436788</v>
+        <v>19129.497244136117</v>
       </c>
       <c r="AD18" s="12">
         <f t="shared" si="15"/>
-        <v>26280.790646200396</v>
+        <v>31155.683287899723</v>
       </c>
       <c r="AE18" s="12">
         <f t="shared" si="16"/>
-        <v>54955.60557791037</v>
+        <v>59830.498219609697</v>
       </c>
       <c r="AF18" s="12">
         <f t="shared" si="17"/>
-        <v>11246.099429273774</v>
+        <v>16120.992070973101</v>
       </c>
       <c r="AG18" s="12">
         <f t="shared" si="18"/>
-        <v>22073.584193105246</v>
+        <v>26948.476834804573</v>
       </c>
       <c r="AH18" s="12">
         <f t="shared" si="19"/>
-        <v>47875.694532385256</v>
+        <v>52750.587174084583</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.3">
@@ -18896,31 +18859,31 @@
       </c>
       <c r="U19" s="7">
         <f>OPEX!$B$15</f>
-        <v>72488.476920599642</v>
+        <v>50088.476920599649</v>
       </c>
       <c r="V19" s="11">
         <f t="shared" si="8"/>
-        <v>95583.523079400358</v>
+        <v>117983.52307940036</v>
       </c>
       <c r="W19" s="11">
         <f t="shared" si="9"/>
-        <v>154359.52307940036</v>
+        <v>176759.52307940036</v>
       </c>
       <c r="X19" s="11">
         <f t="shared" si="1"/>
-        <v>252531.52307940036</v>
+        <v>274931.52307940036</v>
       </c>
       <c r="Y19" s="11">
         <f t="shared" si="10"/>
-        <v>78771.523079400358</v>
+        <v>101171.52307940036</v>
       </c>
       <c r="Z19" s="11">
         <f t="shared" si="11"/>
-        <v>131631.52307940036</v>
+        <v>154031.52307940036</v>
       </c>
       <c r="AA19" s="11">
         <f t="shared" si="12"/>
-        <v>219999.52307940036</v>
+        <v>242399.52307940036</v>
       </c>
       <c r="AB19" s="11">
         <f t="shared" si="13"/>
@@ -18928,27 +18891,27 @@
       </c>
       <c r="AC19" s="12">
         <f t="shared" si="14"/>
-        <v>18910.690475952379</v>
+        <v>23342.411059315404</v>
       </c>
       <c r="AD19" s="12">
         <f t="shared" si="15"/>
-        <v>30539.208735226715</v>
+        <v>34970.92931858974</v>
       </c>
       <c r="AE19" s="12">
         <f t="shared" si="16"/>
-        <v>49962.015570490767</v>
+        <v>54393.736153853795</v>
       </c>
       <c r="AF19" s="12">
         <f t="shared" si="17"/>
-        <v>15584.525902403308</v>
+        <v>20016.246485766333</v>
       </c>
       <c r="AG19" s="12">
         <f t="shared" si="18"/>
-        <v>26042.595100464445</v>
+        <v>30474.31568382747</v>
       </c>
       <c r="AH19" s="12">
         <f t="shared" si="19"/>
-        <v>43525.732801831575</v>
+        <v>47957.453385194603</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.3">
@@ -18998,31 +18961,31 @@
       </c>
       <c r="U20" s="7">
         <f>OPEX!$B$15</f>
-        <v>72488.476920599642</v>
+        <v>50088.476920599649</v>
       </c>
       <c r="V20" s="11">
         <f t="shared" si="8"/>
-        <v>126339.52307940036</v>
+        <v>148739.52307940036</v>
       </c>
       <c r="W20" s="11">
         <f t="shared" si="9"/>
-        <v>183735.52307940036</v>
+        <v>206135.52307940036</v>
       </c>
       <c r="X20" s="11">
         <f t="shared" si="1"/>
-        <v>252531.52307940036</v>
+        <v>274931.52307940036</v>
       </c>
       <c r="Y20" s="11">
         <f t="shared" si="10"/>
-        <v>106443.52307940036</v>
+        <v>128843.52307940036</v>
       </c>
       <c r="Z20" s="11">
         <f t="shared" si="11"/>
-        <v>158079.52307940036</v>
+        <v>180479.52307940036</v>
       </c>
       <c r="AA20" s="11">
         <f t="shared" si="12"/>
-        <v>219999.52307940036</v>
+        <v>242399.52307940036</v>
       </c>
       <c r="AB20" s="11">
         <f t="shared" si="13"/>
@@ -19030,27 +18993,27 @@
       </c>
       <c r="AC20" s="12">
         <f t="shared" si="14"/>
-        <v>22723.273738768115</v>
+        <v>26752.110632734504</v>
       </c>
       <c r="AD20" s="12">
         <f t="shared" si="15"/>
-        <v>33046.448844397346</v>
+        <v>37075.285738363731</v>
       </c>
       <c r="AE20" s="12">
         <f t="shared" si="16"/>
-        <v>45420.014154991608</v>
+        <v>49448.851048957993</v>
       </c>
       <c r="AF20" s="12">
         <f t="shared" si="17"/>
-        <v>19144.803254734401</v>
+        <v>23173.640148700786</v>
       </c>
       <c r="AG20" s="12">
         <f t="shared" si="18"/>
-        <v>28431.991730486559</v>
+        <v>32460.828624452944</v>
       </c>
       <c r="AH20" s="12">
         <f t="shared" si="19"/>
-        <v>39568.848001665065</v>
+        <v>43597.68489563145</v>
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.3">
@@ -19100,31 +19063,31 @@
       </c>
       <c r="U21" s="7">
         <f>OPEX!$B$15</f>
-        <v>72488.476920599642</v>
+        <v>50088.476920599649</v>
       </c>
       <c r="V21" s="11">
         <f t="shared" si="8"/>
-        <v>155595.52307940036</v>
+        <v>177995.52307940036</v>
       </c>
       <c r="W21" s="11">
         <f t="shared" si="9"/>
-        <v>206991.52307940036</v>
+        <v>229391.52307940036</v>
       </c>
       <c r="X21" s="11">
         <f t="shared" si="1"/>
-        <v>252531.52307940036</v>
+        <v>274931.52307940036</v>
       </c>
       <c r="Y21" s="11">
         <f t="shared" si="10"/>
-        <v>132771.52307940036</v>
+        <v>155171.52307940036</v>
       </c>
       <c r="Z21" s="11">
         <f t="shared" si="11"/>
-        <v>179043.52307940036</v>
+        <v>201443.52307940036</v>
       </c>
       <c r="AA21" s="11">
         <f t="shared" si="12"/>
-        <v>219999.52307940036</v>
+        <v>242399.52307940036</v>
       </c>
       <c r="AB21" s="11">
         <f t="shared" si="13"/>
@@ -19132,27 +19095,27 @@
       </c>
       <c r="AC21" s="12">
         <f t="shared" si="14"/>
-        <v>25441.111360320057</v>
+        <v>29103.690354834955</v>
       </c>
       <c r="AD21" s="12">
         <f t="shared" si="15"/>
-        <v>33844.768056841822</v>
+        <v>37507.347051356715</v>
       </c>
       <c r="AE21" s="12">
         <f t="shared" si="16"/>
-        <v>41290.921959083265</v>
+        <v>44953.500953598159</v>
       </c>
       <c r="AF21" s="12">
         <f t="shared" si="17"/>
-        <v>21709.204977694702</v>
+        <v>25371.7839722096</v>
       </c>
       <c r="AG21" s="12">
         <f t="shared" si="18"/>
-        <v>29275.046729221187</v>
+        <v>32937.625723736084</v>
       </c>
       <c r="AH21" s="12">
         <f t="shared" si="19"/>
-        <v>35971.680001513691</v>
+        <v>39634.258996028584</v>
       </c>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.3">
@@ -19202,31 +19165,31 @@
       </c>
       <c r="U22" s="7">
         <f>OPEX!$B$15</f>
-        <v>72488.476920599642</v>
+        <v>50088.476920599649</v>
       </c>
       <c r="V22" s="11">
         <f t="shared" si="8"/>
-        <v>181383.52307940036</v>
+        <v>203783.52307940036</v>
       </c>
       <c r="W22" s="11">
         <f t="shared" si="9"/>
-        <v>223791.52307940036</v>
+        <v>246191.52307940036</v>
       </c>
       <c r="X22" s="11">
         <f t="shared" si="1"/>
-        <v>252531.52307940036</v>
+        <v>274931.52307940036</v>
       </c>
       <c r="Y22" s="11">
         <f t="shared" si="10"/>
-        <v>155991.52307940036</v>
+        <v>178391.52307940036</v>
       </c>
       <c r="Z22" s="11">
         <f t="shared" si="11"/>
-        <v>194139.52307940036</v>
+        <v>216539.52307940036</v>
       </c>
       <c r="AA22" s="11">
         <f t="shared" si="12"/>
-        <v>219999.52307940036</v>
+        <v>242399.52307940036</v>
       </c>
       <c r="AB22" s="11">
         <f t="shared" si="13"/>
@@ -19234,27 +19197,27 @@
       </c>
       <c r="AC22" s="12">
         <f t="shared" si="14"/>
-        <v>26961.504934323035</v>
+        <v>30291.122202063849</v>
       </c>
       <c r="AD22" s="12">
         <f t="shared" si="15"/>
-        <v>33265.183911570908</v>
+        <v>36594.801179311726</v>
       </c>
       <c r="AE22" s="12">
         <f t="shared" si="16"/>
-        <v>37537.201780984797</v>
+        <v>40866.819048725607</v>
       </c>
       <c r="AF22" s="12">
         <f t="shared" si="17"/>
-        <v>23187.145931533982</v>
+        <v>26516.763199274796</v>
       </c>
       <c r="AG22" s="12">
         <f t="shared" si="18"/>
-        <v>28857.603053399009</v>
+        <v>32187.220321139823</v>
       </c>
       <c r="AH22" s="12">
         <f t="shared" si="19"/>
-        <v>32701.527274103359</v>
+        <v>36031.144541844173</v>
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.3">
@@ -20589,9 +20552,9 @@
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="19" max="19" width="14.88671875" customWidth="1"/>
+    <col min="19" max="19" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
@@ -22041,7 +22004,7 @@
       <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -23490,7 +23453,7 @@
       <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -24939,7 +24902,7 @@
       <selection sqref="A1:U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -26388,7 +26351,7 @@
       <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -27837,7 +27800,7 @@
       <selection sqref="A1:U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Working new opex final
</commit_message>
<xml_diff>
--- a/tumlknexpectimax/excel_data/input_data_business.xlsx
+++ b/tumlknexpectimax/excel_data/input_data_business.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="825" windowWidth="13680" windowHeight="11070" tabRatio="847" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="825" windowWidth="13680" windowHeight="11070" tabRatio="847" firstSheet="11" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="CAPEX" sheetId="1" r:id="rId1"/>
@@ -769,7 +769,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -796,6 +796,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1279,11 +1280,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="152826880"/>
-        <c:axId val="152840448"/>
+        <c:axId val="83742720"/>
+        <c:axId val="83744640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="152826880"/>
+        <c:axId val="83742720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1305,13 +1306,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152840448"/>
+        <c:crossAx val="83744640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1319,7 +1321,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152840448"/>
+        <c:axId val="83744640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1342,19 +1344,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152826880"/>
+        <c:crossAx val="83742720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1372,7 +1376,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1481,7 +1485,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>36062.342937580564</c:v>
+                  <c:v>20000</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>19283.042118970367</c:v>
@@ -1540,11 +1544,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153448960"/>
-        <c:axId val="152842752"/>
+        <c:axId val="96283648"/>
+        <c:axId val="96301824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153448960"/>
+        <c:axId val="96283648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1554,7 +1558,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152842752"/>
+        <c:crossAx val="96301824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1562,7 +1566,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152842752"/>
+        <c:axId val="96301824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1592,7 +1596,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153448960"/>
+        <c:crossAx val="96283648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1612,7 +1616,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1921,11 +1925,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153451520"/>
-        <c:axId val="152844480"/>
+        <c:axId val="96438912"/>
+        <c:axId val="96440704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153451520"/>
+        <c:axId val="96438912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1942,10 +1946,10 @@
             <a:pPr>
               <a:defRPr sz="1200"/>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152844480"/>
+        <c:crossAx val="96440704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1953,7 +1957,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152844480"/>
+        <c:axId val="96440704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1976,6 +1980,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1989,10 +1994,10 @@
             <a:pPr>
               <a:defRPr sz="1200"/>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153451520"/>
+        <c:crossAx val="96438912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2008,7 +2013,7 @@
             <a:pPr>
               <a:defRPr sz="1400"/>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
       </c:legendEntry>
@@ -2021,7 +2026,7 @@
             <a:pPr>
               <a:defRPr sz="1400"/>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
       </c:legendEntry>
@@ -2052,7 +2057,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2574,11 +2579,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="164004864"/>
-        <c:axId val="163693120"/>
+        <c:axId val="97123328"/>
+        <c:axId val="84607744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="164004864"/>
+        <c:axId val="97123328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2588,7 +2593,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163693120"/>
+        <c:crossAx val="84607744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2596,7 +2601,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="163693120"/>
+        <c:axId val="84607744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2607,7 +2612,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164004864"/>
+        <c:crossAx val="97123328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2648,7 +2653,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2689,7 +2694,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2730,7 +2735,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2771,7 +2776,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0800-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3081,8 +3086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y46"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+    <sheetView topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3105,7 +3110,7 @@
     <col min="24" max="24" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="9" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -3179,7 +3184,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
@@ -3215,13 +3220,13 @@
       <c r="U2" s="13"/>
       <c r="V2" s="13"/>
       <c r="W2" s="13">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="X2" s="13">
         <v>100000</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>73</v>
       </c>
@@ -3300,7 +3305,7 @@
         <v>307967.22911888885</v>
       </c>
     </row>
-    <row r="4" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>66</v>
       </c>
@@ -3378,7 +3383,7 @@
         <v>216506.84792333335</v>
       </c>
     </row>
-    <row r="5" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>67</v>
       </c>
@@ -3452,7 +3457,7 @@
         <v>145045.86878666666</v>
       </c>
     </row>
-    <row r="6" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>68</v>
       </c>
@@ -3530,7 +3535,7 @@
         <v>218092.13545333332</v>
       </c>
     </row>
-    <row r="7" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>69</v>
       </c>
@@ -3608,7 +3613,7 @@
         <v>288249.58125666669</v>
       </c>
     </row>
-    <row r="8" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>70</v>
       </c>
@@ -3684,7 +3689,7 @@
         <v>347869.80689666665</v>
       </c>
     </row>
-    <row r="9" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>71</v>
       </c>
@@ -3760,7 +3765,7 @@
         <v>221159.28125666664</v>
       </c>
     </row>
-    <row r="10" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>72</v>
       </c>
@@ -3835,7 +3840,7 @@
         <v>147813.53545333334</v>
       </c>
     </row>
-    <row r="11" spans="1:24" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>74</v>
       </c>
@@ -3912,7 +3917,7 @@
         <v>215033.99423000001</v>
       </c>
     </row>
-    <row r="12" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>75</v>
       </c>
@@ -3988,7 +3993,7 @@
         <v>178789.21166999999</v>
       </c>
     </row>
-    <row r="13" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>76</v>
       </c>
@@ -4065,7 +4070,7 @@
         <v>298182.08727000002</v>
       </c>
     </row>
-    <row r="14" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>77</v>
       </c>
@@ -4141,7 +4146,7 @@
         <v>235044.99423000001</v>
       </c>
     </row>
-    <row r="15" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>78</v>
       </c>
@@ -4218,7 +4223,7 @@
         <v>196669.21166999999</v>
       </c>
     </row>
-    <row r="27" spans="17:17" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q27">
         <f>0.02/1000</f>
         <v>2.0000000000000002E-5</v>
@@ -4312,7 +4317,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -4377,7 +4382,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -4442,7 +4447,7 @@
         <v>-1373.815837057527</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -4507,7 +4512,7 @@
         <v>-321.65076096138819</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -4572,7 +4577,7 @@
         <v>1353.871209043366</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -4637,7 +4642,7 @@
         <v>4205.9986197914886</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -4702,7 +4707,7 @@
         <v>9052.7861231763327</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -4767,7 +4772,7 @@
         <v>17327.544791986678</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -4832,7 +4837,7 @@
         <v>30945.693748588084</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -4897,7 +4902,7 @@
         <v>51600.195925279462</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -4962,7 +4967,7 @@
         <v>77844.306419449145</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -5027,7 +5032,7 @@
         <v>100829.28687112352</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -5092,7 +5097,7 @@
         <v>108068.62611646316</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -5157,7 +5162,7 @@
         <v>101444.91585048511</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -5222,7 +5227,7 @@
         <v>92345.005007169064</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -5287,7 +5292,7 @@
         <v>83974.336359869762</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -5352,7 +5357,7 @@
         <v>76346.625731803113</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -5417,7 +5422,7 @@
         <v>69411.768801733138</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -5482,7 +5487,7 @@
         <v>63104.21955120506</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -5547,7 +5552,7 @@
         <v>57369.846455304127</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -5612,7 +5617,7 @@
         <v>52154.405868458292</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -5677,7 +5682,7 @@
         <v>47413.096244052984</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -5761,7 +5766,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -5826,7 +5831,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -5891,7 +5896,7 @@
         <v>-1237.5328644674091</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -5956,7 +5961,7 @@
         <v>-197.75714951582648</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -6021,7 +6026,7 @@
         <v>1466.5017649029676</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -6086,7 +6091,7 @@
         <v>4308.3900342093084</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -6151,7 +6156,7 @@
         <v>9145.8692271925338</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -6216,7 +6221,7 @@
         <v>17412.165795637768</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -6281,7 +6286,7 @@
         <v>31022.621933725437</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -6346,7 +6351,7 @@
         <v>51670.13063904069</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -6411,7 +6416,7 @@
         <v>77907.883431959359</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -6476,7 +6481,7 @@
         <v>100887.08415522371</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -6541,7 +6546,7 @@
         <v>108121.16910200879</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -6606,7 +6611,7 @@
         <v>101492.68220098114</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -6671,7 +6676,7 @@
         <v>92388.428962165461</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -6736,7 +6741,7 @@
         <v>84013.812682593751</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -6801,7 +6806,7 @@
         <v>76382.513297915822</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -6866,7 +6871,7 @@
         <v>69444.393861835604</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -6931,7 +6936,7 @@
         <v>63133.878696752763</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -6996,7 +7001,7 @@
         <v>57396.809314892947</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -7061,7 +7066,7 @@
         <v>52178.917558993584</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -7126,7 +7131,7 @@
         <v>47435.379599085063</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -7213,7 +7218,7 @@
     <col min="19" max="19" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -7278,7 +7283,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -7343,7 +7348,7 @@
         <v>-1298.1283124115794</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -7408,7 +7413,7 @@
         <v>-252.84392037416305</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -7473,7 +7478,7 @@
         <v>1416.4228823044798</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -7538,7 +7543,7 @@
         <v>4262.8637773015917</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -7603,7 +7608,7 @@
         <v>9104.4817209127905</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -7668,7 +7673,7 @@
         <v>17374.540789928909</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -7733,7 +7738,7 @@
         <v>30988.417383081021</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -7798,7 +7803,7 @@
         <v>51639.035593000321</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -7863,7 +7868,7 @@
         <v>77879.615208286297</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -7928,7 +7933,7 @@
         <v>100861.38577006638</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -7993,7 +7998,7 @@
         <v>108097.80693368394</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -8058,7 +8063,7 @@
         <v>101471.44386614037</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -8123,7 +8128,7 @@
         <v>92369.121385037477</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -8188,7 +8193,7 @@
         <v>83996.260339750137</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -8253,7 +8258,7 @@
         <v>76366.556622603443</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -8318,7 +8323,7 @@
         <v>69429.88779336981</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -8383,7 +8388,7 @@
         <v>63120.691361783851</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -8448,7 +8453,7 @@
         <v>57384.820828557575</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -8513,7 +8518,7 @@
         <v>52168.018935052336</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -8578,7 +8583,7 @@
         <v>47425.471759138476</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -8662,7 +8667,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -8727,7 +8732,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -8792,7 +8797,7 @@
         <v>-1072.7975413371182</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -8857,7 +8862,7 @@
         <v>-462.5432193973802</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -8922,7 +8927,7 @@
         <v>487.9359162503157</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -8987,7 +8992,7 @@
         <v>2077.2370087624954</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -9052,7 +9057,7 @@
         <v>4770.1676515694826</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -9117,7 +9122,7 @@
         <v>9348.0962295563986</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -9182,7 +9187,7 @@
         <v>16866.482417857962</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -9247,7 +9252,7 @@
         <v>28261.05567537887</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -9312,7 +9317,7 @@
         <v>42734.689615525116</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -9377,7 +9382,7 @@
         <v>55408.863800220242</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -9442,7 +9447,7 @@
         <v>59408.21219880171</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -9507,7 +9512,7 @@
         <v>55769.74896186671</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -9572,7 +9577,7 @@
         <v>50770.125468065649</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -9637,7 +9642,7 @@
         <v>46166.477823116569</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -9702,7 +9707,7 @@
         <v>41973.317263804332</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -9767,7 +9772,7 @@
         <v>38161.008394423945</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -9832,7 +9837,7 @@
         <v>34693.392742890363</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -9897,7 +9902,7 @@
         <v>31540.872429698233</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -9962,7 +9967,7 @@
         <v>28673.520390634752</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -10027,7 +10032,7 @@
         <v>26066.836718758859</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -10111,7 +10116,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -10176,7 +10181,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -10241,7 +10246,7 @@
         <v>-2032.9008073992691</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -10306,7 +10311,7 @@
         <v>-1128.0916430902446</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -10371,7 +10376,7 @@
         <v>251.8175145460585</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -10436,7 +10441,7 @@
         <v>2533.3577705490084</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -10501,7 +10506,7 @@
         <v>6358.5132112565598</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -10566,7 +10571,7 @@
         <v>12835.126259756675</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -10631,7 +10636,7 @@
         <v>23449.093309573149</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -10696,7 +10701,7 @@
         <v>39515.176006102003</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -10761,7 +10766,7 @@
         <v>59911.816386371538</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -10826,7 +10831,7 @@
         <v>77775.728398294057</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -10891,7 +10896,7 @@
         <v>83426.285578198047</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -10956,7 +10961,7 @@
         <v>78323.574606690105</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -11021,7 +11026,7 @@
         <v>71299.603601721174</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -11086,7 +11091,7 @@
         <v>64835.896513405729</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -11151,7 +11156,7 @@
         <v>58946.780063178769</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -11216,7 +11221,7 @@
         <v>53592.578202964956</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -11281,7 +11286,7 @@
         <v>48722.614878762637</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -11346,7 +11351,7 @@
         <v>44295.185562242019</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -11411,7 +11416,7 @@
         <v>40268.350511129102</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -11476,7 +11481,7 @@
         <v>36607.591373753719</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -11560,7 +11565,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -11625,7 +11630,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -11690,7 +11695,7 @@
         <v>-11486.239659399269</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -11755,7 +11760,7 @@
         <v>-9514.7633267266083</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -11820,7 +11825,7 @@
         <v>-7003.5038507431964</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -11885,7 +11890,7 @@
         <v>-3391.6150709235671</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -11950,7 +11955,7 @@
         <v>2145.864586162646</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -12015,7 +12020,7 @@
         <v>11048.525212883327</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -12080,7 +12085,7 @@
         <v>25237.4941312214</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -12145,7 +12150,7 @@
         <v>46410.923545855207</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -12210,7 +12215,7 @@
         <v>73126.786074518022</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -12275,7 +12280,7 @@
         <v>96540.632012095215</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -12340,7 +12345,7 @@
         <v>104169.84897189197</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -12405,7 +12410,7 @@
         <v>97900.572991784036</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -12470,7 +12475,7 @@
         <v>89122.875135622628</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -12535,7 +12540,7 @@
         <v>81045.127385736647</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -12600,7 +12605,7 @@
         <v>73683.708482591188</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -12665,7 +12670,7 @@
         <v>66990.93493881321</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -12730,7 +12735,7 @@
         <v>60903.461494005125</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -12795,7 +12800,7 @@
         <v>55369.157312395095</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -12860,7 +12865,7 @@
         <v>50335.597556722809</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -12925,7 +12930,7 @@
         <v>45759.634142475268</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -13009,7 +13014,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -13074,7 +13079,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -13139,7 +13144,7 @@
         <v>-1481.7435413371186</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -13204,7 +13209,7 @@
         <v>-419.76685576101687</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -13269,7 +13274,7 @@
         <v>1264.6747592255217</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -13334,7 +13339,7 @@
         <v>4124.9109381389026</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -13399,7 +13404,7 @@
         <v>8979.0700489467108</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -13464,7 +13469,7 @@
         <v>17260.530179050653</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -13529,7 +13534,7 @@
         <v>30884.771373191699</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -13594,7 +13599,7 @@
         <v>51544.811947646391</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -13659,7 +13664,7 @@
         <v>77793.957348873635</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -13724,7 +13729,7 @@
         <v>100783.51498878215</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -13789,7 +13794,7 @@
         <v>108027.01531433463</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -13854,7 +13859,7 @@
         <v>101407.08784855009</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -13919,7 +13924,7 @@
         <v>92310.615914500857</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -13984,7 +13989,7 @@
         <v>83943.073548353204</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -14049,7 +14054,7 @@
         <v>76318.204994060783</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -14114,7 +14119,7 @@
         <v>69385.931767421935</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -14179,7 +14184,7 @@
         <v>63080.731338194877</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -14244,7 +14249,7 @@
         <v>57348.49353438578</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -14309,7 +14314,7 @@
         <v>52134.994122168886</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -14374,7 +14379,7 @@
         <v>47395.4492019717</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -14458,7 +14463,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -14523,7 +14528,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -14588,7 +14593,7 @@
         <v>-1927.2108073992695</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -14653,7 +14658,7 @@
         <v>-824.73709763569946</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -14718,7 +14723,7 @@
         <v>896.51999388490117</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -14783,7 +14788,7 @@
         <v>3790.2247878292478</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -14848,7 +14853,7 @@
         <v>8674.8099123015691</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -14913,7 +14918,7 @@
         <v>16983.930054827797</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -14978,7 +14983,7 @@
         <v>30633.316714807286</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -15043,7 +15048,7 @@
         <v>51316.216803660558</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -15108,7 +15113,7 @@
         <v>77586.143581613782</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -15173,7 +15178,7 @@
         <v>100594.59338218228</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -15238,7 +15243,7 @@
         <v>107855.26839924385</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -15303,7 +15308,7 @@
         <v>101250.95428937666</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -15368,7 +15373,7 @@
         <v>92168.676315252291</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -15433,7 +15438,7 @@
         <v>83814.037549036337</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -15498,7 +15503,7 @@
         <v>76200.89954013635</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -15563,7 +15568,7 @@
         <v>69279.29044567245</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -15628,7 +15633,7 @@
         <v>62983.784682058984</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -15693,7 +15698,7 @@
         <v>57260.360210625877</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -15758,7 +15763,7 @@
         <v>52054.872918750792</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -15823,7 +15828,7 @@
         <v>47322.611744318885</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -15901,8 +15906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15924,7 +15929,7 @@
     <col min="15" max="15" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -15971,7 +15976,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -16031,7 +16036,7 @@
         <v>196669.21166999999</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -16042,8 +16047,8 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <f>D2-C2</f>
-        <v>-91460.381195555499</v>
+        <f>IF(D2-C2&gt;0,D2-C2,0)</f>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -16052,8 +16057,8 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <f>G2-C2</f>
-        <v>-19717.647862222162</v>
+        <f>IF(G2-C2&gt;0,G2-C2,0)</f>
+        <v>0</v>
       </c>
       <c r="H3">
         <f>H2-C2</f>
@@ -16061,7 +16066,7 @@
       </c>
       <c r="I3">
         <f>I2-D2+D3</f>
-        <v>-86807.947862222209</v>
+        <v>4652.4333333332906</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -16082,7 +16087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -16131,7 +16136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -16180,7 +16185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -16227,7 +16232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -16274,7 +16279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -16294,15 +16299,15 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <f>G2-H2</f>
-        <v>-59620.225639999961</v>
+        <f>IF(G2-H2&gt;0,G2-H2,0)</f>
+        <v>0</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <f>I2-H2</f>
-        <v>-126710.52564000001</v>
+        <f>IF(I2-H2&gt;0,I2-H2,0)</f>
+        <v>0</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -16323,7 +16328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -16371,7 +16376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -16419,7 +16424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>74</v>
       </c>
@@ -16454,8 +16459,8 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <f>L2-K2</f>
-        <v>-36244.782560000021</v>
+        <f>IF(L2-K2&gt;0,L2-K2,0)</f>
+        <v>0</v>
       </c>
       <c r="M11">
         <f>M2-K2</f>
@@ -16467,10 +16472,10 @@
       </c>
       <c r="O11">
         <f>O2-L2+L11</f>
-        <v>-18364.782560000021</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+        <v>17880</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>75</v>
       </c>
@@ -16519,7 +16524,7 @@
         <v>17880</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>76</v>
       </c>
@@ -16566,7 +16571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -16611,11 +16616,11 @@
         <v>0</v>
       </c>
       <c r="O14">
-        <f>O2-N2</f>
-        <v>-38375.782560000021</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+        <f>IF(O2-N2&gt;0,O2-N2,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>78</v>
       </c>
@@ -16663,7 +16668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
@@ -16692,8 +16697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16703,7 +16708,7 @@
     <col min="3" max="3" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>22</v>
       </c>
@@ -16711,13 +16716,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="12">
-        <f>AVERAGE(B3:B15)</f>
-        <v>36062.342937580564</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -16857,7 +16861,7 @@
     <col min="34" max="34" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -16937,7 +16941,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2018</v>
       </c>
@@ -17040,7 +17044,7 @@
         <v>-48948.476920599649</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2019</v>
       </c>
@@ -17142,7 +17146,7 @@
         <v>-43571.342655090586</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2020</v>
       </c>
@@ -17253,7 +17257,7 @@
         <v>-37964.03051289227</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2021</v>
       </c>
@@ -17365,7 +17369,7 @@
         <v>-31537.54840014999</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2022</v>
       </c>
@@ -17477,7 +17481,7 @@
         <v>-23441.347531315922</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2023</v>
       </c>
@@ -17589,7 +17593,7 @@
         <v>-12212.576712097187</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2024</v>
       </c>
@@ -17701,7 +17705,7 @@
         <v>4091.0378357845698</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2025</v>
       </c>
@@ -17812,7 +17816,7 @@
         <v>27186.872368185366</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2026</v>
       </c>
@@ -17923,7 +17927,7 @@
         <v>55650.375912999982</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2027</v>
       </c>
@@ -18034,7 +18038,7 @@
         <v>80652.986410715181</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2028</v>
       </c>
@@ -18146,7 +18150,7 @@
         <v>89726.534788819219</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2029</v>
       </c>
@@ -18257,7 +18261,7 @@
         <v>84770.287370808801</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2030</v>
       </c>
@@ -18368,7 +18372,7 @@
         <v>77186.251843826962</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2031</v>
       </c>
@@ -18479,7 +18483,7 @@
         <v>70193.6516659224</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2032</v>
       </c>
@@ -18590,7 +18594,7 @@
         <v>63818.730555487324</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2033</v>
       </c>
@@ -18701,7 +18705,7 @@
         <v>58022.773186900609</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2034</v>
       </c>
@@ -18812,7 +18816,7 @@
         <v>52750.587174084583</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2035</v>
       </c>
@@ -18914,7 +18918,7 @@
         <v>47957.453385194603</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2036</v>
       </c>
@@ -19016,7 +19020,7 @@
         <v>43597.68489563145</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>2037</v>
       </c>
@@ -19118,7 +19122,7 @@
         <v>39634.258996028584</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2038</v>
       </c>
@@ -19220,7 +19224,7 @@
         <v>36031.144541844173</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="J25" s="3">
         <v>29262</v>
       </c>
@@ -19231,7 +19235,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -19239,7 +19243,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -19262,7 +19266,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2018</v>
       </c>
@@ -19297,7 +19301,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>2019</v>
       </c>
@@ -19332,7 +19336,7 @@
         <v>2049</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2020</v>
       </c>
@@ -19361,7 +19365,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2021</v>
       </c>
@@ -19390,7 +19394,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2022</v>
       </c>
@@ -19419,7 +19423,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>2023</v>
       </c>
@@ -19448,7 +19452,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>2024</v>
       </c>
@@ -19491,7 +19495,7 @@
       <c r="AC35" s="10"/>
       <c r="AD35" s="10"/>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2025</v>
       </c>
@@ -19520,7 +19524,7 @@
         <v>7008</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>2026</v>
       </c>
@@ -19549,7 +19553,7 @@
         <v>11517</v>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>2027</v>
       </c>
@@ -19578,7 +19582,7 @@
         <v>16335</v>
       </c>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>2028</v>
       </c>
@@ -19607,7 +19611,7 @@
         <v>19227</v>
       </c>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>2029</v>
       </c>
@@ -19636,7 +19640,7 @@
         <v>19847</v>
       </c>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2030</v>
       </c>
@@ -19665,7 +19669,7 @@
         <v>19876</v>
       </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>2031</v>
       </c>
@@ -19694,7 +19698,7 @@
         <v>19880</v>
       </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>2032</v>
       </c>
@@ -19723,7 +19727,7 @@
         <v>19882</v>
       </c>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>2033</v>
       </c>
@@ -19752,7 +19756,7 @@
         <v>19884</v>
       </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>2034</v>
       </c>
@@ -19781,7 +19785,7 @@
         <v>19885</v>
       </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>2035</v>
       </c>
@@ -19810,7 +19814,7 @@
         <v>19886</v>
       </c>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>2036</v>
       </c>
@@ -19839,7 +19843,7 @@
         <v>19886</v>
       </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>2037</v>
       </c>
@@ -19868,7 +19872,7 @@
         <v>19886</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>2038</v>
       </c>
@@ -19897,12 +19901,12 @@
         <v>19886</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>24</v>
       </c>
@@ -19925,7 +19929,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>2018</v>
       </c>
@@ -19954,7 +19958,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>2019</v>
       </c>
@@ -19983,7 +19987,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>2020</v>
       </c>
@@ -20012,7 +20016,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>2021</v>
       </c>
@@ -20041,7 +20045,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>2022</v>
       </c>
@@ -20070,7 +20074,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>2023</v>
       </c>
@@ -20099,7 +20103,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>2024</v>
       </c>
@@ -20128,7 +20132,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>2025</v>
       </c>
@@ -20157,7 +20161,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>2026</v>
       </c>
@@ -20186,7 +20190,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>2027</v>
       </c>
@@ -20215,7 +20219,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>2028</v>
       </c>
@@ -20244,7 +20248,7 @@
         <v>1447</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>2029</v>
       </c>
@@ -20273,7 +20277,7 @@
         <v>1494</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>2030</v>
       </c>
@@ -20302,7 +20306,7 @@
         <v>1495</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>2031</v>
       </c>
@@ -20331,7 +20335,7 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>2032</v>
       </c>
@@ -20360,7 +20364,7 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>2033</v>
       </c>
@@ -20389,7 +20393,7 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>2034</v>
       </c>
@@ -20418,7 +20422,7 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>2035</v>
       </c>
@@ -20447,7 +20451,7 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>2036</v>
       </c>
@@ -20476,7 +20480,7 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>2037</v>
       </c>
@@ -20505,7 +20509,7 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>2038</v>
       </c>
@@ -20557,7 +20561,7 @@
     <col min="19" max="19" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -20622,7 +20626,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -20687,7 +20691,7 @@
         <v>-2190.4</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -20752,7 +20756,7 @@
         <v>-1745.8181818181818</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -20817,7 +20821,7 @@
         <v>-1152.7272727272725</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -20882,7 +20886,7 @@
         <v>-271.6754320060104</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -20947,7 +20951,7 @@
         <v>1132.4363089952869</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -21012,7 +21016,7 @@
         <v>3421.2764900559437</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -21077,7 +21081,7 @@
         <v>7111.4683603895064</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -21142,7 +21146,7 @@
         <v>12637.031819549376</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -21207,7 +21211,7 @@
         <v>19631.750176938076</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -21272,7 +21276,7 @@
         <v>25757.144754234483</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -21337,7 +21341,7 @@
         <v>27732.128808666199</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -21402,7 +21406,7 @@
         <v>26051.37036309313</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -21467,7 +21471,7 @@
         <v>23718.623165704772</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -21532,7 +21536,7 @@
         <v>21567.598654930509</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -21597,7 +21601,7 @@
         <v>19609.751845665145</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -21662,7 +21666,7 @@
         <v>17828.770755178317</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -21727,7 +21731,7 @@
         <v>16208.756878687314</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -21792,7 +21796,7 @@
         <v>14735.233526079377</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -21857,7 +21861,7 @@
         <v>13396.314333534016</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -21922,7 +21926,7 @@
         <v>12178.467575940011</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -22006,7 +22010,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -22071,7 +22075,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -22136,7 +22140,7 @@
         <v>-643.25983705752697</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -22201,7 +22205,7 @@
         <v>-72.05439732502451</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -22266,7 +22270,7 @@
         <v>842.92575449791173</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -22331,7 +22335,7 @@
         <v>2399.955043533037</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -22396,7 +22400,7 @@
         <v>5063.5476831790656</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -22461,7 +22465,7 @@
         <v>9614.8053492014751</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -22526,7 +22530,7 @@
         <v>17108.945253898943</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -22591,7 +22595,7 @@
         <v>28481.47643541612</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -22656,7 +22660,7 @@
         <v>42935.072124649887</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -22721,7 +22725,7 @@
         <v>55591.029717606398</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -22786,7 +22790,7 @@
         <v>59573.817578243667</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -22851,7 +22855,7 @@
         <v>55920.299306813948</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -22916,7 +22920,7 @@
         <v>50906.989418017678</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -22981,7 +22985,7 @@
         <v>46290.899595800242</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -23046,7 +23050,7 @@
         <v>42086.427966244024</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -23111,7 +23115,7 @@
         <v>38263.836305732766</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -23176,7 +23180,7 @@
         <v>34786.872662262016</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -23241,7 +23245,7 @@
         <v>31625.854174581553</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -23306,7 +23310,7 @@
         <v>28750.776522346863</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -23371,7 +23375,7 @@
         <v>26137.069565769867</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -23455,7 +23459,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -23520,7 +23524,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -23585,7 +23589,7 @@
         <v>-1109.126864467409</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -23650,7 +23654,7 @@
         <v>-288.29714951582633</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -23715,7 +23719,7 @@
         <v>1015.2670541591659</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -23780,7 +23784,7 @@
         <v>3227.4028065609241</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -23845,7 +23849,7 @@
         <v>6989.4632439946645</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -23910,7 +23914,7 @@
         <v>13408.717198609498</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -23975,7 +23979,7 @@
         <v>23970.539617621173</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -24040,7 +24044,7 @@
         <v>39989.218104327483</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -24105,7 +24109,7 @@
         <v>60342.763748394696</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -24170,7 +24174,7 @@
         <v>78167.498727406026</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -24235,7 +24239,7 @@
         <v>83782.440422845291</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -24300,7 +24304,7 @@
         <v>78647.351738187601</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -24365,7 +24369,7 @@
         <v>71593.946448537085</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -24430,7 +24434,7 @@
         <v>65103.480919602007</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -24495,7 +24499,7 @@
         <v>59190.038614266297</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -24560,7 +24564,7 @@
         <v>53813.722340317247</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -24625,7 +24629,7 @@
         <v>48923.655003628359</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -24690,7 +24694,7 @@
         <v>44477.949312119948</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -24755,7 +24759,7 @@
         <v>40434.499374654493</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -24820,7 +24824,7 @@
         <v>36758.635795140442</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -24904,7 +24908,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -24969,7 +24973,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -25034,7 +25038,7 @@
         <v>-1540.4913604115791</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -25099,7 +25103,7 @@
         <v>-680.4466912832537</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -25164,7 +25168,7 @@
         <v>658.76747073423201</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -25229,7 +25233,7 @@
         <v>2903.3122761746204</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -25294,7 +25298,7 @@
         <v>6694.8354890980245</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -25359,7 +25363,7 @@
         <v>13140.873785067099</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -25424,7 +25428,7 @@
         <v>23727.045605309897</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -25489,7 +25493,7 @@
         <v>39767.859911317231</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -25554,7 +25558,7 @@
         <v>60141.529027476296</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -25619,7 +25623,7 @@
         <v>77984.558072025655</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -25684,7 +25688,7 @@
         <v>83616.130736135863</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -25749,7 +25753,7 @@
         <v>78496.161113906302</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -25814,7 +25818,7 @@
         <v>71456.500426463172</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -25879,7 +25883,7 @@
         <v>64978.529990443909</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -25944,7 +25948,7 @@
         <v>59076.446860486205</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -26009,7 +26013,7 @@
         <v>53710.457109608076</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -26074,7 +26078,7 @@
         <v>48829.777521165473</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -26139,7 +26143,7 @@
         <v>44392.606146244601</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -26204,7 +26208,7 @@
         <v>40356.91467840418</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -26269,7 +26273,7 @@
         <v>36688.104253094702</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -26353,7 +26357,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -26418,7 +26422,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -26483,7 +26487,7 @@
         <v>-11344.748312411579</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -26548,7 +26552,7 @@
         <v>-9386.1348294650707</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -26613,7 +26617,7 @@
         <v>-6886.5688532327094</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -26678,7 +26682,7 @@
         <v>-3285.3105277322147</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -26743,7 +26747,7 @@
         <v>2242.5050799729665</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -26808,7 +26812,7 @@
         <v>11136.380207256343</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -26873,7 +26877,7 @@
         <v>25317.362307924141</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -26938,7 +26942,7 @@
         <v>46483.530979221337</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -27003,7 +27007,7 @@
         <v>73192.792832123596</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -27068,7 +27072,7 @@
         <v>96600.638155373017</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -27133,7 +27137,7 @@
         <v>104224.40001123541</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -27198,7 +27202,7 @@
         <v>97950.164845732623</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -27263,7 +27267,7 @@
         <v>89167.958639212258</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -27328,7 +27332,7 @@
         <v>81086.112388999929</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -27393,7 +27397,7 @@
         <v>73720.967576466894</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -27458,7 +27462,7 @@
         <v>67024.806842336591</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -27523,7 +27527,7 @@
         <v>60934.254133571834</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -27588,7 +27592,7 @@
         <v>55397.1506210921</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -27653,7 +27657,7 @@
         <v>50361.046019174632</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -27718,7 +27722,7 @@
         <v>45782.769108340566</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -27802,7 +27806,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -27867,7 +27871,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -27932,7 +27936,7 @@
         <v>-7392.4157164674089</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -27997,7 +28001,7 @@
         <v>-5793.1051967885533</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -28062,7 +28066,7 @@
         <v>-3620.1782780722383</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -28127,7 +28131,7 @@
         <v>-315.86455031360538</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -28192,7 +28196,7 @@
         <v>4942.0014230807928</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -28257,7 +28261,7 @@
         <v>13590.46779189982</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -28322,7 +28326,7 @@
         <v>27548.351021236394</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -28387,7 +28391,7 @@
         <v>48511.702536777928</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -28452,7 +28456,7 @@
         <v>75036.585157175039</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -28517,7 +28521,7 @@
         <v>98276.812996328881</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -28582,7 +28586,7 @@
         <v>105748.19532119529</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -28647,7 +28651,7 @@
         <v>99335.433309332511</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -28712,7 +28716,7 @@
         <v>90427.293606121239</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -28777,7 +28781,7 @@
         <v>82230.962358917197</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -28842,7 +28846,7 @@
         <v>74761.740276391676</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -28907,7 +28911,7 @@
         <v>67970.963842268204</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -28972,7 +28976,7 @@
         <v>61794.396860782392</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -29037,7 +29041,7 @@
         <v>56179.098554919889</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -29102,7 +29106,7 @@
         <v>51071.907777199893</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -29167,7 +29171,7 @@
         <v>46429.007070181709</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2038</v>
       </c>

</xml_diff>

<commit_message>
inflated opex and reduced FIT for dslam. Need to change UDWDM FIT"
</commit_message>
<xml_diff>
--- a/tumlknexpectimax/excel_data/input_data_business.xlsx
+++ b/tumlknexpectimax/excel_data/input_data_business.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="945" windowWidth="13680" windowHeight="10950" tabRatio="847"/>
+    <workbookView xWindow="480" yWindow="1005" windowWidth="13680" windowHeight="10890" tabRatio="847" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CAPEX" sheetId="1" r:id="rId1"/>
@@ -1013,10 +1013,10 @@
                   <c:v>14.612123172178348</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25.497323172178351</c:v>
+                  <c:v>14.612123172178348</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.519389886676155</c:v>
+                  <c:v>12.814589886676153</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5.1327825331856927</c:v>
@@ -1034,7 +1034,7 @@
                   <c:v>12.211670303203721</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>23.096870303203723</c:v>
+                  <c:v>10.331648594515361</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>12.594228370284263</c:v>
@@ -1129,7 +1129,7 @@
                   <c:v>5299.166666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5866.833333333333</c:v>
+                  <c:v>41616.833333333336</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>12618.666666666666</c:v>
@@ -1141,7 +1141,7 @@
                   <c:v>12818.666666666666</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5866.833333333333</c:v>
+                  <c:v>11216.333333333334</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>4000</c:v>
@@ -1153,7 +1153,7 @@
                   <c:v>14160</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14800</c:v>
+                  <c:v>27600</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>14160</c:v>
@@ -1245,10 +1245,10 @@
                   <c:v>60860</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>133338.59999999998</c:v>
+                  <c:v>160920</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>129280.20000000001</c:v>
+                  <c:v>69280.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>195086.4</c:v>
@@ -1266,7 +1266,7 @@
                   <c:v>55966.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>168466.5</c:v>
+                  <c:v>108466.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>105356</c:v>
@@ -1293,11 +1293,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="156622336"/>
-        <c:axId val="181991616"/>
+        <c:axId val="107522560"/>
+        <c:axId val="164367168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="156622336"/>
+        <c:axId val="107522560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1326,7 +1326,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181991616"/>
+        <c:crossAx val="164367168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1334,7 +1334,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181991616"/>
+        <c:axId val="164367168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1364,7 +1364,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156622336"/>
+        <c:crossAx val="107522560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1498,46 +1498,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>10000</c:v>
+                  <c:v>17943.470018396354</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19283.042118970367</c:v>
+                  <c:v>12084.153604213881</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43709.823692218881</c:v>
+                  <c:v>15054.912498229378</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44248.4220525376</c:v>
+                  <c:v>15632.081293303681</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10540.776519765759</c:v>
+                  <c:v>13016.782126163325</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11938.918689039821</c:v>
+                  <c:v>10614.873704727679</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50983.71612182937</c:v>
+                  <c:v>24531.165908089675</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>47726.863400003029</c:v>
+                  <c:v>18497.537602056324</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>48220.289169209609</c:v>
+                  <c:v>19546.717423799677</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>37682.867713520049</c:v>
+                  <c:v>26111.97524384196</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44827.8721002112</c:v>
+                  <c:v>15670.9950339712</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12139.814930199653</c:v>
+                  <c:v>11922.241758999651</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>47419.574760442287</c:v>
+                  <c:v>29749.536208516522</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>50088.476920599649</c:v>
+                  <c:v>20832.137833239656</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1557,11 +1557,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="161823744"/>
-        <c:axId val="186269696"/>
+        <c:axId val="167343616"/>
+        <c:axId val="164368896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="161823744"/>
+        <c:axId val="167343616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1571,7 +1571,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186269696"/>
+        <c:crossAx val="164368896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1579,7 +1579,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="186269696"/>
+        <c:axId val="164368896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1609,7 +1609,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161823744"/>
+        <c:crossAx val="167343616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1938,11 +1938,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="186197504"/>
-        <c:axId val="186271424"/>
+        <c:axId val="167345664"/>
+        <c:axId val="164370624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="186197504"/>
+        <c:axId val="167345664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1962,7 +1962,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="186271424"/>
+        <c:crossAx val="164370624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1970,7 +1970,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="186271424"/>
+        <c:axId val="164370624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2009,7 +2009,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="186197504"/>
+        <c:crossAx val="167345664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2591,11 +2591,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="183370240"/>
-        <c:axId val="186273728"/>
+        <c:axId val="166842368"/>
+        <c:axId val="166527552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="183370240"/>
+        <c:axId val="166842368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2605,7 +2605,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186273728"/>
+        <c:crossAx val="166527552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2613,7 +2613,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="186273728"/>
+        <c:axId val="166527552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2624,7 +2624,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183370240"/>
+        <c:crossAx val="166842368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3098,8 +3098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2:W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3196,7 +3196,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
@@ -3227,18 +3227,10 @@
       <c r="P2" s="13"/>
       <c r="Q2" s="13"/>
       <c r="R2" s="13"/>
-      <c r="S2" s="13">
-        <v>0</v>
-      </c>
-      <c r="T2" s="13">
-        <v>0</v>
-      </c>
-      <c r="U2" s="13">
-        <v>0</v>
-      </c>
-      <c r="V2" s="13">
-        <v>0</v>
-      </c>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
       <c r="W2" s="13">
         <v>10000</v>
       </c>
@@ -3246,7 +3238,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>73</v>
       </c>
@@ -3305,11 +3297,9 @@
         <v>0</v>
       </c>
       <c r="S3" s="11">
-        <f>(M3+N3)*$S$46+O3*$W$46</f>
         <v>96261.143172944852</v>
       </c>
       <c r="T3" s="11">
-        <f>(P3+Q3+R3)*$W$44</f>
         <v>5.1327825331856927</v>
       </c>
       <c r="U3" s="11">
@@ -3319,7 +3309,7 @@
         <v>158553.60000000001</v>
       </c>
       <c r="W3" s="11">
-        <f>SUM(U3,V3)</f>
+        <f>U3+V3</f>
         <v>161610.48888888888</v>
       </c>
       <c r="X3" s="12">
@@ -3327,7 +3317,7 @@
         <v>257876.76484436693</v>
       </c>
     </row>
-    <row r="4" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>66</v>
       </c>
@@ -3385,11 +3375,9 @@
         <v>384090.36767452297</v>
       </c>
       <c r="S4" s="11">
-        <f t="shared" ref="S4:S15" si="0">(M4+N4)*$S$46+O4*$W$46</f>
         <v>146337.87420813384</v>
       </c>
       <c r="T4" s="11">
-        <f t="shared" ref="T4:T15" si="1">(P4+Q4+R4)*$W$44</f>
         <v>12.814589886676153</v>
       </c>
       <c r="U4" s="11">
@@ -3399,15 +3387,15 @@
         <v>63750.8</v>
       </c>
       <c r="W4" s="11">
-        <f t="shared" ref="W4:W15" si="2">SUM(U4,V4)</f>
+        <f t="shared" ref="W4:W15" si="0">U4+V4</f>
         <v>70156.133333333331</v>
       </c>
       <c r="X4" s="12">
-        <f t="shared" ref="X4:X14" si="3">S4+T4+U4+V4</f>
+        <f t="shared" ref="X4:X14" si="1">S4+T4+U4+V4</f>
         <v>216506.82213135384</v>
       </c>
     </row>
-    <row r="5" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>67</v>
       </c>
@@ -3461,11 +3449,9 @@
         <v>658286.15266324603</v>
       </c>
       <c r="S5" s="11">
-        <f t="shared" si="0"/>
         <v>78872.086550701642</v>
       </c>
       <c r="T5" s="11">
-        <f t="shared" si="1"/>
         <v>14.612123172178348</v>
       </c>
       <c r="U5" s="11">
@@ -3475,15 +3461,15 @@
         <v>60860</v>
       </c>
       <c r="W5" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>66159.166666666672</v>
       </c>
       <c r="X5" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>145045.86534054048</v>
       </c>
     </row>
-    <row r="6" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>68</v>
       </c>
@@ -3543,29 +3529,27 @@
         <v>1202546.152663246</v>
       </c>
       <c r="S6" s="11">
+        <v>78872.086550701642</v>
+      </c>
+      <c r="T6" s="11">
+        <v>14.612123172178348</v>
+      </c>
+      <c r="U6" s="11">
+        <v>41616.833333333336</v>
+      </c>
+      <c r="V6" s="11">
+        <v>160920</v>
+      </c>
+      <c r="W6" s="11">
         <f t="shared" si="0"/>
-        <v>78872.086550701642</v>
-      </c>
-      <c r="T6" s="11">
+        <v>202536.83333333334</v>
+      </c>
+      <c r="X6" s="12">
         <f t="shared" si="1"/>
-        <v>25.497323172178351</v>
-      </c>
-      <c r="U6" s="11">
-        <v>5866.833333333333</v>
-      </c>
-      <c r="V6" s="11">
-        <v>133338.59999999998</v>
-      </c>
-      <c r="W6" s="11">
-        <f t="shared" si="2"/>
-        <v>139205.43333333332</v>
-      </c>
-      <c r="X6" s="12">
-        <f t="shared" si="3"/>
-        <v>218103.01720720713</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <v>281423.53200720716</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>69</v>
       </c>
@@ -3624,29 +3608,27 @@
         <v>969330.36767452303</v>
       </c>
       <c r="S7" s="11">
-        <f t="shared" si="0"/>
         <v>146337.87420813384</v>
       </c>
       <c r="T7" s="11">
-        <f t="shared" si="1"/>
-        <v>24.519389886676155</v>
+        <v>12.814589886676153</v>
       </c>
       <c r="U7" s="11">
         <v>12618.666666666666</v>
       </c>
       <c r="V7" s="11">
-        <v>129280.20000000001</v>
+        <v>69280.2</v>
       </c>
       <c r="W7" s="11">
-        <f t="shared" si="2"/>
-        <v>141898.86666666667</v>
+        <f t="shared" si="0"/>
+        <v>81898.866666666669</v>
       </c>
       <c r="X7" s="12">
-        <f t="shared" si="3"/>
-        <v>288261.26026468718</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>228249.55546468718</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>70</v>
       </c>
@@ -3702,11 +3684,9 @@
         <v>0</v>
       </c>
       <c r="S8" s="11">
-        <f t="shared" si="0"/>
         <v>96261.143172944852</v>
       </c>
       <c r="T8" s="11">
-        <f t="shared" si="1"/>
         <v>5.1327825331856927</v>
       </c>
       <c r="U8" s="11">
@@ -3716,15 +3696,15 @@
         <v>195086.4</v>
       </c>
       <c r="W8" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>201513.06666666665</v>
       </c>
       <c r="X8" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>297779.34262214473</v>
       </c>
     </row>
-    <row r="9" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>71</v>
       </c>
@@ -3780,11 +3760,9 @@
         <v>384090.36767452297</v>
       </c>
       <c r="S9" s="11">
-        <f t="shared" si="0"/>
         <v>146337.87420813384</v>
       </c>
       <c r="T9" s="11">
-        <f t="shared" si="1"/>
         <v>12.814589886676153</v>
       </c>
       <c r="U9" s="11">
@@ -3794,15 +3772,15 @@
         <v>61989.9</v>
       </c>
       <c r="W9" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>74808.566666666666</v>
       </c>
       <c r="X9" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>221159.25546468716</v>
       </c>
     </row>
-    <row r="10" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>72</v>
       </c>
@@ -3857,29 +3835,27 @@
         <v>658286.15266324603</v>
       </c>
       <c r="S10" s="11">
-        <f t="shared" si="0"/>
         <v>78872.086550701642</v>
       </c>
       <c r="T10" s="11">
-        <f t="shared" si="1"/>
         <v>14.612123172178348</v>
       </c>
       <c r="U10" s="11">
-        <v>5866.833333333333</v>
+        <v>11216.333333333334</v>
       </c>
       <c r="V10" s="11">
         <v>63060</v>
       </c>
       <c r="W10" s="11">
-        <f t="shared" si="2"/>
-        <v>68926.833333333328</v>
+        <f t="shared" si="0"/>
+        <v>74276.333333333328</v>
       </c>
       <c r="X10" s="12">
-        <f t="shared" si="3"/>
-        <v>147813.53200720716</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>153163.03200720716</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>74</v>
       </c>
@@ -3936,11 +3912,9 @@
         <v>387592.626526276</v>
       </c>
       <c r="S11" s="11">
-        <f t="shared" si="0"/>
         <v>114876.35990534152</v>
       </c>
       <c r="T11" s="11">
-        <f t="shared" si="1"/>
         <v>12.594228370284263</v>
       </c>
       <c r="U11" s="11">
@@ -3950,15 +3924,15 @@
         <v>96145</v>
       </c>
       <c r="W11" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>100145</v>
       </c>
       <c r="X11" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>215033.95413371181</v>
       </c>
     </row>
-    <row r="12" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>75</v>
       </c>
@@ -4014,11 +3988,9 @@
         <v>368464.72317224898</v>
       </c>
       <c r="S12" s="11">
-        <f t="shared" si="0"/>
         <v>115530.46906962365</v>
       </c>
       <c r="T12" s="11">
-        <f t="shared" si="1"/>
         <v>12.211670303203721</v>
       </c>
       <c r="U12" s="11">
@@ -4028,15 +4000,15 @@
         <v>55966.5</v>
       </c>
       <c r="W12" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>63246.5</v>
       </c>
       <c r="X12" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>178789.18073992687</v>
       </c>
     </row>
-    <row r="13" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>76</v>
       </c>
@@ -4093,29 +4065,27 @@
         <v>912724.72317224904</v>
       </c>
       <c r="S13" s="11">
-        <f t="shared" si="0"/>
         <v>115530.46906962365</v>
       </c>
       <c r="T13" s="11">
-        <f t="shared" si="1"/>
-        <v>23.096870303203723</v>
+        <v>10.331648594515361</v>
       </c>
       <c r="U13" s="11">
         <v>14160</v>
       </c>
       <c r="V13" s="11">
-        <v>168466.5</v>
+        <v>108466.5</v>
       </c>
       <c r="W13" s="11">
-        <f t="shared" si="2"/>
-        <v>182626.5</v>
+        <f t="shared" si="0"/>
+        <v>122626.5</v>
       </c>
       <c r="X13" s="12">
-        <f t="shared" si="3"/>
-        <v>298180.06593992683</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>238167.30071821815</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>77</v>
       </c>
@@ -4171,29 +4141,27 @@
         <v>387592.626526276</v>
       </c>
       <c r="S14" s="11">
-        <f t="shared" si="0"/>
         <v>114876.35990534152</v>
       </c>
       <c r="T14" s="11">
-        <f t="shared" si="1"/>
         <v>12.594228370284263</v>
       </c>
       <c r="U14" s="11">
-        <v>14800</v>
+        <v>27600</v>
       </c>
       <c r="V14" s="11">
         <v>105356</v>
       </c>
       <c r="W14" s="11">
-        <f t="shared" si="2"/>
-        <v>120156</v>
+        <f t="shared" si="0"/>
+        <v>132956</v>
       </c>
       <c r="X14" s="12">
-        <f t="shared" si="3"/>
-        <v>235044.95413371181</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>247844.95413371181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>78</v>
       </c>
@@ -4250,11 +4218,9 @@
         <v>233483.63773783101</v>
       </c>
       <c r="S15" s="11">
-        <f t="shared" si="0"/>
         <v>115530.46906962365</v>
       </c>
       <c r="T15" s="11">
-        <f t="shared" si="1"/>
         <v>9.5120485945153614</v>
       </c>
       <c r="U15" s="11">
@@ -4264,11 +4230,11 @@
         <v>66966.5</v>
       </c>
       <c r="W15" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>81126.5</v>
       </c>
       <c r="X15" s="12">
-        <f t="shared" ref="X15" si="4">SUM(S15:V15)</f>
+        <f t="shared" ref="X15" si="2">SUM(S15:V15)</f>
         <v>196666.48111821816</v>
       </c>
     </row>
@@ -17405,8 +17371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17429,111 +17395,112 @@
         <v>23</v>
       </c>
       <c r="B2" s="12">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <f>AVERAGE(B3:B15)</f>
+        <v>17943.470018396354</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>73</v>
       </c>
       <c r="B3" s="12">
-        <v>19283.042118970367</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>12084.153604213881</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>66</v>
       </c>
       <c r="B4" s="12">
-        <v>43709.823692218881</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>15054.912498229378</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>67</v>
       </c>
       <c r="B5" s="12">
-        <v>44248.4220525376</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>15632.081293303681</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>68</v>
       </c>
       <c r="B6" s="12">
-        <v>10540.776519765759</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>13016.782126163325</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>69</v>
       </c>
       <c r="B7" s="12">
-        <v>11938.918689039821</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>10614.873704727679</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>70</v>
       </c>
       <c r="B8" s="12">
-        <v>50983.71612182937</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>24531.165908089675</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B9" s="12">
-        <v>47726.863400003029</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>18497.537602056324</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>72</v>
       </c>
       <c r="B10" s="12">
-        <v>48220.289169209609</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>19546.717423799677</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>74</v>
       </c>
       <c r="B11" s="12">
-        <v>37682.867713520049</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <v>26111.97524384196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>75</v>
       </c>
       <c r="B12" s="12">
-        <v>44827.8721002112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>15670.9950339712</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>76</v>
       </c>
       <c r="B13" s="12">
-        <v>12139.814930199653</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+        <v>11922.241758999651</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>77</v>
       </c>
       <c r="B14" s="12">
-        <v>47419.574760442287</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+        <v>29749.536208516522</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>78</v>
       </c>
       <c r="B15" s="12">
-        <v>50088.476920599649</v>
+        <v>20832.137833239656</v>
       </c>
     </row>
   </sheetData>
@@ -17697,31 +17664,31 @@
       </c>
       <c r="U2" s="7">
         <f>OPEX!$B$6</f>
-        <v>10540.776519765759</v>
+        <v>13016.782126163325</v>
       </c>
       <c r="V2" s="11">
         <f>O2-U2</f>
-        <v>-9256.7765197657591</v>
+        <v>-11732.782126163325</v>
       </c>
       <c r="W2" s="11">
         <f>P2-U2</f>
-        <v>-9256.7765197657591</v>
+        <v>-11732.782126163325</v>
       </c>
       <c r="X2" s="11">
         <f t="shared" ref="X2:X22" si="1">Q2-U2</f>
-        <v>-9256.7765197657591</v>
+        <v>-11732.782126163325</v>
       </c>
       <c r="Y2" s="11">
         <f>R2-$U2</f>
-        <v>-9400.7765197657591</v>
+        <v>-11876.782126163325</v>
       </c>
       <c r="Z2" s="11">
         <f>S2-$U2</f>
-        <v>-9400.7765197657591</v>
+        <v>-11876.782126163325</v>
       </c>
       <c r="AA2" s="11">
         <f>T2-$U2</f>
-        <v>-9400.7765197657591</v>
+        <v>-11876.782126163325</v>
       </c>
       <c r="AB2" s="11">
         <f>1/POWER(1+$L$25,N2-2018)</f>
@@ -17729,27 +17696,27 @@
       </c>
       <c r="AC2" s="12">
         <f>V2*AB2</f>
-        <v>-9256.7765197657591</v>
+        <v>-11732.782126163325</v>
       </c>
       <c r="AD2" s="12">
         <f>W2*AB2</f>
-        <v>-9256.7765197657591</v>
+        <v>-11732.782126163325</v>
       </c>
       <c r="AE2" s="12">
         <f>X2*AB2</f>
-        <v>-9256.7765197657591</v>
+        <v>-11732.782126163325</v>
       </c>
       <c r="AF2" s="12">
         <f>Y2*$AB2</f>
-        <v>-9400.7765197657591</v>
+        <v>-11876.782126163325</v>
       </c>
       <c r="AG2" s="12">
         <f>Z2*$AB2</f>
-        <v>-9400.7765197657591</v>
+        <v>-11876.782126163325</v>
       </c>
       <c r="AH2" s="12">
         <f>AA2*$AB2</f>
-        <v>-9400.7765197657591</v>
+        <v>-11876.782126163325</v>
       </c>
     </row>
     <row r="3" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -17799,31 +17766,31 @@
       </c>
       <c r="U3" s="7">
         <f>OPEX!$B$6</f>
-        <v>10540.776519765759</v>
+        <v>13016.782126163325</v>
       </c>
       <c r="V3" s="11">
         <f t="shared" ref="V3:V22" si="8">O3-U3</f>
-        <v>-8824.7765197657591</v>
+        <v>-11300.782126163325</v>
       </c>
       <c r="W3" s="11">
         <f t="shared" ref="W3:W22" si="9">P3-U3</f>
-        <v>-8740.7765197657591</v>
+        <v>-11216.782126163325</v>
       </c>
       <c r="X3" s="11">
         <f t="shared" si="1"/>
-        <v>-8104.7765197657591</v>
+        <v>-10580.782126163325</v>
       </c>
       <c r="Y3" s="11">
         <f t="shared" ref="Y3:Y22" si="10">R3-$U3</f>
-        <v>-9004.7765197657591</v>
+        <v>-11480.782126163325</v>
       </c>
       <c r="Z3" s="11">
         <f t="shared" ref="Z3:Z22" si="11">S3-$U3</f>
-        <v>-8932.7765197657591</v>
+        <v>-11408.782126163325</v>
       </c>
       <c r="AA3" s="11">
         <f t="shared" ref="AA3:AA22" si="12">T3-$U3</f>
-        <v>-8380.7765197657591</v>
+        <v>-10856.782126163325</v>
       </c>
       <c r="AB3" s="11">
         <f t="shared" ref="AB3:AB22" si="13">1/POWER(1+$L$25,N3-2018)</f>
@@ -17831,27 +17798,27 @@
       </c>
       <c r="AC3" s="12">
         <f t="shared" ref="AC3:AC22" si="14">V3*AB3</f>
-        <v>-8022.5241088779621</v>
+        <v>-10273.438296512113</v>
       </c>
       <c r="AD3" s="12">
         <f t="shared" ref="AD3:AD22" si="15">W3*AB3</f>
-        <v>-7946.1604725143261</v>
+        <v>-10197.074660148477</v>
       </c>
       <c r="AE3" s="12">
         <f t="shared" ref="AE3:AE22" si="16">X3*AB3</f>
-        <v>-7367.9786543325081</v>
+        <v>-9618.892841966659</v>
       </c>
       <c r="AF3" s="12">
         <f t="shared" ref="AF3:AF22" si="17">Y3*$AB3</f>
-        <v>-8186.1604725143261</v>
+        <v>-10437.074660148477</v>
       </c>
       <c r="AG3" s="12">
         <f t="shared" ref="AG3:AG22" si="18">Z3*$AB3</f>
-        <v>-8120.7059270597811</v>
+        <v>-10371.620114693931</v>
       </c>
       <c r="AH3" s="12">
         <f t="shared" ref="AH3:AH22" si="19">AA3*$AB3</f>
-        <v>-7618.8877452415991</v>
+        <v>-9869.8019328757491</v>
       </c>
     </row>
     <row r="4" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -17910,31 +17877,31 @@
       </c>
       <c r="U4" s="7">
         <f>OPEX!$B$6</f>
-        <v>10540.776519765759</v>
+        <v>13016.782126163325</v>
       </c>
       <c r="V4" s="11">
         <f t="shared" si="8"/>
-        <v>-8188.7765197657591</v>
+        <v>-10664.782126163325</v>
       </c>
       <c r="W4" s="11">
         <f t="shared" si="9"/>
-        <v>-8068.7765197657591</v>
+        <v>-10544.782126163325</v>
       </c>
       <c r="X4" s="11">
         <f t="shared" si="1"/>
-        <v>-5896.7765197657591</v>
+        <v>-8372.7821261633253</v>
       </c>
       <c r="Y4" s="11">
         <f t="shared" si="10"/>
-        <v>-8452.7765197657591</v>
+        <v>-10928.782126163325</v>
       </c>
       <c r="Z4" s="11">
         <f t="shared" si="11"/>
-        <v>-8344.7765197657591</v>
+        <v>-10820.782126163325</v>
       </c>
       <c r="AA4" s="11">
         <f t="shared" si="12"/>
-        <v>-6388.7765197657591</v>
+        <v>-8864.7821261633253</v>
       </c>
       <c r="AB4" s="11">
         <f t="shared" si="13"/>
@@ -17942,27 +17909,27 @@
       </c>
       <c r="AC4" s="12">
         <f t="shared" si="14"/>
-        <v>-6767.5839006328579</v>
+        <v>-8813.8695257548134</v>
       </c>
       <c r="AD4" s="12">
         <f t="shared" si="15"/>
-        <v>-6668.4103469138499</v>
+        <v>-8714.6959720358045</v>
       </c>
       <c r="AE4" s="12">
         <f t="shared" si="16"/>
-        <v>-4873.3690245998005</v>
+        <v>-6919.654649721756</v>
       </c>
       <c r="AF4" s="12">
         <f t="shared" si="17"/>
-        <v>-6985.7657188146759</v>
+        <v>-9032.0513439366314</v>
       </c>
       <c r="AG4" s="12">
         <f t="shared" si="18"/>
-        <v>-6896.509520467569</v>
+        <v>-8942.7951455895236</v>
       </c>
       <c r="AH4" s="12">
         <f t="shared" si="19"/>
-        <v>-5279.9805948477342</v>
+        <v>-7326.2662199696897</v>
       </c>
     </row>
     <row r="5" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -18022,31 +17989,31 @@
       </c>
       <c r="U5" s="7">
         <f>OPEX!$B$6</f>
-        <v>10540.776519765759</v>
+        <v>13016.782126163325</v>
       </c>
       <c r="V5" s="11">
         <f t="shared" si="8"/>
-        <v>-7360.7765197657591</v>
+        <v>-9836.7821261633253</v>
       </c>
       <c r="W5" s="11">
         <f t="shared" si="9"/>
-        <v>-7024.7765197657591</v>
+        <v>-9500.7821261633253</v>
       </c>
       <c r="X5" s="11">
         <f t="shared" si="1"/>
-        <v>-1504.7765197657591</v>
+        <v>-3980.7821261633253</v>
       </c>
       <c r="Y5" s="11">
         <f t="shared" si="10"/>
-        <v>-7696.7765197657591</v>
+        <v>-10172.782126163325</v>
       </c>
       <c r="Z5" s="11">
         <f t="shared" si="11"/>
-        <v>-7384.7765197657591</v>
+        <v>-9860.7821261633253</v>
       </c>
       <c r="AA5" s="11">
         <f t="shared" si="12"/>
-        <v>-2428.7765197657591</v>
+        <v>-4904.7821261633253</v>
       </c>
       <c r="AB5" s="11">
         <f t="shared" si="13"/>
@@ -18054,27 +18021,27 @@
       </c>
       <c r="AC5" s="12">
         <f t="shared" si="14"/>
-        <v>-5530.2603454288183</v>
+        <v>-7390.5200046305954</v>
       </c>
       <c r="AD5" s="12">
         <f t="shared" si="15"/>
-        <v>-5277.8185723258885</v>
+        <v>-7138.0782315276656</v>
       </c>
       <c r="AE5" s="12">
         <f t="shared" si="16"/>
-        <v>-1130.5608713491799</v>
+        <v>-2990.8205305509573</v>
       </c>
       <c r="AF5" s="12">
         <f t="shared" si="17"/>
-        <v>-5782.7021185317481</v>
+        <v>-7642.9617777335252</v>
       </c>
       <c r="AG5" s="12">
         <f t="shared" si="18"/>
-        <v>-5548.2919006504562</v>
+        <v>-7408.5515598522334</v>
       </c>
       <c r="AH5" s="12">
         <f t="shared" si="19"/>
-        <v>-1824.7757473822378</v>
+        <v>-3685.0354065840147</v>
       </c>
     </row>
     <row r="6" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -18134,31 +18101,31 @@
       </c>
       <c r="U6" s="7">
         <f>OPEX!$B$6</f>
-        <v>10540.776519765759</v>
+        <v>13016.782126163325</v>
       </c>
       <c r="V6" s="11">
         <f t="shared" si="8"/>
-        <v>-6196.7765197657591</v>
+        <v>-8672.7821261633253</v>
       </c>
       <c r="W6" s="11">
         <f t="shared" si="9"/>
-        <v>-5584.7765197657591</v>
+        <v>-8060.7821261633253</v>
       </c>
       <c r="X6" s="11">
         <f t="shared" si="1"/>
-        <v>6991.2234802342409</v>
+        <v>4515.2178738366747</v>
       </c>
       <c r="Y6" s="11">
         <f t="shared" si="10"/>
-        <v>-6664.7765197657591</v>
+        <v>-9140.7821261633253</v>
       </c>
       <c r="Z6" s="11">
         <f t="shared" si="11"/>
-        <v>-6100.7765197657591</v>
+        <v>-8576.7821261633253</v>
       </c>
       <c r="AA6" s="11">
         <f t="shared" si="12"/>
-        <v>5227.2234802342409</v>
+        <v>2751.2178738366747</v>
       </c>
       <c r="AB6" s="11">
         <f t="shared" si="13"/>
@@ -18166,27 +18133,27 @@
       </c>
       <c r="AC6" s="12">
         <f t="shared" si="14"/>
-        <v>-4232.481742890347</v>
+        <v>-5923.6268876192362</v>
       </c>
       <c r="AD6" s="12">
         <f t="shared" si="15"/>
-        <v>-3814.4775082069241</v>
+        <v>-5505.6226529358128</v>
       </c>
       <c r="AE6" s="12">
         <f t="shared" si="16"/>
-        <v>4775.0997064642024</v>
+        <v>3083.9545617353142</v>
       </c>
       <c r="AF6" s="12">
         <f t="shared" si="17"/>
-        <v>-4552.1320400012</v>
+        <v>-6243.2771847300892</v>
       </c>
       <c r="AG6" s="12">
         <f t="shared" si="18"/>
-        <v>-4166.9124511753007</v>
+        <v>-5858.0575959041889</v>
       </c>
       <c r="AH6" s="12">
         <f t="shared" si="19"/>
-        <v>3570.2639712002183</v>
+        <v>1879.1188264713298</v>
       </c>
     </row>
     <row r="7" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -18246,31 +18213,31 @@
       </c>
       <c r="U7" s="7">
         <f>OPEX!$B$6</f>
-        <v>10540.776519765759</v>
+        <v>13016.782126163325</v>
       </c>
       <c r="V7" s="11">
         <f t="shared" si="8"/>
-        <v>-4612.7765197657591</v>
+        <v>-7088.7821261633253</v>
       </c>
       <c r="W7" s="11">
         <f t="shared" si="9"/>
-        <v>-3544.7765197657591</v>
+        <v>-6020.7821261633253</v>
       </c>
       <c r="X7" s="11">
         <f t="shared" si="1"/>
-        <v>23287.223480234243</v>
+        <v>20811.217873836675</v>
       </c>
       <c r="Y7" s="11">
         <f t="shared" si="10"/>
-        <v>-5212.7765197657591</v>
+        <v>-7688.7821261633253</v>
       </c>
       <c r="Z7" s="11">
         <f t="shared" si="11"/>
-        <v>-4264.7765197657591</v>
+        <v>-6740.7821261633253</v>
       </c>
       <c r="AA7" s="11">
         <f t="shared" si="12"/>
-        <v>19879.223480234243</v>
+        <v>17403.217873836675</v>
       </c>
       <c r="AB7" s="11">
         <f t="shared" si="13"/>
@@ -18278,27 +18245,27 @@
       </c>
       <c r="AC7" s="12">
         <f t="shared" si="14"/>
-        <v>-2864.1712996291594</v>
+        <v>-4401.5759766554211</v>
       </c>
       <c r="AD7" s="12">
         <f t="shared" si="15"/>
-        <v>-2201.0273266019817</v>
+        <v>-3738.4320036282438</v>
       </c>
       <c r="AE7" s="12">
         <f t="shared" si="16"/>
-        <v>14459.533613721265</v>
+        <v>12922.128936695</v>
       </c>
       <c r="AF7" s="12">
         <f t="shared" si="17"/>
-        <v>-3236.724093464652</v>
+        <v>-4774.1287704909146</v>
       </c>
       <c r="AG7" s="12">
         <f t="shared" si="18"/>
-        <v>-2648.0906792045735</v>
+        <v>-4185.4953562308356</v>
       </c>
       <c r="AH7" s="12">
         <f t="shared" si="19"/>
-        <v>12343.433744735665</v>
+        <v>10806.029067709402</v>
       </c>
     </row>
     <row r="8" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -18358,31 +18325,31 @@
       </c>
       <c r="U8" s="7">
         <f>OPEX!$B$6</f>
-        <v>10540.776519765759</v>
+        <v>13016.782126163325</v>
       </c>
       <c r="V8" s="11">
         <f t="shared" si="8"/>
-        <v>-2428.7765197657591</v>
+        <v>-4904.7821261633253</v>
       </c>
       <c r="W8" s="11">
         <f t="shared" si="9"/>
-        <v>-628.77651976575908</v>
+        <v>-3104.7821261633253</v>
       </c>
       <c r="X8" s="11">
         <f t="shared" si="1"/>
-        <v>53191.223480234243</v>
+        <v>50715.217873836678</v>
       </c>
       <c r="Y8" s="11">
         <f t="shared" si="10"/>
-        <v>-3280.7765197657591</v>
+        <v>-5756.7821261633253</v>
       </c>
       <c r="Z8" s="11">
         <f t="shared" si="11"/>
-        <v>-1624.7765197657591</v>
+        <v>-4100.7821261633253</v>
       </c>
       <c r="AA8" s="11">
         <f t="shared" si="12"/>
-        <v>46795.223480234243</v>
+        <v>44319.217873836678</v>
       </c>
       <c r="AB8" s="11">
         <f t="shared" si="13"/>
@@ -18390,27 +18357,27 @@
       </c>
       <c r="AC8" s="12">
         <f t="shared" si="14"/>
-        <v>-1370.9810273345136</v>
+        <v>-2768.6216428129337</v>
       </c>
       <c r="AD8" s="12">
         <f t="shared" si="15"/>
-        <v>-354.92795323771458</v>
+        <v>-1752.5685687161347</v>
       </c>
       <c r="AE8" s="12">
         <f t="shared" si="16"/>
-        <v>30025.058962256575</v>
+        <v>28627.418346778159</v>
       </c>
       <c r="AF8" s="12">
         <f t="shared" si="17"/>
-        <v>-1851.9128157403318</v>
+        <v>-3249.5534312187519</v>
       </c>
       <c r="AG8" s="12">
         <f t="shared" si="18"/>
-        <v>-917.14398757127663</v>
+        <v>-2314.7846030496967</v>
       </c>
       <c r="AH8" s="12">
         <f t="shared" si="19"/>
-        <v>26414.683705632619</v>
+        <v>25017.043090154199</v>
       </c>
     </row>
     <row r="9" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -18469,31 +18436,31 @@
       </c>
       <c r="U9" s="7">
         <f>OPEX!$B$6</f>
-        <v>10540.776519765759</v>
+        <v>13016.782126163325</v>
       </c>
       <c r="V9" s="11">
         <f t="shared" si="8"/>
-        <v>547.22348023424092</v>
+        <v>-1928.7821261633253</v>
       </c>
       <c r="W9" s="11">
         <f t="shared" si="9"/>
-        <v>3475.2234802342409</v>
+        <v>999.2178738366747</v>
       </c>
       <c r="X9" s="11">
         <f t="shared" si="1"/>
-        <v>103999.22348023424</v>
+        <v>101523.21787383668</v>
       </c>
       <c r="Y9" s="11">
         <f t="shared" si="10"/>
-        <v>-580.77651976575908</v>
+        <v>-3056.7821261633253</v>
       </c>
       <c r="Z9" s="11">
         <f t="shared" si="11"/>
-        <v>2035.2234802342409</v>
+        <v>-440.7821261633253</v>
       </c>
       <c r="AA9" s="11">
         <f t="shared" si="12"/>
-        <v>92527.223480234243</v>
+        <v>90051.217873836678</v>
       </c>
       <c r="AB9" s="11">
         <f t="shared" si="13"/>
@@ -18501,27 +18468,27 @@
       </c>
       <c r="AC9" s="12">
         <f t="shared" si="14"/>
-        <v>280.81217136866127</v>
+        <v>-989.77020633899303</v>
       </c>
       <c r="AD9" s="12">
         <f t="shared" si="15"/>
-        <v>1783.3391415481697</v>
+        <v>512.75676384051542</v>
       </c>
       <c r="AE9" s="12">
         <f t="shared" si="16"/>
-        <v>53368.045818571707</v>
+        <v>52097.463440864056</v>
       </c>
       <c r="AF9" s="12">
         <f t="shared" si="17"/>
-        <v>-298.03018599557561</v>
+        <v>-1568.6125637032299</v>
       </c>
       <c r="AG9" s="12">
         <f t="shared" si="18"/>
-        <v>1044.3914512959525</v>
+        <v>-226.19092641170184</v>
       </c>
       <c r="AH9" s="12">
         <f t="shared" si="19"/>
-        <v>47481.095886229043</v>
+        <v>46210.513508521391</v>
       </c>
     </row>
     <row r="10" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -18580,31 +18547,31 @@
       </c>
       <c r="U10" s="7">
         <f>OPEX!$B$6</f>
-        <v>10540.776519765759</v>
+        <v>13016.782126163325</v>
       </c>
       <c r="V10" s="11">
         <f t="shared" si="8"/>
-        <v>4603.2234802342409</v>
+        <v>2127.2178738366747</v>
       </c>
       <c r="W10" s="11">
         <f t="shared" si="9"/>
-        <v>9235.2234802342409</v>
+        <v>6759.2178738366747</v>
       </c>
       <c r="X10" s="11">
         <f t="shared" si="1"/>
-        <v>177691.22348023424</v>
+        <v>175215.21787383666</v>
       </c>
       <c r="Y10" s="11">
         <f t="shared" si="10"/>
-        <v>3067.2234802342409</v>
+        <v>591.2178738366747</v>
       </c>
       <c r="Z10" s="11">
         <f t="shared" si="11"/>
-        <v>7219.2234802342409</v>
+        <v>4743.2178738366747</v>
       </c>
       <c r="AA10" s="11">
         <f t="shared" si="12"/>
-        <v>158839.22348023424</v>
+        <v>156363.21787383666</v>
       </c>
       <c r="AB10" s="11">
         <f t="shared" si="13"/>
@@ -18612,27 +18579,27 @@
       </c>
       <c r="AC10" s="12">
         <f t="shared" si="14"/>
-        <v>2147.4377262840062</v>
+        <v>992.36283745886578</v>
       </c>
       <c r="AD10" s="12">
         <f t="shared" si="15"/>
-        <v>4308.29991141549</v>
+        <v>3153.2250225903499</v>
       </c>
       <c r="AE10" s="12">
         <f t="shared" si="16"/>
-        <v>82894.267152026296</v>
+        <v>81739.192263201156</v>
       </c>
       <c r="AF10" s="12">
         <f t="shared" si="17"/>
-        <v>1430.882390281856</v>
+        <v>275.80750145671567</v>
       </c>
       <c r="AG10" s="12">
         <f t="shared" si="18"/>
-        <v>3367.8210329126678</v>
+        <v>2212.7461440875277</v>
       </c>
       <c r="AH10" s="12">
         <f t="shared" si="19"/>
-        <v>74099.670020312406</v>
+        <v>72944.595131487265</v>
       </c>
     </row>
     <row r="11" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -18691,31 +18658,31 @@
       </c>
       <c r="U11" s="7">
         <f>OPEX!$B$6</f>
-        <v>10540.776519765759</v>
+        <v>13016.782126163325</v>
       </c>
       <c r="V11" s="11">
         <f t="shared" si="8"/>
-        <v>10075.223480234241</v>
+        <v>7599.2178738366747</v>
       </c>
       <c r="W11" s="11">
         <f t="shared" si="9"/>
-        <v>17203.223480234243</v>
+        <v>14727.217873836675</v>
       </c>
       <c r="X11" s="11">
         <f t="shared" si="1"/>
-        <v>256435.22348023424</v>
+        <v>253959.21787383666</v>
       </c>
       <c r="Y11" s="11">
         <f t="shared" si="10"/>
-        <v>7987.2234802342409</v>
+        <v>5511.2178738366747</v>
       </c>
       <c r="Z11" s="11">
         <f t="shared" si="11"/>
-        <v>14395.223480234241</v>
+        <v>11919.217873836675</v>
       </c>
       <c r="AA11" s="11">
         <f t="shared" si="12"/>
-        <v>229723.22348023424</v>
+        <v>227247.21787383666</v>
       </c>
       <c r="AB11" s="11">
         <f t="shared" si="13"/>
@@ -18723,27 +18690,27 @@
       </c>
       <c r="AC11" s="12">
         <f t="shared" si="14"/>
-        <v>4272.8782825378776</v>
+        <v>3222.8102017877504</v>
       </c>
       <c r="AD11" s="12">
         <f t="shared" si="15"/>
-        <v>7295.8461062969491</v>
+        <v>6245.7780255468215</v>
       </c>
       <c r="AE11" s="12">
         <f t="shared" si="16"/>
-        <v>108753.5675447832</v>
+        <v>107703.49946403307</v>
       </c>
       <c r="AF11" s="12">
         <f t="shared" si="17"/>
-        <v>3387.3624553761301</v>
+        <v>2337.2943746260025</v>
       </c>
       <c r="AG11" s="12">
         <f t="shared" si="18"/>
-        <v>6104.9799939070117</v>
+        <v>5054.9119131568841</v>
       </c>
       <c r="AH11" s="12">
         <f t="shared" si="19"/>
-        <v>97425.071962817383</v>
+        <v>96375.003882067263</v>
       </c>
     </row>
     <row r="12" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -18803,31 +18770,31 @@
       </c>
       <c r="U12" s="7">
         <f>OPEX!$B$6</f>
-        <v>10540.776519765759</v>
+        <v>13016.782126163325</v>
       </c>
       <c r="V12" s="11">
         <f t="shared" si="8"/>
-        <v>17419.223480234243</v>
+        <v>14943.217873836675</v>
       </c>
       <c r="W12" s="11">
         <f t="shared" si="9"/>
-        <v>28039.223480234243</v>
+        <v>25563.217873836675</v>
       </c>
       <c r="X12" s="11">
         <f t="shared" si="1"/>
-        <v>303715.22348023421</v>
+        <v>301239.21787383669</v>
       </c>
       <c r="Y12" s="11">
         <f t="shared" si="10"/>
-        <v>14587.223480234241</v>
+        <v>12111.217873836675</v>
       </c>
       <c r="Z12" s="11">
         <f t="shared" si="11"/>
-        <v>24163.223480234243</v>
+        <v>21687.217873836675</v>
       </c>
       <c r="AA12" s="11">
         <f t="shared" si="12"/>
-        <v>272275.22348023421</v>
+        <v>269799.21787383669</v>
       </c>
       <c r="AB12" s="11">
         <f t="shared" si="13"/>
@@ -18835,27 +18802,27 @@
       </c>
       <c r="AC12" s="12">
         <f t="shared" si="14"/>
-        <v>6715.8647198776416</v>
+        <v>5761.2573737411612</v>
       </c>
       <c r="AD12" s="12">
         <f t="shared" si="15"/>
-        <v>10810.334453619265</v>
+        <v>9855.7271074827859</v>
       </c>
       <c r="AE12" s="12">
         <f t="shared" si="16"/>
-        <v>117095.36631039478</v>
+        <v>116140.75896425832</v>
       </c>
       <c r="AF12" s="12">
         <f t="shared" si="17"/>
-        <v>5624.0061242132069</v>
+        <v>4669.3987780767275</v>
       </c>
       <c r="AG12" s="12">
         <f t="shared" si="18"/>
-        <v>9315.9686637904015</v>
+        <v>8361.361317653922</v>
       </c>
       <c r="AH12" s="12">
         <f t="shared" si="19"/>
-        <v>104973.88529073031</v>
+        <v>104019.27794459384</v>
       </c>
     </row>
     <row r="13" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -18914,31 +18881,31 @@
       </c>
       <c r="U13" s="7">
         <f>OPEX!$B$6</f>
-        <v>10540.776519765759</v>
+        <v>13016.782126163325</v>
       </c>
       <c r="V13" s="11">
         <f t="shared" si="8"/>
-        <v>27067.223480234243</v>
+        <v>24591.217873836675</v>
       </c>
       <c r="W13" s="11">
         <f t="shared" si="9"/>
-        <v>42631.223480234243</v>
+        <v>40155.217873836678</v>
       </c>
       <c r="X13" s="11">
         <f t="shared" si="1"/>
-        <v>313855.22348023421</v>
+        <v>311379.21787383669</v>
       </c>
       <c r="Y13" s="11">
         <f t="shared" si="10"/>
-        <v>23275.223480234243</v>
+        <v>20799.217873836675</v>
       </c>
       <c r="Z13" s="11">
         <f t="shared" si="11"/>
-        <v>37279.223480234243</v>
+        <v>34803.217873836678</v>
       </c>
       <c r="AA13" s="11">
         <f t="shared" si="12"/>
-        <v>281407.22348023421</v>
+        <v>278931.21787383669</v>
       </c>
       <c r="AB13" s="11">
         <f t="shared" si="13"/>
@@ -18946,27 +18913,27 @@
       </c>
       <c r="AC13" s="12">
         <f t="shared" si="14"/>
-        <v>9486.8967057215996</v>
+        <v>8619.0718455975275</v>
       </c>
       <c r="AD13" s="12">
         <f t="shared" si="15"/>
-        <v>14941.983757249987</v>
+        <v>14074.158897125917</v>
       </c>
       <c r="AE13" s="12">
         <f t="shared" si="16"/>
-        <v>110004.3411501911</v>
+        <v>109136.51629006704</v>
       </c>
       <c r="AF13" s="12">
         <f t="shared" si="17"/>
-        <v>8157.82383888816</v>
+        <v>7289.998978764087</v>
       </c>
       <c r="AG13" s="12">
         <f t="shared" si="18"/>
-        <v>13066.140407225577</v>
+        <v>12198.315547101505</v>
       </c>
       <c r="AH13" s="12">
         <f t="shared" si="19"/>
-        <v>98631.515099818876</v>
+        <v>97763.690239694828</v>
       </c>
     </row>
     <row r="14" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -19025,31 +18992,31 @@
       </c>
       <c r="U14" s="7">
         <f>OPEX!$B$6</f>
-        <v>10540.776519765759</v>
+        <v>13016.782126163325</v>
       </c>
       <c r="V14" s="11">
         <f t="shared" si="8"/>
-        <v>39691.223480234243</v>
+        <v>37215.217873836678</v>
       </c>
       <c r="W14" s="11">
         <f t="shared" si="9"/>
-        <v>61675.223480234243</v>
+        <v>59199.217873836678</v>
       </c>
       <c r="X14" s="11">
         <f t="shared" si="1"/>
-        <v>314311.22348023421</v>
+        <v>311835.21787383669</v>
       </c>
       <c r="Y14" s="11">
         <f t="shared" si="10"/>
-        <v>34651.223480234243</v>
+        <v>32175.217873836675</v>
       </c>
       <c r="Z14" s="11">
         <f t="shared" si="11"/>
-        <v>54439.223480234243</v>
+        <v>51963.217873836678</v>
       </c>
       <c r="AA14" s="11">
         <f t="shared" si="12"/>
-        <v>281791.22348023421</v>
+        <v>279315.21787383669</v>
       </c>
       <c r="AB14" s="11">
         <f t="shared" si="13"/>
@@ -19057,27 +19024,27 @@
       </c>
       <c r="AC14" s="12">
         <f t="shared" si="14"/>
-        <v>12646.846993431542</v>
+        <v>11857.915302409658</v>
       </c>
       <c r="AD14" s="12">
         <f t="shared" si="15"/>
-        <v>19651.626889976022</v>
+        <v>18862.695198954138</v>
       </c>
       <c r="AE14" s="12">
         <f t="shared" si="16"/>
-        <v>100149.24215304965</v>
+        <v>99360.310462027788</v>
       </c>
       <c r="AF14" s="12">
         <f t="shared" si="17"/>
-        <v>11040.947672171344</v>
+        <v>10252.01598114946</v>
       </c>
       <c r="AG14" s="12">
         <f t="shared" si="18"/>
-        <v>17346.01429302388</v>
+        <v>16557.082602001996</v>
       </c>
       <c r="AH14" s="12">
         <f t="shared" si="19"/>
-        <v>89787.367961108859</v>
+        <v>88998.436270086982</v>
       </c>
     </row>
     <row r="15" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -19136,31 +19103,31 @@
       </c>
       <c r="U15" s="7">
         <f>OPEX!$B$6</f>
-        <v>10540.776519765759</v>
+        <v>13016.782126163325</v>
       </c>
       <c r="V15" s="11">
         <f t="shared" si="8"/>
-        <v>55771.223480234243</v>
+        <v>53295.217873836678</v>
       </c>
       <c r="W15" s="11">
         <f t="shared" si="9"/>
-        <v>85795.223480234243</v>
+        <v>83319.217873836678</v>
       </c>
       <c r="X15" s="11">
         <f t="shared" si="1"/>
-        <v>314395.22348023421</v>
+        <v>311919.21787383669</v>
       </c>
       <c r="Y15" s="11">
         <f t="shared" si="10"/>
-        <v>49135.223480234243</v>
+        <v>46659.217873836678</v>
       </c>
       <c r="Z15" s="11">
         <f t="shared" si="11"/>
-        <v>76135.223480234243</v>
+        <v>73659.217873836678</v>
       </c>
       <c r="AA15" s="11">
         <f t="shared" si="12"/>
-        <v>281875.22348023421</v>
+        <v>279399.21787383669</v>
       </c>
       <c r="AB15" s="11">
         <f t="shared" si="13"/>
@@ -19168,27 +19135,27 @@
       </c>
       <c r="AC15" s="12">
         <f t="shared" si="14"/>
-        <v>16154.93685655825</v>
+        <v>15437.726228356538</v>
       </c>
       <c r="AD15" s="12">
         <f t="shared" si="15"/>
-        <v>24851.820193772564</v>
+        <v>24134.609565570852</v>
       </c>
       <c r="AE15" s="12">
         <f t="shared" si="16"/>
-        <v>91069.097401579391</v>
+        <v>90351.886773377686</v>
       </c>
       <c r="AF15" s="12">
         <f t="shared" si="17"/>
-        <v>14232.724032625591</v>
+        <v>13515.513404423878</v>
       </c>
       <c r="AG15" s="12">
         <f t="shared" si="18"/>
-        <v>22053.662285516162</v>
+        <v>21336.45165731445</v>
       </c>
       <c r="AH15" s="12">
         <f t="shared" si="19"/>
-        <v>81649.211772542301</v>
+        <v>80932.001144340597</v>
       </c>
     </row>
     <row r="16" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -19247,31 +19214,31 @@
       </c>
       <c r="U16" s="7">
         <f>OPEX!$B$6</f>
-        <v>10540.776519765759</v>
+        <v>13016.782126163325</v>
       </c>
       <c r="V16" s="11">
         <f t="shared" si="8"/>
-        <v>75763.223480234243</v>
+        <v>73287.217873836678</v>
       </c>
       <c r="W16" s="11">
         <f t="shared" si="9"/>
-        <v>114823.22348023424</v>
+        <v>112347.21787383668</v>
       </c>
       <c r="X16" s="11">
         <f t="shared" si="1"/>
-        <v>314431.22348023421</v>
+        <v>311955.21787383669</v>
       </c>
       <c r="Y16" s="11">
         <f t="shared" si="10"/>
-        <v>67099.223480234243</v>
+        <v>64623.217873836678</v>
       </c>
       <c r="Z16" s="11">
         <f t="shared" si="11"/>
-        <v>102247.22348023424</v>
+        <v>99771.217873836678</v>
       </c>
       <c r="AA16" s="11">
         <f t="shared" si="12"/>
-        <v>281899.22348023421</v>
+        <v>279423.21787383669</v>
       </c>
       <c r="AB16" s="11">
         <f t="shared" si="13"/>
@@ -19279,27 +19246,27 @@
       </c>
       <c r="AC16" s="12">
         <f t="shared" si="14"/>
-        <v>19950.824669321915</v>
+        <v>19298.815007320358</v>
       </c>
       <c r="AD16" s="12">
         <f t="shared" si="15"/>
-        <v>30236.543462517388</v>
+        <v>29584.533800515834</v>
       </c>
       <c r="AE16" s="12">
         <f t="shared" si="16"/>
-        <v>82799.568472045343</v>
+        <v>82147.558810043804</v>
       </c>
       <c r="AF16" s="12">
         <f t="shared" si="17"/>
-        <v>17669.322682014041</v>
+        <v>17017.313020012483</v>
       </c>
       <c r="AG16" s="12">
         <f t="shared" si="18"/>
-        <v>26924.88960836413</v>
+        <v>26272.879946362573</v>
       </c>
       <c r="AH16" s="12">
         <f t="shared" si="19"/>
-        <v>74232.876106959957</v>
+        <v>73580.866444958418</v>
       </c>
     </row>
     <row r="17" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -19358,31 +19325,31 @@
       </c>
       <c r="U17" s="7">
         <f>OPEX!$B$6</f>
-        <v>10540.776519765759</v>
+        <v>13016.782126163325</v>
       </c>
       <c r="V17" s="11">
         <f t="shared" si="8"/>
-        <v>99799.223480234243</v>
+        <v>97323.217873836678</v>
       </c>
       <c r="W17" s="11">
         <f t="shared" si="9"/>
-        <v>147847.22348023424</v>
+        <v>145371.21787383666</v>
       </c>
       <c r="X17" s="11">
         <f t="shared" si="1"/>
-        <v>314455.22348023421</v>
+        <v>311979.21787383669</v>
       </c>
       <c r="Y17" s="11">
         <f t="shared" si="10"/>
-        <v>88735.223480234243</v>
+        <v>86259.217873836678</v>
       </c>
       <c r="Z17" s="11">
         <f t="shared" si="11"/>
-        <v>132007.22348023424</v>
+        <v>129531.21787383668</v>
       </c>
       <c r="AA17" s="11">
         <f t="shared" si="12"/>
-        <v>281923.22348023421</v>
+        <v>279447.21787383669</v>
       </c>
       <c r="AB17" s="11">
         <f t="shared" si="13"/>
@@ -19390,27 +19357,27 @@
       </c>
       <c r="AC17" s="12">
         <f t="shared" si="14"/>
-        <v>23891.140634384406</v>
+        <v>23298.404578019356</v>
       </c>
       <c r="AD17" s="12">
         <f t="shared" si="15"/>
-        <v>35393.449822473965</v>
+        <v>34800.713766108915</v>
       </c>
       <c r="AE17" s="12">
         <f t="shared" si="16"/>
-        <v>75278.080383771536</v>
+        <v>74685.344327406492</v>
       </c>
       <c r="AF17" s="12">
         <f t="shared" si="17"/>
-        <v>21242.507000163983</v>
+        <v>20649.770943798932</v>
       </c>
       <c r="AG17" s="12">
         <f t="shared" si="18"/>
-        <v>31601.47976046642</v>
+        <v>31008.743704101369</v>
       </c>
       <c r="AH17" s="12">
         <f t="shared" si="19"/>
-        <v>67490.178233693907</v>
+        <v>66897.442177328878</v>
       </c>
     </row>
     <row r="18" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -19469,31 +19436,31 @@
       </c>
       <c r="U18" s="7">
         <f>OPEX!$B$6</f>
-        <v>10540.776519765759</v>
+        <v>13016.782126163325</v>
       </c>
       <c r="V18" s="11">
         <f t="shared" si="8"/>
-        <v>127447.22348023424</v>
+        <v>124971.21787383668</v>
       </c>
       <c r="W18" s="11">
         <f t="shared" si="9"/>
-        <v>182707.22348023424</v>
+        <v>180231.21787383666</v>
       </c>
       <c r="X18" s="11">
         <f t="shared" si="1"/>
-        <v>314467.22348023421</v>
+        <v>311991.21787383669</v>
       </c>
       <c r="Y18" s="11">
         <f t="shared" si="10"/>
-        <v>113623.22348023424</v>
+        <v>111147.21787383668</v>
       </c>
       <c r="Z18" s="11">
         <f t="shared" si="11"/>
-        <v>163375.22348023424</v>
+        <v>160899.21787383666</v>
       </c>
       <c r="AA18" s="11">
         <f t="shared" si="12"/>
-        <v>281935.22348023421</v>
+        <v>279459.21787383669</v>
       </c>
       <c r="AB18" s="11">
         <f t="shared" si="13"/>
@@ -19501,27 +19468,27 @@
       </c>
       <c r="AC18" s="12">
         <f t="shared" si="14"/>
-        <v>27736.229104857306</v>
+        <v>27197.378144525439</v>
       </c>
       <c r="AD18" s="12">
         <f t="shared" si="15"/>
-        <v>39762.415148620916</v>
+        <v>39223.564188289041</v>
       </c>
       <c r="AE18" s="12">
         <f t="shared" si="16"/>
-        <v>68437.230080330875</v>
+        <v>67898.379119999023</v>
       </c>
       <c r="AF18" s="12">
         <f t="shared" si="17"/>
-        <v>24727.723931694291</v>
+        <v>24188.872971362427</v>
       </c>
       <c r="AG18" s="12">
         <f t="shared" si="18"/>
-        <v>35555.208695525762</v>
+        <v>35016.357735193895</v>
       </c>
       <c r="AH18" s="12">
         <f t="shared" si="19"/>
-        <v>61357.319034805761</v>
+        <v>60818.468074473909</v>
       </c>
     </row>
     <row r="19" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -19571,31 +19538,31 @@
       </c>
       <c r="U19" s="7">
         <f>OPEX!$B$6</f>
-        <v>10540.776519765759</v>
+        <v>13016.782126163325</v>
       </c>
       <c r="V19" s="11">
         <f t="shared" si="8"/>
-        <v>157531.22348023424</v>
+        <v>155055.21787383666</v>
       </c>
       <c r="W19" s="11">
         <f t="shared" si="9"/>
-        <v>216307.22348023424</v>
+        <v>213831.21787383666</v>
       </c>
       <c r="X19" s="11">
         <f t="shared" si="1"/>
-        <v>314479.22348023421</v>
+        <v>312003.21787383669</v>
       </c>
       <c r="Y19" s="11">
         <f t="shared" si="10"/>
-        <v>140719.22348023424</v>
+        <v>138243.21787383666</v>
       </c>
       <c r="Z19" s="11">
         <f t="shared" si="11"/>
-        <v>193579.22348023424</v>
+        <v>191103.21787383666</v>
       </c>
       <c r="AA19" s="11">
         <f t="shared" si="12"/>
-        <v>281947.22348023421</v>
+        <v>279471.21787383669</v>
       </c>
       <c r="AB19" s="11">
         <f t="shared" si="13"/>
@@ -19603,27 +19570,27 @@
       </c>
       <c r="AC19" s="12">
         <f t="shared" si="14"/>
-        <v>31166.71275088012</v>
+        <v>30676.848241487514</v>
       </c>
       <c r="AD19" s="12">
         <f t="shared" si="15"/>
-        <v>42795.231010154457</v>
+        <v>42305.366500761847</v>
       </c>
       <c r="AE19" s="12">
         <f t="shared" si="16"/>
-        <v>62218.037845418505</v>
+        <v>61728.17333602591</v>
       </c>
       <c r="AF19" s="12">
         <f t="shared" si="17"/>
-        <v>27840.548177331049</v>
+        <v>27350.683667938443</v>
       </c>
       <c r="AG19" s="12">
         <f t="shared" si="18"/>
-        <v>38298.61737539219</v>
+        <v>37808.752865999581</v>
       </c>
       <c r="AH19" s="12">
         <f t="shared" si="19"/>
-        <v>55781.755076759313</v>
+        <v>55291.890567366718</v>
       </c>
     </row>
     <row r="20" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -19673,31 +19640,31 @@
       </c>
       <c r="U20" s="7">
         <f>OPEX!$B$6</f>
-        <v>10540.776519765759</v>
+        <v>13016.782126163325</v>
       </c>
       <c r="V20" s="11">
         <f t="shared" si="8"/>
-        <v>188287.22348023424</v>
+        <v>185811.21787383666</v>
       </c>
       <c r="W20" s="11">
         <f t="shared" si="9"/>
-        <v>245683.22348023424</v>
+        <v>243207.21787383666</v>
       </c>
       <c r="X20" s="11">
         <f t="shared" si="1"/>
-        <v>314479.22348023421</v>
+        <v>312003.21787383669</v>
       </c>
       <c r="Y20" s="11">
         <f t="shared" si="10"/>
-        <v>168391.22348023424</v>
+        <v>165915.21787383666</v>
       </c>
       <c r="Z20" s="11">
         <f t="shared" si="11"/>
-        <v>220027.22348023424</v>
+        <v>217551.21787383666</v>
       </c>
       <c r="AA20" s="11">
         <f t="shared" si="12"/>
-        <v>281947.22348023421</v>
+        <v>279471.21787383669</v>
       </c>
       <c r="AB20" s="11">
         <f t="shared" si="13"/>
@@ -19705,27 +19672,27 @@
       </c>
       <c r="AC20" s="12">
         <f t="shared" si="14"/>
-        <v>33865.11217052061</v>
+        <v>33419.780798345513</v>
       </c>
       <c r="AD20" s="12">
         <f t="shared" si="15"/>
-        <v>44188.287276149837</v>
+        <v>43742.95590397474</v>
       </c>
       <c r="AE20" s="12">
         <f t="shared" si="16"/>
-        <v>56561.852586744091</v>
+        <v>56116.521214569002</v>
       </c>
       <c r="AF20" s="12">
         <f t="shared" si="17"/>
-        <v>30286.641686486895</v>
+        <v>29841.310314311795</v>
       </c>
       <c r="AG20" s="12">
         <f t="shared" si="18"/>
-        <v>39573.83016223905</v>
+        <v>39128.498790063953</v>
       </c>
       <c r="AH20" s="12">
         <f t="shared" si="19"/>
-        <v>50710.686433417555</v>
+        <v>50265.355061242466</v>
       </c>
     </row>
     <row r="21" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -19775,31 +19742,31 @@
       </c>
       <c r="U21" s="7">
         <f>OPEX!$B$6</f>
-        <v>10540.776519765759</v>
+        <v>13016.782126163325</v>
       </c>
       <c r="V21" s="11">
         <f t="shared" si="8"/>
-        <v>217543.22348023424</v>
+        <v>215067.21787383666</v>
       </c>
       <c r="W21" s="11">
         <f t="shared" si="9"/>
-        <v>268939.22348023421</v>
+        <v>266463.21787383669</v>
       </c>
       <c r="X21" s="11">
         <f t="shared" si="1"/>
-        <v>314479.22348023421</v>
+        <v>312003.21787383669</v>
       </c>
       <c r="Y21" s="11">
         <f t="shared" si="10"/>
-        <v>194719.22348023424</v>
+        <v>192243.21787383666</v>
       </c>
       <c r="Z21" s="11">
         <f t="shared" si="11"/>
-        <v>240991.22348023424</v>
+        <v>238515.21787383666</v>
       </c>
       <c r="AA21" s="11">
         <f t="shared" si="12"/>
-        <v>281947.22348023421</v>
+        <v>279471.21787383669</v>
       </c>
       <c r="AB21" s="11">
         <f t="shared" si="13"/>
@@ -19807,27 +19774,27 @@
       </c>
       <c r="AC21" s="12">
         <f t="shared" si="14"/>
-        <v>35570.05538918596</v>
+        <v>35165.208687208593</v>
       </c>
       <c r="AD21" s="12">
         <f t="shared" si="15"/>
-        <v>43973.712085707717</v>
+        <v>43568.865383730365</v>
       </c>
       <c r="AE21" s="12">
         <f t="shared" si="16"/>
-        <v>51419.865987949161</v>
+        <v>51015.019285971808</v>
       </c>
       <c r="AF21" s="12">
         <f t="shared" si="17"/>
-        <v>31838.149006560601</v>
+        <v>31433.302304583241</v>
       </c>
       <c r="AG21" s="12">
         <f t="shared" si="18"/>
-        <v>39403.990758087086</v>
+        <v>38999.144056109726</v>
       </c>
       <c r="AH21" s="12">
         <f t="shared" si="19"/>
-        <v>46100.624030379578</v>
+        <v>45695.777328402233</v>
       </c>
     </row>
     <row r="22" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -19877,31 +19844,31 @@
       </c>
       <c r="U22" s="7">
         <f>OPEX!$B$6</f>
-        <v>10540.776519765759</v>
+        <v>13016.782126163325</v>
       </c>
       <c r="V22" s="11">
         <f t="shared" si="8"/>
-        <v>243331.22348023424</v>
+        <v>240855.21787383666</v>
       </c>
       <c r="W22" s="11">
         <f t="shared" si="9"/>
-        <v>285739.22348023421</v>
+        <v>283263.21787383669</v>
       </c>
       <c r="X22" s="11">
         <f t="shared" si="1"/>
-        <v>314479.22348023421</v>
+        <v>312003.21787383669</v>
       </c>
       <c r="Y22" s="11">
         <f t="shared" si="10"/>
-        <v>217939.22348023424</v>
+        <v>215463.21787383666</v>
       </c>
       <c r="Z22" s="11">
         <f t="shared" si="11"/>
-        <v>256087.22348023424</v>
+        <v>253611.21787383666</v>
       </c>
       <c r="AA22" s="11">
         <f t="shared" si="12"/>
-        <v>281947.22348023421</v>
+        <v>279471.21787383669</v>
       </c>
       <c r="AB22" s="11">
         <f t="shared" si="13"/>
@@ -19909,37 +19876,37 @@
       </c>
       <c r="AC22" s="12">
         <f t="shared" si="14"/>
-        <v>36169.635869655671</v>
+        <v>35801.593413312614</v>
       </c>
       <c r="AD22" s="12">
         <f t="shared" si="15"/>
-        <v>42473.314846903544</v>
+        <v>42105.272390560494</v>
       </c>
       <c r="AE22" s="12">
         <f t="shared" si="16"/>
-        <v>46745.332716317425</v>
+        <v>46377.290259974383</v>
       </c>
       <c r="AF22" s="12">
         <f t="shared" si="17"/>
-        <v>32395.276866866618</v>
+        <v>32027.234410523564</v>
       </c>
       <c r="AG22" s="12">
         <f t="shared" si="18"/>
-        <v>38065.733988731641</v>
+        <v>37697.691532388591</v>
       </c>
       <c r="AH22" s="12">
         <f t="shared" si="19"/>
-        <v>41909.658209435991</v>
+        <v>41541.615753092941</v>
       </c>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AG23" s="15">
         <f>SUM(AG2:AG22)</f>
-        <v>284024.29749058327</v>
+        <v>260468.66038364053</v>
       </c>
       <c r="AH23" s="15">
         <f>SUM(AH2:AH22)</f>
-        <v>1009834.8759333425</v>
+        <v>986279.2388263999</v>
       </c>
     </row>
     <row r="25" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -19985,7 +19952,7 @@
       </c>
       <c r="AF28">
         <f>AG23-CAPEX!X6</f>
-        <v>65921.280283376138</v>
+        <v>-20954.871623566636</v>
       </c>
     </row>
     <row r="29" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
@@ -21365,11 +21332,11 @@
       </c>
       <c r="F2">
         <f>CAPEX!$X6</f>
-        <v>218103.01720720713</v>
+        <v>281423.53200720716</v>
       </c>
       <c r="G2">
         <f>CAPEX!$X7</f>
-        <v>288261.26026468718</v>
+        <v>228249.55546468718</v>
       </c>
       <c r="H2">
         <f>CAPEX!$X8</f>
@@ -21381,7 +21348,7 @@
       </c>
       <c r="J2">
         <f>CAPEX!$X10</f>
-        <v>147813.53200720716</v>
+        <v>153163.03200720716</v>
       </c>
       <c r="K2">
         <f>CAPEX!$X11</f>
@@ -21393,11 +21360,11 @@
       </c>
       <c r="M2">
         <f>CAPEX!$X13</f>
-        <v>298180.06593992683</v>
+        <v>238167.30071821815</v>
       </c>
       <c r="N2">
         <f>CAPEX!$X14</f>
-        <v>235044.95413371181</v>
+        <v>247844.95413371181</v>
       </c>
       <c r="O2">
         <f>CAPEX!$X15</f>
@@ -21426,7 +21393,7 @@
       </c>
       <c r="G3">
         <f>CAPEX!S7-CAPEX!$S$3+CAPEX!W7-CAPEX!$T$3+CAPEX!T7</f>
-        <v>191994.98430920913</v>
+        <v>131983.27950920913</v>
       </c>
       <c r="H3">
         <f>CAPEX!S8-CAPEX!$S$3+CAPEX!W8-CAPEX!$T$3+CAPEX!T8</f>
@@ -21476,7 +21443,7 @@
       </c>
       <c r="G4">
         <f>CAPEX!S7-CAPEX!S4+CAPEX!T7-CAPEX!T4+CAPEX!U7-CAPEX!U4+CAPEX!V8-CAPEX!V4</f>
-        <v>137560.6381333333</v>
+        <v>137548.93333333335</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -21522,7 +21489,7 @@
       </c>
       <c r="F5">
         <f>CAPEX!S6-CAPEX!S5+CAPEX!T6-CAPEX!T5+CAPEX!U6-CAPEX!U5+CAPEX!V6-CAPEX!V5</f>
-        <v>73057.151866666652</v>
+        <v>136377.66666666669</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -21535,7 +21502,7 @@
       </c>
       <c r="J5">
         <f>CAPEX!S10-CAPEX!S5+CAPEX!T10-CAPEX!T5+CAPEX!U10-CAPEX!U5+CAPEX!V10-CAPEX!V5</f>
-        <v>2767.6666666666642</v>
+        <v>8117.1666666666715</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -21668,7 +21635,7 @@
       </c>
       <c r="G8">
         <f>CAPEX!S7-CAPEX!S8+CAPEX!T7-CAPEX!T8+CAPEX!W7</f>
-        <v>191994.98430920916</v>
+        <v>131983.27950920915</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -21717,7 +21684,7 @@
       </c>
       <c r="G9">
         <f>CAPEX!S7-CAPEX!S9+CAPEX!T7-CAPEX!T9+CAPEX!X10</f>
-        <v>147825.23680720717</v>
+        <v>153163.03200720716</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -21762,7 +21729,7 @@
       </c>
       <c r="F10" s="14">
         <f>F2-J2</f>
-        <v>70289.485199999966</v>
+        <v>128260.5</v>
       </c>
       <c r="G10" s="14">
         <v>0</v>
@@ -21832,11 +21799,11 @@
       </c>
       <c r="M11">
         <f>M2-K2</f>
-        <v>83146.11180621502</v>
+        <v>23133.346584506333</v>
       </c>
       <c r="N11">
         <f>N2-K2</f>
-        <v>20011</v>
+        <v>32811</v>
       </c>
       <c r="O11">
         <f>O2-L2+L11</f>
@@ -21882,7 +21849,7 @@
       </c>
       <c r="M12">
         <f>M2-L2</f>
-        <v>119390.88519999996</v>
+        <v>59378.119978291274</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -21978,7 +21945,7 @@
       </c>
       <c r="M14">
         <f>M2-N2</f>
-        <v>63135.11180621502</v>
+        <v>-9677.6534154936671</v>
       </c>
       <c r="N14">
         <v>0</v>
@@ -22027,7 +21994,7 @@
       </c>
       <c r="M15">
         <f>M2-O2</f>
-        <v>101513.58482170868</v>
+        <v>41500.819599999988</v>
       </c>
       <c r="N15">
         <v>0</v>

</xml_diff>